<commit_message>
add check values to excel template
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04069BFE-A368-3B4C-B763-F5FCBB318577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EABD538-FB79-5A48-BB74-4F17771AB02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31580" yWindow="-2360" windowWidth="28760" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="6880" yWindow="500" windowWidth="22740" windowHeight="15880" activeTab="2" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="184">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>2.4</t>
-  </si>
-  <si>
-    <t>MATLAB/PYTHON OUTPUT</t>
   </si>
   <si>
     <t>ref_tag</t>
@@ -603,12 +600,6 @@
     <t>Copy and paste in values for ref #2: B6 reference gas</t>
   </si>
   <si>
-    <t>Template for algebraic solution for gamma and kappa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Both algebraic and least squares methods are also available in the "Scrambling" function of pyisotopomer.</t>
-  </si>
-  <si>
     <t>CA06261 (EMPA STD1, "Joni")</t>
   </si>
   <si>
@@ -616,6 +607,18 @@
   </si>
   <si>
     <t>CA08214 (EMPA STD3)</t>
+  </si>
+  <si>
+    <t>SCRAMBLING OUTPUT: CHECK VALUES</t>
+  </si>
+  <si>
+    <t>ISOTOPOMER OUTPUT</t>
+  </si>
+  <si>
+    <t>Template for algebraic solution for gamma and kappa. Alternatively, use the Scrambling function of pyisotopomer.</t>
+  </si>
+  <si>
+    <t>Requires recent version of Excel: 16.58 on the Current Channel, or 16.45 on the Beta Channel.</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
       <name val="MS Sans Serif"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +859,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF7B0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,7 +1108,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1333,6 +1342,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -3034,10 +3047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
-  <dimension ref="A1:BH54"/>
+  <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AR16" sqref="AR16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3055,24 +3068,25 @@
     <col min="38" max="40" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.6640625" style="62" customWidth="1"/>
     <col min="42" max="42" width="10.1640625" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" style="44" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" customWidth="1"/>
-    <col min="46" max="46" width="13.5" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" style="44" customWidth="1"/>
+    <col min="45" max="45" width="14.33203125" customWidth="1"/>
+    <col min="46" max="48" width="10.83203125" style="50"/>
+    <col min="51" max="51" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="17" thickBot="1">
+    <row r="1" spans="1:65" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="1"/>
       <c r="W1" s="76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
@@ -3084,47 +3098,52 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AI1" s="79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AJ1" s="80"/>
       <c r="AL1" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" s="52"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="59"/>
       <c r="AP1" s="52"/>
-      <c r="AQ1" s="45"/>
-      <c r="AS1" s="38" t="s">
+      <c r="AR1" s="45"/>
+      <c r="AT1" s="125" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU1" s="125"/>
+      <c r="AV1" s="125"/>
+      <c r="AX1" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="109" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF1" s="109"/>
+      <c r="BG1" s="109"/>
+      <c r="BH1" s="109"/>
+      <c r="BI1" s="110"/>
+      <c r="BJ1" s="111"/>
+      <c r="BK1" s="111"/>
+      <c r="BL1" s="111"/>
+      <c r="BM1" s="111"/>
+    </row>
+    <row r="2" spans="1:65" ht="52" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ1" s="109" t="s">
-        <v>166</v>
-      </c>
-      <c r="BA1" s="109"/>
-      <c r="BB1" s="109"/>
-      <c r="BC1" s="109"/>
-      <c r="BD1" s="110"/>
-      <c r="BE1" s="111"/>
-      <c r="BF1" s="111"/>
-      <c r="BG1" s="111"/>
-      <c r="BH1" s="111"/>
-    </row>
-    <row r="2" spans="1:60" ht="52" thickBot="1">
-      <c r="A2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1</v>
@@ -3212,10 +3231,10 @@
         <v>27</v>
       </c>
       <c r="AI2" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ2" s="81" t="s">
         <v>122</v>
-      </c>
-      <c r="AJ2" s="81" t="s">
-        <v>123</v>
       </c>
       <c r="AK2" s="23"/>
       <c r="AL2" s="56" t="s">
@@ -3228,65 +3247,74 @@
         <v>30</v>
       </c>
       <c r="AO2" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP2" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="AP2" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ2" s="46" t="s">
+      <c r="AR2" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="39" t="s">
+      <c r="AT2" s="126" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU2" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="128" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="AT2" s="39" t="s">
+      <c r="AY2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AU2" s="39" t="s">
+      <c r="AZ2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AV2" s="39" t="s">
+      <c r="BA2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AW2" s="39" t="s">
+      <c r="BB2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="40" t="s">
+      <c r="BC2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="112" t="s">
+      <c r="BD2" s="44"/>
+      <c r="BE2" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="BF2" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="BA2" s="112" t="s">
+      <c r="BG2" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="BB2" s="112" t="s">
+      <c r="BH2" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="BC2" s="112" t="s">
+      <c r="BI2" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="BD2" s="113" t="s">
+      <c r="BJ2" s="114" t="s">
         <v>171</v>
       </c>
-      <c r="BE2" s="114" t="s">
+      <c r="BK2" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="BF2" s="115" t="s">
+      <c r="BL2" s="114" t="s">
         <v>173</v>
       </c>
-      <c r="BG2" s="114" t="s">
-        <v>174</v>
-      </c>
-      <c r="BH2" s="116" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:60" ht="17" thickBot="1">
+      <c r="BM2" s="116" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" ht="17" thickBot="1">
       <c r="A3">
         <v>201204</v>
       </c>
@@ -3402,73 +3430,82 @@
         <v>2.1161148587211971E-3</v>
       </c>
       <c r="AO3" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP3" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ3" s="47">
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR3" s="47">
         <f>A3</f>
         <v>201204</v>
       </c>
-      <c r="AR3" t="str">
+      <c r="AS3" t="str">
         <f>D3</f>
         <v>ATM_EQ_SW</v>
       </c>
-      <c r="AS3" s="50">
-        <v>15.105455486877901</v>
-      </c>
       <c r="AT3" s="50">
-        <v>-2.7098456777153701</v>
+        <v>6.1837131146746902</v>
       </c>
       <c r="AU3" s="50">
-        <v>17.815301164593201</v>
+        <v>24.279175342507699</v>
       </c>
       <c r="AV3" s="50">
-        <v>6.19780490458127</v>
-      </c>
-      <c r="AW3" s="50">
-        <v>24.009727067820499</v>
+        <v>47.588174908592201</v>
       </c>
       <c r="AX3" s="50">
-        <v>47.054171086232202</v>
-      </c>
-      <c r="AY3" s="44"/>
-      <c r="AZ3">
+        <v>15.0490394410522</v>
+      </c>
+      <c r="AY3" s="50">
+        <v>-2.6534292738701302</v>
+      </c>
+      <c r="AZ3" s="50">
+        <v>17.7024687149224</v>
+      </c>
+      <c r="BA3" s="50">
+        <v>6.1978050835910796</v>
+      </c>
+      <c r="BB3" s="50">
+        <v>24.00972360307</v>
+      </c>
+      <c r="BC3" s="50">
+        <v>47.054164220492602</v>
+      </c>
+      <c r="BD3" s="44"/>
+      <c r="BE3">
         <v>265</v>
       </c>
-      <c r="BA3">
+      <c r="BF3">
         <v>109</v>
       </c>
-      <c r="BB3">
-        <f>AZ3-BA3</f>
+      <c r="BG3">
+        <f>BE3-BF3</f>
         <v>156</v>
       </c>
-      <c r="BC3" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD3" s="84">
-        <f>BB3*concentration_constants!$B$6</f>
+      <c r="BH3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI3" s="84">
+        <f>BG3*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE3" s="50">
+      <c r="BJ3" s="50">
         <f>I3*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3147589419488055</v>
       </c>
-      <c r="BF3" s="50">
-        <f>BE3*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK3" s="50">
+        <f>BJ3*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32759693848642901</v>
       </c>
-      <c r="BG3" s="50">
-        <f>BE3/BD3</f>
+      <c r="BL3" s="50">
+        <f>BJ3/BI3</f>
         <v>15.223991502817144</v>
       </c>
-      <c r="BH3" s="50">
-        <f>BF3/BD3</f>
+      <c r="BM3" s="50">
+        <f>BK3/BI3</f>
         <v>2.1545798646607448</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="17" thickBot="1">
+    <row r="4" spans="1:65" ht="17" thickBot="1">
       <c r="A4">
         <v>201205</v>
       </c>
@@ -3575,73 +3612,82 @@
         <v>2.09139498425152E-3</v>
       </c>
       <c r="AO4" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP4" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ4" s="47">
-        <f t="shared" ref="AQ4:AQ17" si="10">A4</f>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR4" s="47">
+        <f>A4</f>
         <v>201205</v>
       </c>
-      <c r="AR4" s="41" t="str">
-        <f t="shared" ref="AR4:AR17" si="11">D4</f>
+      <c r="AS4" s="41" t="str">
+        <f>D4</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS4" s="50">
-        <v>6.8736240880515798</v>
-      </c>
       <c r="AT4" s="50">
-        <v>-13.881471917271901</v>
+        <v>-3.5025945279739599</v>
       </c>
       <c r="AU4" s="50">
-        <v>20.755096005323502</v>
+        <v>17.995404021976</v>
       </c>
       <c r="AV4" s="50">
-        <v>-3.5039239146101799</v>
-      </c>
-      <c r="AW4" s="50">
-        <v>17.848649659933699</v>
+        <v>35.169038165624201</v>
       </c>
       <c r="AX4" s="50">
-        <v>34.879852068524698</v>
-      </c>
-      <c r="AY4" s="44"/>
-      <c r="AZ4">
+        <v>6.8186628672068901</v>
+      </c>
+      <c r="AY4" s="50">
+        <v>-13.8265102937522</v>
+      </c>
+      <c r="AZ4" s="50">
+        <v>20.6451731609591</v>
+      </c>
+      <c r="BA4" s="50">
+        <v>-3.5039237132726799</v>
+      </c>
+      <c r="BB4" s="50">
+        <v>17.848645763027498</v>
+      </c>
+      <c r="BC4" s="50">
+        <v>34.879844390014398</v>
+      </c>
+      <c r="BD4" s="44"/>
+      <c r="BE4">
         <v>265</v>
       </c>
-      <c r="BA4">
+      <c r="BF4">
         <v>109</v>
       </c>
-      <c r="BB4">
-        <f t="shared" ref="BB4:BB5" si="12">AZ4-BA4</f>
+      <c r="BG4">
+        <f t="shared" ref="BG4:BG5" si="10">BE4-BF4</f>
         <v>156</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BH4" t="s">
         <v>39</v>
       </c>
-      <c r="BD4" s="84">
-        <f>BB4*concentration_constants!$F$6</f>
+      <c r="BI4" s="84">
+        <f>BG4*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE4" s="50">
+      <c r="BJ4" s="50">
         <f>I4*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.0120000289208293</v>
       </c>
-      <c r="BF4" s="50">
-        <f>BE4*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK4" s="50">
+        <f>BJ4*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33318789796769971</v>
       </c>
-      <c r="BG4" s="50">
-        <f t="shared" ref="BG4:BG5" si="13">BE4/BD4</f>
+      <c r="BL4" s="50">
+        <f t="shared" ref="BL4:BL5" si="11">BJ4/BI4</f>
         <v>19.272938646594689</v>
       </c>
-      <c r="BH4" s="50">
-        <f t="shared" ref="BH4:BH5" si="14">BF4/BD4</f>
+      <c r="BM4" s="50">
+        <f t="shared" ref="BM4:BM5" si="12">BK4/BI4</f>
         <v>2.1319753830215245</v>
       </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:65">
       <c r="A5">
         <v>201205</v>
       </c>
@@ -3703,7 +3749,7 @@
         <v>0.42933650000000001</v>
       </c>
       <c r="W5" s="76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
@@ -3753,73 +3799,82 @@
         <v>2.1097889665454826E-3</v>
       </c>
       <c r="AO5" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP5" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ5" s="47">
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR5" s="47">
+        <f>A5</f>
+        <v>201205</v>
+      </c>
+      <c r="AS5" s="41" t="str">
+        <f>D5</f>
+        <v>B6_ref_1</v>
+      </c>
+      <c r="AT5" s="50">
+        <v>0.359221158885425</v>
+      </c>
+      <c r="AU5" s="50">
+        <v>22.697206561636399</v>
+      </c>
+      <c r="AV5" s="50">
+        <v>44.4548477102446</v>
+      </c>
+      <c r="AX5" s="50">
+        <v>-0.60159200015230596</v>
+      </c>
+      <c r="AY5" s="50">
+        <v>1.34440496353738</v>
+      </c>
+      <c r="AZ5" s="50">
+        <v>-1.9459969636896799</v>
+      </c>
+      <c r="BA5" s="50">
+        <v>0.37140648169253698</v>
+      </c>
+      <c r="BB5" s="50">
+        <v>22.461390832676202</v>
+      </c>
+      <c r="BC5" s="50">
+        <v>43.988168235934403</v>
+      </c>
+      <c r="BD5" s="44"/>
+      <c r="BE5">
+        <v>265</v>
+      </c>
+      <c r="BF5">
+        <v>109</v>
+      </c>
+      <c r="BG5">
         <f t="shared" si="10"/>
-        <v>201205</v>
-      </c>
-      <c r="AR5" s="41" t="str">
-        <f t="shared" si="11"/>
-        <v>B6_ref_1</v>
-      </c>
-      <c r="AS5" s="50">
-        <v>-0.53970856962448599</v>
-      </c>
-      <c r="AT5" s="50">
-        <v>1.2825215740412901</v>
-      </c>
-      <c r="AU5" s="50">
-        <v>-1.82223014366578</v>
-      </c>
-      <c r="AV5" s="50">
-        <v>0.37140650220840399</v>
-      </c>
-      <c r="AW5" s="50">
-        <v>22.461390435589401</v>
-      </c>
-      <c r="AX5" s="50">
-        <v>43.988167450184299</v>
-      </c>
-      <c r="AY5" s="44"/>
-      <c r="AZ5">
-        <v>265</v>
-      </c>
-      <c r="BA5">
-        <v>109</v>
-      </c>
-      <c r="BB5">
-        <f t="shared" si="12"/>
         <v>156</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BH5" t="s">
         <v>39</v>
       </c>
-      <c r="BD5" s="84">
-        <f>BB5*concentration_constants!$F$6</f>
+      <c r="BI5" s="84">
+        <f>BG5*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE5" s="50">
+      <c r="BJ5" s="50">
         <f>I5*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.9048847269174694</v>
       </c>
-      <c r="BF5" s="50">
-        <f>BE5*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK5" s="50">
+        <f>BJ5*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38845979713665457</v>
       </c>
-      <c r="BG5" s="50">
-        <f t="shared" si="13"/>
+      <c r="BL5" s="50">
+        <f t="shared" si="11"/>
         <v>63.378563682109089</v>
       </c>
-      <c r="BH5" s="50">
-        <f t="shared" si="14"/>
+      <c r="BM5" s="50">
+        <f t="shared" si="12"/>
         <v>2.4856446762936448</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:65">
       <c r="A6">
         <v>201205</v>
       </c>
@@ -3935,73 +3990,82 @@
         <v>2.1164798861162187E-3</v>
       </c>
       <c r="AO6" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP6" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ6" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR6" s="47">
+        <f>A6</f>
         <v>201205</v>
       </c>
-      <c r="AR6" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS6" t="str">
+        <f>D6</f>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS6" s="50">
-        <v>14.851574153242799</v>
-      </c>
       <c r="AT6" s="50">
-        <v>-0.85838254078074405</v>
+        <v>6.9823553262469096</v>
       </c>
       <c r="AU6" s="50">
-        <v>15.7099566940236</v>
+        <v>24.3669184468542</v>
       </c>
       <c r="AV6" s="50">
-        <v>6.9965958062310696</v>
-      </c>
-      <c r="AW6" s="50">
-        <v>24.095420378555701</v>
+        <v>47.762096293894203</v>
       </c>
       <c r="AX6" s="50">
-        <v>47.223987370547697</v>
-      </c>
-      <c r="AY6" s="44"/>
-      <c r="AZ6">
+        <v>14.7944751196213</v>
+      </c>
+      <c r="AY6" s="50">
+        <v>-0.80128319311811802</v>
+      </c>
+      <c r="AZ6" s="50">
+        <v>15.5957583127395</v>
+      </c>
+      <c r="BA6" s="50">
+        <v>6.9965959632516297</v>
+      </c>
+      <c r="BB6" s="50">
+        <v>24.095417339407199</v>
+      </c>
+      <c r="BC6" s="50">
+        <v>47.223981347707102</v>
+      </c>
+      <c r="BD6" s="44"/>
+      <c r="BE6">
         <v>265</v>
       </c>
-      <c r="BA6">
+      <c r="BF6">
         <v>109</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB17" si="15">AZ6-BA6</f>
+      <c r="BG6">
+        <f t="shared" ref="BG6:BG17" si="13">BE6-BF6</f>
         <v>156</v>
       </c>
-      <c r="BC6" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD6" s="84">
-        <f>BB6*concentration_constants!$B$6</f>
+      <c r="BH6" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI6" s="84">
+        <f>BG6*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE6" s="50">
+      <c r="BJ6" s="50">
         <f>I6*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4178655483113793</v>
       </c>
-      <c r="BF6" s="50">
-        <f>BE6*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK6" s="50">
+        <f>BJ6*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32842371830361955</v>
       </c>
-      <c r="BG6" s="50">
-        <f t="shared" ref="BG6:BG17" si="16">BE6/BD6</f>
+      <c r="BL6" s="50">
+        <f t="shared" ref="BL6:BL17" si="14">BJ6/BI6</f>
         <v>15.90211572158638</v>
       </c>
-      <c r="BH6" s="50">
-        <f t="shared" ref="BH6:BH17" si="17">BF6/BD6</f>
+      <c r="BM6" s="50">
+        <f t="shared" ref="BM6:BM17" si="15">BK6/BI6</f>
         <v>2.1600175319199595</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="17" thickBot="1">
+    <row r="7" spans="1:65" ht="17" thickBot="1">
       <c r="A7">
         <v>201205</v>
       </c>
@@ -4117,73 +4181,82 @@
         <v>2.0917613635465034E-3</v>
       </c>
       <c r="AO7" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP7" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ7" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR7" s="47">
+        <f>A7</f>
         <v>201205</v>
       </c>
-      <c r="AR7" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS7" t="str">
+        <f>D7</f>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS7" s="50">
-        <v>6.6566362138331598</v>
-      </c>
       <c r="AT7" s="50">
-        <v>-13.8026489120794</v>
+        <v>-3.5713502434924198</v>
       </c>
       <c r="AU7" s="50">
-        <v>20.459285125912601</v>
+        <v>18.090066846573698</v>
       </c>
       <c r="AV7" s="50">
-        <v>-3.5730063491231601</v>
-      </c>
-      <c r="AW7" s="50">
-        <v>17.941820061995799</v>
+        <v>35.355596284351698</v>
       </c>
       <c r="AX7" s="50">
-        <v>35.063444020270097</v>
-      </c>
-      <c r="AY7" s="44"/>
-      <c r="AZ7">
+        <v>6.6015916386952203</v>
+      </c>
+      <c r="AY7" s="50">
+        <v>-13.7476039394125</v>
+      </c>
+      <c r="AZ7" s="50">
+        <v>20.3491955781077</v>
+      </c>
+      <c r="BA7" s="50">
+        <v>-3.5730061503586601</v>
+      </c>
+      <c r="BB7" s="50">
+        <v>17.9418162148927</v>
+      </c>
+      <c r="BC7" s="50">
+        <v>35.0634364392414</v>
+      </c>
+      <c r="BD7" s="44"/>
+      <c r="BE7">
         <v>265</v>
       </c>
-      <c r="BA7">
+      <c r="BF7">
         <v>109</v>
       </c>
-      <c r="BB7">
-        <f t="shared" si="15"/>
+      <c r="BG7">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BH7" t="s">
         <v>39</v>
       </c>
-      <c r="BD7" s="84">
-        <f>BB7*concentration_constants!$F$6</f>
+      <c r="BI7" s="84">
+        <f>BG7*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE7" s="50">
+      <c r="BJ7" s="50">
         <f>I7*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>17.089981869851989</v>
       </c>
-      <c r="BF7" s="50">
-        <f>BE7*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK7" s="50">
+        <f>BJ7*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.44607485704311811</v>
       </c>
-      <c r="BG7" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL7" s="50">
+        <f t="shared" si="14"/>
         <v>109.35397373388625</v>
       </c>
-      <c r="BH7" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM7" s="50">
+        <f t="shared" si="15"/>
         <v>2.8543071942335927</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="17" thickBot="1">
+    <row r="8" spans="1:65" ht="17" thickBot="1">
       <c r="A8">
         <v>201205</v>
       </c>
@@ -4290,73 +4363,82 @@
         <v>2.1059970799231576E-3</v>
       </c>
       <c r="AO8" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP8" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ8" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR8" s="47">
+        <f>A8</f>
         <v>201205</v>
       </c>
-      <c r="AR8" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS8" t="str">
+        <f>D8</f>
         <v>B6_ref_2</v>
       </c>
-      <c r="AS8" s="50">
-        <v>-1.15628904358433</v>
-      </c>
       <c r="AT8" s="50">
-        <v>-0.70441124849329695</v>
+        <v>-0.94152706968220201</v>
       </c>
       <c r="AU8" s="50">
-        <v>-0.45187779509103798</v>
+        <v>21.732150005308199</v>
       </c>
       <c r="AV8" s="50">
-        <v>-0.93035014603881605</v>
-      </c>
-      <c r="AW8" s="50">
-        <v>21.5157968077277</v>
+        <v>42.5456389567846</v>
       </c>
       <c r="AX8" s="50">
-        <v>42.117851051899301</v>
-      </c>
-      <c r="AY8" s="44"/>
-      <c r="AZ8">
+        <v>-1.217686963634</v>
+      </c>
+      <c r="AY8" s="50">
+        <v>-0.643013339496456</v>
+      </c>
+      <c r="AZ8" s="50">
+        <v>-0.57467362413754497</v>
+      </c>
+      <c r="BA8" s="50">
+        <v>-0.93035015156522904</v>
+      </c>
+      <c r="BB8" s="50">
+        <v>21.515796914688998</v>
+      </c>
+      <c r="BC8" s="50">
+        <v>42.117851263369303</v>
+      </c>
+      <c r="BD8" s="44"/>
+      <c r="BE8">
         <v>265</v>
       </c>
-      <c r="BA8">
+      <c r="BF8">
         <v>109</v>
       </c>
-      <c r="BB8">
-        <f t="shared" si="15"/>
+      <c r="BG8">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BH8" t="s">
         <v>39</v>
       </c>
-      <c r="BD8" s="84">
-        <f>BB8*concentration_constants!$F$6</f>
+      <c r="BI8" s="84">
+        <f>BG8*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE8" s="50">
+      <c r="BJ8" s="50">
         <f>I8*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.8350681459275666</v>
       </c>
-      <c r="BF8" s="50">
-        <f>BE8*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK8" s="50">
+        <f>BJ8*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.387899959681965</v>
       </c>
-      <c r="BG8" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL8" s="50">
+        <f t="shared" si="14"/>
         <v>62.931827072210872</v>
       </c>
-      <c r="BH8" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM8" s="50">
+        <f t="shared" si="15"/>
         <v>2.4820624343239581</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:65">
       <c r="A9">
         <v>201205</v>
       </c>
@@ -4418,7 +4500,7 @@
         <v>0.42850050000000001</v>
       </c>
       <c r="X9" s="76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y9" s="3"/>
       <c r="AA9" s="28">
@@ -4466,72 +4548,81 @@
         <v>2.1125489546459449E-3</v>
       </c>
       <c r="AO9" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP9" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ9" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR9" s="47">
+        <f>A9</f>
         <v>201205</v>
       </c>
-      <c r="AR9" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS9" s="41" t="str">
+        <f>D9</f>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS9" s="50">
-        <v>16.036656468840999</v>
-      </c>
       <c r="AT9" s="50">
-        <v>-4.8656873390863202</v>
+        <v>5.57244533353684</v>
       </c>
       <c r="AU9" s="50">
-        <v>20.902343807927299</v>
+        <v>23.366934635269601</v>
       </c>
       <c r="AV9" s="50">
-        <v>5.5854845648773397</v>
-      </c>
-      <c r="AW9" s="50">
-        <v>23.117269398744899</v>
+        <v>45.7807904317755</v>
       </c>
       <c r="AX9" s="50">
-        <v>45.286402388126902</v>
-      </c>
-      <c r="AZ9">
+        <v>15.9811824695308</v>
+      </c>
+      <c r="AY9" s="50">
+        <v>-4.8102129708880099</v>
+      </c>
+      <c r="AZ9" s="50">
+        <v>20.7913954404188</v>
+      </c>
+      <c r="BA9" s="50">
+        <v>5.5854847493214104</v>
+      </c>
+      <c r="BB9" s="50">
+        <v>23.117265828815</v>
+      </c>
+      <c r="BC9" s="50">
+        <v>45.286395319747101</v>
+      </c>
+      <c r="BE9">
         <v>265</v>
       </c>
-      <c r="BA9">
+      <c r="BF9">
         <v>109</v>
       </c>
-      <c r="BB9">
-        <f t="shared" si="15"/>
+      <c r="BG9">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC9" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD9" s="84">
-        <f>BB9*concentration_constants!$B$6</f>
+      <c r="BH9" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI9" s="84">
+        <f>BG9*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE9" s="50">
+      <c r="BJ9" s="50">
         <f>I9*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4132419336762863</v>
       </c>
-      <c r="BF9" s="50">
-        <f>BE9*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK9" s="50">
+        <f>BJ9*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32838664297549441</v>
       </c>
-      <c r="BG9" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL9" s="50">
+        <f t="shared" si="14"/>
         <v>15.871706563794037</v>
       </c>
-      <c r="BH9" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM9" s="50">
+        <f t="shared" si="15"/>
         <v>2.1597736903388287</v>
       </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:65">
       <c r="A10">
         <v>201205</v>
       </c>
@@ -4640,72 +4731,81 @@
         <v>2.1110245425008428E-3</v>
       </c>
       <c r="AO10" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP10" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ10" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR10" s="47">
+        <f>A10</f>
         <v>201205</v>
       </c>
-      <c r="AR10" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS10" t="str">
+        <f>D10</f>
         <v>DI</v>
       </c>
-      <c r="AS10" s="50">
-        <v>14.4579715364672</v>
-      </c>
       <c r="AT10" s="50">
-        <v>-34.815304667159701</v>
+        <v>-10.0998672074388</v>
       </c>
       <c r="AU10" s="50">
-        <v>49.273276203626899</v>
+        <v>23.078452800784302</v>
       </c>
       <c r="AV10" s="50">
-        <v>-10.1786665653462</v>
-      </c>
-      <c r="AW10" s="50">
-        <v>22.853627356464699</v>
+        <v>45.209547777639301</v>
       </c>
       <c r="AX10" s="50">
-        <v>44.764460247631298</v>
-      </c>
-      <c r="AZ10">
+        <v>14.4118651961093</v>
+      </c>
+      <c r="AY10" s="50">
+        <v>-34.769197528393804</v>
+      </c>
+      <c r="AZ10" s="50">
+        <v>49.1810627245031</v>
+      </c>
+      <c r="BA10" s="50">
+        <v>-10.1786661661422</v>
+      </c>
+      <c r="BB10" s="50">
+        <v>22.853619629831201</v>
+      </c>
+      <c r="BC10" s="50">
+        <v>44.7644449527711</v>
+      </c>
+      <c r="BE10">
         <v>265</v>
       </c>
-      <c r="BA10">
+      <c r="BF10">
         <v>109</v>
       </c>
-      <c r="BB10">
-        <f t="shared" si="15"/>
+      <c r="BG10">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC10" t="s">
+      <c r="BH10" t="s">
         <v>39</v>
       </c>
-      <c r="BD10" s="84">
-        <f>BB10*concentration_constants!$F$6</f>
+      <c r="BI10" s="84">
+        <f>BG10*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE10" s="50">
+      <c r="BJ10" s="50">
         <f>I10*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>7.9745256167661447</v>
       </c>
-      <c r="BF10" s="50">
-        <f>BE10*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK10" s="50">
+        <f>BJ10*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3729808476444097</v>
       </c>
-      <c r="BG10" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL10" s="50">
+        <f t="shared" si="14"/>
         <v>51.026740196512598</v>
       </c>
-      <c r="BH10" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM10" s="50">
+        <f t="shared" si="15"/>
         <v>2.386599244350319</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="17" thickBot="1">
+    <row r="11" spans="1:65" ht="17" thickBot="1">
       <c r="A11">
         <v>201207</v>
       </c>
@@ -4819,72 +4919,81 @@
         <v>2.11205838421125E-3</v>
       </c>
       <c r="AO11" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP11" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ11" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR11" s="47">
+        <f>A11</f>
         <v>201207</v>
       </c>
-      <c r="AR11" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS11" s="41" t="str">
+        <f>D11</f>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS11" s="50">
-        <v>17.1518234709566</v>
-      </c>
       <c r="AT11" s="50">
-        <v>-4.5745335204508901</v>
+        <v>6.2757163469961901</v>
       </c>
       <c r="AU11" s="50">
-        <v>21.726356991407499</v>
+        <v>23.235402273854501</v>
       </c>
       <c r="AV11" s="50">
-        <v>6.2886449752528799</v>
-      </c>
-      <c r="AW11" s="50">
-        <v>22.988533215933799</v>
+        <v>45.520315450628203</v>
       </c>
       <c r="AX11" s="50">
-        <v>45.031522726332703</v>
-      </c>
-      <c r="AZ11">
+        <v>17.096555270453798</v>
+      </c>
+      <c r="AY11" s="50">
+        <v>-4.5192648951586296</v>
+      </c>
+      <c r="AZ11" s="50">
+        <v>21.615820165612401</v>
+      </c>
+      <c r="BA11" s="50">
+        <v>6.2886451876476004</v>
+      </c>
+      <c r="BB11" s="50">
+        <v>22.988529105010201</v>
+      </c>
+      <c r="BC11" s="50">
+        <v>45.031514587758402</v>
+      </c>
+      <c r="BE11">
         <v>265</v>
       </c>
-      <c r="BA11">
+      <c r="BF11">
         <v>109</v>
       </c>
-      <c r="BB11">
-        <f t="shared" si="15"/>
+      <c r="BG11">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC11" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD11" s="84">
-        <f>BB11*concentration_constants!$B$6</f>
+      <c r="BH11" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI11" s="84">
+        <f>BG11*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE11" s="50">
+      <c r="BJ11" s="50">
         <f>I11*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2611250121817261</v>
       </c>
-      <c r="BF11" s="50">
-        <f>BE11*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK11" s="50">
+        <f>BJ11*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32716686468017736</v>
       </c>
-      <c r="BG11" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL11" s="50">
+        <f t="shared" si="14"/>
         <v>14.871245272425968</v>
       </c>
-      <c r="BH11" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM11" s="50">
+        <f t="shared" si="15"/>
         <v>2.151751302319628</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:65">
       <c r="A12">
         <v>201207</v>
       </c>
@@ -4990,72 +5099,81 @@
         <v>2.0890378267892978E-3</v>
       </c>
       <c r="AO12" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP12" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ12" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR12" s="47">
+        <f>A12</f>
         <v>201207</v>
       </c>
-      <c r="AR12" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS12" s="41" t="str">
+        <f>D12</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS12" s="50">
-        <v>7.0098620813652204</v>
-      </c>
       <c r="AT12" s="50">
-        <v>-14.5751415214816</v>
+        <v>-3.7789086077021299</v>
       </c>
       <c r="AU12" s="50">
-        <v>21.5850036028468</v>
+        <v>17.3910621684267</v>
       </c>
       <c r="AV12" s="50">
-        <v>-3.78263972005821</v>
-      </c>
-      <c r="AW12" s="50">
-        <v>17.254451999306699</v>
+        <v>33.978406326581499</v>
       </c>
       <c r="AX12" s="50">
-        <v>33.709358475152598</v>
-      </c>
-      <c r="AZ12">
+        <v>6.9551636951770099</v>
+      </c>
+      <c r="AY12" s="50">
+        <v>-14.5204427181152</v>
+      </c>
+      <c r="AZ12" s="50">
+        <v>21.475606413292201</v>
+      </c>
+      <c r="BA12" s="50">
+        <v>-3.78263951146912</v>
+      </c>
+      <c r="BB12" s="50">
+        <v>17.254447962045099</v>
+      </c>
+      <c r="BC12" s="50">
+        <v>33.709350524440303</v>
+      </c>
+      <c r="BE12">
         <v>265</v>
       </c>
-      <c r="BA12">
+      <c r="BF12">
         <v>109</v>
       </c>
-      <c r="BB12">
-        <f t="shared" si="15"/>
+      <c r="BG12">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC12" t="s">
+      <c r="BH12" t="s">
         <v>39</v>
       </c>
-      <c r="BD12" s="84">
-        <f>BB12*concentration_constants!$F$6</f>
+      <c r="BI12" s="84">
+        <f>BG12*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE12" s="50">
+      <c r="BJ12" s="50">
         <f>I12*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.6625426080784145</v>
       </c>
-      <c r="BF12" s="50">
-        <f>BE12*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK12" s="50">
+        <f>BJ12*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33840439663490651</v>
       </c>
-      <c r="BG12" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL12" s="50">
+        <f t="shared" si="14"/>
         <v>23.435577124255598</v>
       </c>
-      <c r="BH12" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM12" s="50">
+        <f t="shared" si="15"/>
         <v>2.1653542866728439</v>
       </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:65">
       <c r="A13">
         <v>201207</v>
       </c>
@@ -5161,72 +5279,81 @@
         <v>2.1092446228371492E-3</v>
       </c>
       <c r="AO13" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP13" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ13" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR13" s="47">
+        <f>A13</f>
         <v>201207</v>
       </c>
-      <c r="AR13" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS13" s="41" t="str">
+        <f>D13</f>
         <v>B6_ref_1</v>
       </c>
-      <c r="AS13" s="50">
-        <v>8.2241945278393999E-2</v>
-      </c>
       <c r="AT13" s="50">
-        <v>0.22102332359041901</v>
+        <v>0.13959532425555901</v>
       </c>
       <c r="AU13" s="50">
-        <v>-0.138781378312025</v>
+        <v>22.5589202485119</v>
       </c>
       <c r="AV13" s="50">
-        <v>0.151632634434406</v>
-      </c>
-      <c r="AW13" s="50">
-        <v>22.3259423648012</v>
+        <v>44.181166769186902</v>
       </c>
       <c r="AX13" s="50">
-        <v>43.720161276728597</v>
-      </c>
-      <c r="AZ13">
+        <v>2.0870367696490501E-2</v>
+      </c>
+      <c r="AY13" s="50">
+        <v>0.28239489685111202</v>
+      </c>
+      <c r="AZ13" s="50">
+        <v>-0.26152452915462199</v>
+      </c>
+      <c r="BA13" s="50">
+        <v>0.151632632273801</v>
+      </c>
+      <c r="BB13" s="50">
+        <v>22.325942406621301</v>
+      </c>
+      <c r="BC13" s="50">
+        <v>43.720161359471298</v>
+      </c>
+      <c r="BE13">
         <v>265</v>
       </c>
-      <c r="BA13">
+      <c r="BF13">
         <v>109</v>
       </c>
-      <c r="BB13">
-        <f t="shared" si="15"/>
+      <c r="BG13">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC13" t="s">
+      <c r="BH13" t="s">
         <v>39</v>
       </c>
-      <c r="BD13" s="84">
-        <f>BB13*concentration_constants!$F$6</f>
+      <c r="BI13" s="84">
+        <f>BG13*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE13" s="50">
+      <c r="BJ13" s="50">
         <f>I13*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.6085110288080102</v>
       </c>
-      <c r="BF13" s="50">
-        <f>BE13*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK13" s="50">
+        <f>BJ13*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38608326860383324</v>
       </c>
-      <c r="BG13" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL13" s="50">
+        <f t="shared" si="14"/>
         <v>61.482151980488176</v>
       </c>
-      <c r="BH13" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM13" s="50">
+        <f t="shared" si="15"/>
         <v>2.4704379405150405</v>
       </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:65">
       <c r="A14">
         <v>201207</v>
       </c>
@@ -5332,72 +5459,81 @@
         <v>2.1118562233900973E-3</v>
       </c>
       <c r="AO14" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP14" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ14" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR14" s="47">
+        <f>A14</f>
         <v>201207</v>
       </c>
-      <c r="AR14" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS14" s="41" t="str">
+        <f>D14</f>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS14" s="50">
-        <v>14.393773542834699</v>
-      </c>
       <c r="AT14" s="50">
-        <v>-3.6809189289388402</v>
+        <v>5.3435875779892497</v>
       </c>
       <c r="AU14" s="50">
-        <v>18.074692471773599</v>
+        <v>23.190561718908899</v>
       </c>
       <c r="AV14" s="50">
-        <v>5.3564273069479604</v>
-      </c>
-      <c r="AW14" s="50">
-        <v>22.94455532836</v>
+        <v>45.431524384704502</v>
       </c>
       <c r="AX14" s="50">
-        <v>44.944459545090702</v>
-      </c>
-      <c r="AZ14">
+        <v>14.337476770066299</v>
+      </c>
+      <c r="AY14" s="50">
+        <v>-3.6246218372294399</v>
+      </c>
+      <c r="AZ14" s="50">
+        <v>17.9620986072958</v>
+      </c>
+      <c r="BA14" s="50">
+        <v>5.3564274664184497</v>
+      </c>
+      <c r="BB14" s="50">
+        <v>22.9445522417919</v>
+      </c>
+      <c r="BC14" s="50">
+        <v>44.944453434723798</v>
+      </c>
+      <c r="BE14">
         <v>265</v>
       </c>
-      <c r="BA14">
+      <c r="BF14">
         <v>109</v>
       </c>
-      <c r="BB14">
-        <f t="shared" si="15"/>
+      <c r="BG14">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC14" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD14" s="84">
-        <f>BB14*concentration_constants!$B$6</f>
+      <c r="BH14" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI14" s="84">
+        <f>BG14*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE14" s="50">
+      <c r="BJ14" s="50">
         <f>I14*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3526725819565679</v>
       </c>
-      <c r="BF14" s="50">
-        <f>BE14*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK14" s="50">
+        <f>BJ14*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32790095617705511</v>
       </c>
-      <c r="BG14" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL14" s="50">
+        <f t="shared" si="14"/>
         <v>15.473346596714352</v>
       </c>
-      <c r="BH14" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM14" s="50">
+        <f t="shared" si="15"/>
         <v>2.1565793656260164</v>
       </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:65">
       <c r="A15">
         <v>201207</v>
       </c>
@@ -5503,72 +5639,81 @@
         <v>2.1140383039962136E-3</v>
       </c>
       <c r="AO15" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP15" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ15" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR15" s="47">
+        <f>A15</f>
         <v>201207</v>
       </c>
-      <c r="AR15" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS15" t="str">
+        <f>D15</f>
         <v>ATM_EQ_SW_3</v>
       </c>
-      <c r="AS15" s="50">
-        <v>16.679833428360201</v>
-      </c>
       <c r="AT15" s="50">
-        <v>-4.3336183513273898</v>
+        <v>6.1596227211071497</v>
       </c>
       <c r="AU15" s="50">
-        <v>21.0134517796876</v>
+        <v>23.745401762334801</v>
       </c>
       <c r="AV15" s="50">
-        <v>6.1731075385164003</v>
-      </c>
-      <c r="AW15" s="50">
-        <v>23.487665779901398</v>
+        <v>46.530448225756899</v>
       </c>
       <c r="AX15" s="50">
-        <v>46.019903286484897</v>
-      </c>
-      <c r="AZ15">
+        <v>16.6243703054385</v>
+      </c>
+      <c r="AY15" s="50">
+        <v>-4.27815481119453</v>
+      </c>
+      <c r="AZ15" s="50">
+        <v>20.902525116633001</v>
+      </c>
+      <c r="BA15" s="50">
+        <v>6.1731077471219802</v>
+      </c>
+      <c r="BB15" s="50">
+        <v>23.487661742321102</v>
+      </c>
+      <c r="BC15" s="50">
+        <v>46.019895289453402</v>
+      </c>
+      <c r="BE15">
         <v>265</v>
       </c>
-      <c r="BA15">
+      <c r="BF15">
         <v>109</v>
       </c>
-      <c r="BB15">
-        <f t="shared" si="15"/>
+      <c r="BG15">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC15" t="s">
-        <v>175</v>
-      </c>
-      <c r="BD15" s="84">
-        <f>BB15*concentration_constants!$B$6</f>
+      <c r="BH15" t="s">
+        <v>174</v>
+      </c>
+      <c r="BI15" s="84">
+        <f>BG15*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE15" s="50">
+      <c r="BJ15" s="50">
         <f>I15*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2375445775427525</v>
       </c>
-      <c r="BF15" s="50">
-        <f>BE15*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK15" s="50">
+        <f>BJ15*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3269777805067392</v>
       </c>
-      <c r="BG15" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL15" s="50">
+        <f t="shared" si="14"/>
         <v>14.716158567685026</v>
       </c>
-      <c r="BH15" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM15" s="50">
+        <f t="shared" si="15"/>
         <v>2.1505077102558618</v>
       </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:65">
       <c r="A16">
         <v>201207</v>
       </c>
@@ -5674,72 +5819,81 @@
         <v>2.0909357320700551E-3</v>
       </c>
       <c r="AO16" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP16" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ16" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR16" s="47">
+        <f>A16</f>
         <v>201207</v>
       </c>
-      <c r="AR16" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS16" t="str">
+        <f>D16</f>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS16" s="50">
-        <v>7.1029978910310803</v>
-      </c>
       <c r="AT16" s="50">
-        <v>-14.893050092214599</v>
+        <v>-3.8910374902335598</v>
       </c>
       <c r="AU16" s="50">
-        <v>21.996047983245699</v>
+        <v>17.879824476930899</v>
       </c>
       <c r="AV16" s="50">
-        <v>-3.8950261005917799</v>
-      </c>
-      <c r="AW16" s="50">
-        <v>17.735485742880101</v>
+        <v>34.941280181798497</v>
       </c>
       <c r="AX16" s="50">
-        <v>34.656884164523802</v>
-      </c>
-      <c r="AZ16">
+        <v>7.0484281107991897</v>
+      </c>
+      <c r="AY16" s="50">
+        <v>-14.8384798879742</v>
+      </c>
+      <c r="AZ16" s="50">
+        <v>21.886907998773399</v>
+      </c>
+      <c r="BA16" s="50">
+        <v>-3.8950258885875302</v>
+      </c>
+      <c r="BB16" s="50">
+        <v>17.735481639519399</v>
+      </c>
+      <c r="BC16" s="50">
+        <v>34.6568760800563</v>
+      </c>
+      <c r="BE16">
         <v>265</v>
       </c>
-      <c r="BA16">
+      <c r="BF16">
         <v>109</v>
       </c>
-      <c r="BB16">
-        <f t="shared" si="15"/>
+      <c r="BG16">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC16" t="s">
+      <c r="BH16" t="s">
         <v>39</v>
       </c>
-      <c r="BD16" s="84">
-        <f>BB16*concentration_constants!$F$6</f>
+      <c r="BI16" s="84">
+        <f>BG16*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE16" s="50">
+      <c r="BJ16" s="50">
         <f>I16*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.9394971247204844</v>
       </c>
-      <c r="BF16" s="50">
-        <f>BE16*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK16" s="50">
+        <f>BJ16*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.34062520878960229</v>
       </c>
-      <c r="BG16" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL16" s="50">
+        <f t="shared" si="14"/>
         <v>25.207730960871714</v>
       </c>
-      <c r="BH16" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM16" s="50">
+        <f t="shared" si="15"/>
         <v>2.179564637267827</v>
       </c>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:65">
       <c r="A17">
         <v>201207</v>
       </c>
@@ -5842,72 +5996,81 @@
         <v>2.1099653819650526E-3</v>
       </c>
       <c r="AO17" s="57">
-        <v>0.18325645634287266</v>
+        <v>0.18344928548237474</v>
       </c>
       <c r="AP17" s="58">
-        <v>9.0490249769565087E-2</v>
-      </c>
-      <c r="AQ17" s="47">
-        <f t="shared" si="10"/>
+        <v>9.0727587262159418E-2</v>
+      </c>
+      <c r="AR17" s="47">
+        <f>A17</f>
         <v>201207</v>
       </c>
-      <c r="AR17" s="41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AS17" s="41" t="str">
+        <f>D17</f>
         <v>DI</v>
       </c>
-      <c r="AS17" s="50">
-        <v>13.725240315331099</v>
-      </c>
       <c r="AT17" s="50">
-        <v>-28.3353648321477</v>
+        <v>-7.2725212903335104</v>
       </c>
       <c r="AU17" s="50">
-        <v>42.060605147478803</v>
+        <v>22.792929757643901</v>
       </c>
       <c r="AV17" s="50">
-        <v>-7.3050622584082596</v>
-      </c>
-      <c r="AW17" s="50">
-        <v>22.565126816266901</v>
+        <v>44.644312779463498</v>
       </c>
       <c r="AX17" s="50">
-        <v>44.193449376003002</v>
-      </c>
-      <c r="AZ17">
+        <v>13.676821526785201</v>
+      </c>
+      <c r="AY17" s="50">
+        <v>-28.286945321078701</v>
+      </c>
+      <c r="AZ17" s="50">
+        <v>41.963766847864001</v>
+      </c>
+      <c r="BA17" s="50">
+        <v>-7.3050618971467403</v>
+      </c>
+      <c r="BB17" s="50">
+        <v>22.565119824016399</v>
+      </c>
+      <c r="BC17" s="50">
+        <v>44.193435538514699</v>
+      </c>
+      <c r="BE17">
         <v>265</v>
       </c>
-      <c r="BA17">
+      <c r="BF17">
         <v>109</v>
       </c>
-      <c r="BB17">
-        <f t="shared" si="15"/>
+      <c r="BG17">
+        <f t="shared" si="13"/>
         <v>156</v>
       </c>
-      <c r="BC17" t="s">
+      <c r="BH17" t="s">
         <v>39</v>
       </c>
-      <c r="BD17" s="84">
-        <f>BB17*concentration_constants!$F$6</f>
+      <c r="BI17" s="84">
+        <f>BG17*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE17" s="50">
+      <c r="BJ17" s="50">
         <f>I17*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>6.3978730261994317</v>
       </c>
-      <c r="BF17" s="50">
-        <f>BE17*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK17" s="50">
+        <f>BJ17*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.36033816075373781</v>
       </c>
-      <c r="BG17" s="50">
-        <f t="shared" si="16"/>
+      <c r="BL17" s="50">
+        <f t="shared" si="14"/>
         <v>40.938184966360723</v>
       </c>
-      <c r="BH17" s="50">
-        <f t="shared" si="17"/>
+      <c r="BM17" s="50">
+        <f t="shared" si="15"/>
         <v>2.3057022568229555</v>
       </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:65">
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -5939,16 +6102,16 @@
       <c r="AN18" s="33"/>
       <c r="AO18" s="57"/>
       <c r="AP18" s="55"/>
-      <c r="AQ18" s="49"/>
-      <c r="AR18" s="48"/>
+      <c r="AR18" s="49"/>
       <c r="AS18" s="48"/>
-      <c r="AT18" s="48"/>
-      <c r="AU18" s="48"/>
-      <c r="AV18" s="48"/>
-      <c r="AW18" s="48"/>
       <c r="AX18" s="48"/>
-    </row>
-    <row r="19" spans="1:60">
+      <c r="AY18" s="48"/>
+      <c r="AZ18" s="48"/>
+      <c r="BA18" s="48"/>
+      <c r="BB18" s="48"/>
+      <c r="BC18" s="48"/>
+    </row>
+    <row r="19" spans="1:65">
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -5980,16 +6143,16 @@
       <c r="AN19" s="33"/>
       <c r="AO19" s="57"/>
       <c r="AP19" s="55"/>
-      <c r="AQ19" s="49"/>
-      <c r="AR19" s="48"/>
+      <c r="AR19" s="49"/>
       <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="48"/>
-      <c r="AV19" s="48"/>
-      <c r="AW19" s="48"/>
       <c r="AX19" s="48"/>
-    </row>
-    <row r="20" spans="1:60">
+      <c r="AY19" s="48"/>
+      <c r="AZ19" s="48"/>
+      <c r="BA19" s="48"/>
+      <c r="BB19" s="48"/>
+      <c r="BC19" s="48"/>
+    </row>
+    <row r="20" spans="1:65">
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -6021,16 +6184,16 @@
       <c r="AN20" s="33"/>
       <c r="AO20" s="57"/>
       <c r="AP20" s="55"/>
-      <c r="AQ20" s="49"/>
-      <c r="AR20" s="48"/>
+      <c r="AR20" s="49"/>
       <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
-      <c r="AV20" s="48"/>
-      <c r="AW20" s="48"/>
       <c r="AX20" s="48"/>
-    </row>
-    <row r="21" spans="1:60">
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+      <c r="BA20" s="48"/>
+      <c r="BB20" s="48"/>
+      <c r="BC20" s="48"/>
+    </row>
+    <row r="21" spans="1:65">
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -6062,16 +6225,16 @@
       <c r="AN21" s="33"/>
       <c r="AO21" s="57"/>
       <c r="AP21" s="55"/>
-      <c r="AQ21" s="49"/>
-      <c r="AR21" s="48"/>
+      <c r="AR21" s="49"/>
       <c r="AS21" s="48"/>
-      <c r="AT21" s="48"/>
-      <c r="AU21" s="48"/>
-      <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
       <c r="AX21" s="48"/>
-    </row>
-    <row r="22" spans="1:60">
+      <c r="AY21" s="48"/>
+      <c r="AZ21" s="48"/>
+      <c r="BA21" s="48"/>
+      <c r="BB21" s="48"/>
+      <c r="BC21" s="48"/>
+    </row>
+    <row r="22" spans="1:65">
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -6103,16 +6266,16 @@
       <c r="AN22" s="33"/>
       <c r="AO22" s="57"/>
       <c r="AP22" s="55"/>
-      <c r="AQ22" s="49"/>
-      <c r="AR22" s="48"/>
+      <c r="AR22" s="49"/>
       <c r="AS22" s="48"/>
-      <c r="AT22" s="48"/>
-      <c r="AU22" s="48"/>
-      <c r="AV22" s="48"/>
-      <c r="AW22" s="48"/>
       <c r="AX22" s="48"/>
-    </row>
-    <row r="23" spans="1:60">
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="48"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+    </row>
+    <row r="23" spans="1:65">
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -6144,16 +6307,16 @@
       <c r="AN23" s="33"/>
       <c r="AO23" s="57"/>
       <c r="AP23" s="55"/>
-      <c r="AQ23" s="49"/>
-      <c r="AR23" s="48"/>
+      <c r="AR23" s="49"/>
       <c r="AS23" s="48"/>
-      <c r="AT23" s="48"/>
-      <c r="AU23" s="48"/>
-      <c r="AV23" s="48"/>
-      <c r="AW23" s="48"/>
       <c r="AX23" s="48"/>
-    </row>
-    <row r="24" spans="1:60">
+      <c r="AY23" s="48"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48"/>
+      <c r="BC23" s="48"/>
+    </row>
+    <row r="24" spans="1:65">
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -6185,16 +6348,16 @@
       <c r="AN24" s="33"/>
       <c r="AO24" s="57"/>
       <c r="AP24" s="55"/>
-      <c r="AQ24" s="49"/>
-      <c r="AR24" s="48"/>
+      <c r="AR24" s="49"/>
       <c r="AS24" s="48"/>
-      <c r="AT24" s="48"/>
-      <c r="AU24" s="48"/>
-      <c r="AV24" s="48"/>
-      <c r="AW24" s="48"/>
       <c r="AX24" s="48"/>
-    </row>
-    <row r="25" spans="1:60">
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="48"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="48"/>
+      <c r="BC24" s="48"/>
+    </row>
+    <row r="25" spans="1:65">
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
@@ -6226,16 +6389,16 @@
       <c r="AN25" s="33"/>
       <c r="AO25" s="57"/>
       <c r="AP25" s="55"/>
-      <c r="AQ25" s="49"/>
-      <c r="AR25" s="48"/>
+      <c r="AR25" s="49"/>
       <c r="AS25" s="48"/>
-      <c r="AT25" s="48"/>
-      <c r="AU25" s="48"/>
-      <c r="AV25" s="48"/>
-      <c r="AW25" s="48"/>
       <c r="AX25" s="48"/>
-    </row>
-    <row r="26" spans="1:60">
+      <c r="AY25" s="48"/>
+      <c r="AZ25" s="48"/>
+      <c r="BA25" s="48"/>
+      <c r="BB25" s="48"/>
+      <c r="BC25" s="48"/>
+    </row>
+    <row r="26" spans="1:65">
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -6267,16 +6430,16 @@
       <c r="AN26" s="33"/>
       <c r="AO26" s="57"/>
       <c r="AP26" s="55"/>
-      <c r="AQ26" s="49"/>
-      <c r="AR26" s="48"/>
+      <c r="AR26" s="49"/>
       <c r="AS26" s="48"/>
-      <c r="AT26" s="48"/>
-      <c r="AU26" s="48"/>
-      <c r="AV26" s="48"/>
-      <c r="AW26" s="48"/>
       <c r="AX26" s="48"/>
-    </row>
-    <row r="27" spans="1:60">
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="48"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="48"/>
+      <c r="BC26" s="48"/>
+    </row>
+    <row r="27" spans="1:65">
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -6308,16 +6471,16 @@
       <c r="AN27" s="33"/>
       <c r="AO27" s="57"/>
       <c r="AP27" s="55"/>
-      <c r="AQ27" s="49"/>
-      <c r="AR27" s="48"/>
+      <c r="AR27" s="49"/>
       <c r="AS27" s="48"/>
-      <c r="AT27" s="48"/>
-      <c r="AU27" s="48"/>
-      <c r="AV27" s="48"/>
-      <c r="AW27" s="48"/>
       <c r="AX27" s="48"/>
-    </row>
-    <row r="28" spans="1:60">
+      <c r="AY27" s="48"/>
+      <c r="AZ27" s="48"/>
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="48"/>
+      <c r="BC27" s="48"/>
+    </row>
+    <row r="28" spans="1:65">
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -6349,16 +6512,16 @@
       <c r="AN28" s="33"/>
       <c r="AO28" s="57"/>
       <c r="AP28" s="55"/>
-      <c r="AQ28" s="49"/>
-      <c r="AR28" s="48"/>
+      <c r="AR28" s="49"/>
       <c r="AS28" s="48"/>
-      <c r="AT28" s="48"/>
-      <c r="AU28" s="48"/>
-      <c r="AV28" s="48"/>
-      <c r="AW28" s="48"/>
       <c r="AX28" s="48"/>
-    </row>
-    <row r="29" spans="1:60">
+      <c r="AY28" s="48"/>
+      <c r="AZ28" s="48"/>
+      <c r="BA28" s="48"/>
+      <c r="BB28" s="48"/>
+      <c r="BC28" s="48"/>
+    </row>
+    <row r="29" spans="1:65">
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -6390,16 +6553,16 @@
       <c r="AN29" s="33"/>
       <c r="AO29" s="57"/>
       <c r="AP29" s="55"/>
-      <c r="AQ29" s="49"/>
-      <c r="AR29" s="48"/>
+      <c r="AR29" s="49"/>
       <c r="AS29" s="48"/>
-      <c r="AT29" s="48"/>
-      <c r="AU29" s="48"/>
-      <c r="AV29" s="48"/>
-      <c r="AW29" s="48"/>
       <c r="AX29" s="48"/>
-    </row>
-    <row r="30" spans="1:60">
+      <c r="AY29" s="48"/>
+      <c r="AZ29" s="48"/>
+      <c r="BA29" s="48"/>
+      <c r="BB29" s="48"/>
+      <c r="BC29" s="48"/>
+    </row>
+    <row r="30" spans="1:65">
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -6431,16 +6594,16 @@
       <c r="AN30" s="33"/>
       <c r="AO30" s="61"/>
       <c r="AP30" s="32"/>
-      <c r="AQ30" s="49"/>
-      <c r="AR30" s="48"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="45"/>
-      <c r="AU30" s="45"/>
-      <c r="AV30" s="45"/>
-      <c r="AW30" s="45"/>
+      <c r="AR30" s="49"/>
+      <c r="AS30" s="48"/>
       <c r="AX30" s="45"/>
-    </row>
-    <row r="31" spans="1:60">
+      <c r="AY30" s="45"/>
+      <c r="AZ30" s="45"/>
+      <c r="BA30" s="45"/>
+      <c r="BB30" s="45"/>
+      <c r="BC30" s="45"/>
+    </row>
+    <row r="31" spans="1:65">
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -6470,16 +6633,16 @@
       <c r="AL31" s="33"/>
       <c r="AM31" s="33"/>
       <c r="AN31" s="33"/>
-      <c r="AQ31" s="49"/>
-      <c r="AR31" s="48"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="45"/>
-      <c r="AU31" s="45"/>
-      <c r="AV31" s="45"/>
-      <c r="AW31" s="45"/>
+      <c r="AR31" s="49"/>
+      <c r="AS31" s="48"/>
       <c r="AX31" s="45"/>
-    </row>
-    <row r="32" spans="1:60">
+      <c r="AY31" s="45"/>
+      <c r="AZ31" s="45"/>
+      <c r="BA31" s="45"/>
+      <c r="BB31" s="45"/>
+      <c r="BC31" s="45"/>
+    </row>
+    <row r="32" spans="1:65">
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
@@ -6509,16 +6672,16 @@
       <c r="AL32" s="33"/>
       <c r="AM32" s="33"/>
       <c r="AN32" s="33"/>
-      <c r="AQ32" s="49"/>
-      <c r="AR32" s="48"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="45"/>
-      <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
+      <c r="AR32" s="49"/>
+      <c r="AS32" s="48"/>
       <c r="AX32" s="45"/>
-    </row>
-    <row r="33" spans="3:50">
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+    </row>
+    <row r="33" spans="3:55">
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
@@ -6536,16 +6699,16 @@
       <c r="AL33" s="33"/>
       <c r="AM33" s="33"/>
       <c r="AN33" s="33"/>
-      <c r="AQ33" s="49"/>
-      <c r="AR33" s="48"/>
-      <c r="AS33" s="45"/>
-      <c r="AT33" s="45"/>
-      <c r="AU33" s="45"/>
-      <c r="AV33" s="45"/>
-      <c r="AW33" s="45"/>
+      <c r="AR33" s="49"/>
+      <c r="AS33" s="48"/>
       <c r="AX33" s="45"/>
-    </row>
-    <row r="34" spans="3:50">
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+    </row>
+    <row r="34" spans="3:55">
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
@@ -6563,16 +6726,16 @@
       <c r="AL34" s="33"/>
       <c r="AM34" s="33"/>
       <c r="AN34" s="33"/>
-      <c r="AQ34" s="49"/>
-      <c r="AR34" s="48"/>
-      <c r="AS34" s="45"/>
-      <c r="AT34" s="45"/>
-      <c r="AU34" s="45"/>
-      <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
+      <c r="AR34" s="49"/>
+      <c r="AS34" s="48"/>
       <c r="AX34" s="45"/>
-    </row>
-    <row r="35" spans="3:50">
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+    </row>
+    <row r="35" spans="3:55">
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -6590,16 +6753,16 @@
       <c r="AL35" s="33"/>
       <c r="AM35" s="33"/>
       <c r="AN35" s="33"/>
-      <c r="AQ35" s="49"/>
-      <c r="AR35" s="48"/>
-      <c r="AS35" s="45"/>
-      <c r="AT35" s="45"/>
-      <c r="AU35" s="45"/>
-      <c r="AV35" s="45"/>
-      <c r="AW35" s="45"/>
+      <c r="AR35" s="49"/>
+      <c r="AS35" s="48"/>
       <c r="AX35" s="45"/>
-    </row>
-    <row r="36" spans="3:50">
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="45"/>
+      <c r="BA35" s="45"/>
+      <c r="BB35" s="45"/>
+      <c r="BC35" s="45"/>
+    </row>
+    <row r="36" spans="3:55">
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -6629,16 +6792,16 @@
       <c r="AL36" s="33"/>
       <c r="AM36" s="33"/>
       <c r="AN36" s="33"/>
-      <c r="AQ36" s="49"/>
-      <c r="AR36" s="48"/>
-      <c r="AS36" s="45"/>
-      <c r="AT36" s="45"/>
-      <c r="AU36" s="45"/>
-      <c r="AV36" s="45"/>
-      <c r="AW36" s="45"/>
+      <c r="AR36" s="49"/>
+      <c r="AS36" s="48"/>
       <c r="AX36" s="45"/>
-    </row>
-    <row r="37" spans="3:50">
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="45"/>
+      <c r="BA36" s="45"/>
+      <c r="BB36" s="45"/>
+      <c r="BC36" s="45"/>
+    </row>
+    <row r="37" spans="3:55">
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -6668,16 +6831,16 @@
       <c r="AL37" s="33"/>
       <c r="AM37" s="33"/>
       <c r="AN37" s="33"/>
-      <c r="AQ37" s="49"/>
-      <c r="AR37" s="48"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45"/>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
+      <c r="AR37" s="49"/>
+      <c r="AS37" s="48"/>
       <c r="AX37" s="45"/>
-    </row>
-    <row r="38" spans="3:50">
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="45"/>
+      <c r="BA37" s="45"/>
+      <c r="BB37" s="45"/>
+      <c r="BC37" s="45"/>
+    </row>
+    <row r="38" spans="3:55">
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -6707,16 +6870,16 @@
       <c r="AL38" s="33"/>
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
-      <c r="AQ38" s="49"/>
-      <c r="AR38" s="48"/>
-      <c r="AS38" s="45"/>
-      <c r="AT38" s="45"/>
-      <c r="AU38" s="45"/>
-      <c r="AV38" s="45"/>
-      <c r="AW38" s="45"/>
+      <c r="AR38" s="49"/>
+      <c r="AS38" s="48"/>
       <c r="AX38" s="45"/>
-    </row>
-    <row r="39" spans="3:50">
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="45"/>
+      <c r="BA38" s="45"/>
+      <c r="BB38" s="45"/>
+      <c r="BC38" s="45"/>
+    </row>
+    <row r="39" spans="3:55">
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -6746,57 +6909,57 @@
       <c r="AL39" s="33"/>
       <c r="AM39" s="33"/>
       <c r="AN39" s="33"/>
-      <c r="AQ39" s="49"/>
-      <c r="AR39" s="48"/>
-      <c r="AS39" s="45"/>
-      <c r="AT39" s="45"/>
-      <c r="AU39" s="45"/>
-      <c r="AV39" s="45"/>
-      <c r="AW39" s="45"/>
+      <c r="AR39" s="49"/>
+      <c r="AS39" s="48"/>
       <c r="AX39" s="45"/>
-    </row>
-    <row r="40" spans="3:50">
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="45"/>
+      <c r="BA39" s="45"/>
+      <c r="BB39" s="45"/>
+      <c r="BC39" s="45"/>
+    </row>
+    <row r="40" spans="3:55">
       <c r="AA40" s="28"/>
       <c r="AI40" s="80"/>
       <c r="AJ40" s="80"/>
-      <c r="AQ40" s="45"/>
       <c r="AR40" s="45"/>
       <c r="AS40" s="45"/>
-      <c r="AT40" s="45"/>
-      <c r="AU40" s="45"/>
-      <c r="AV40" s="45"/>
-      <c r="AW40" s="45"/>
       <c r="AX40" s="45"/>
-    </row>
-    <row r="41" spans="3:50">
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="45"/>
+      <c r="BB40" s="45"/>
+      <c r="BC40" s="45"/>
+    </row>
+    <row r="41" spans="3:55">
       <c r="AI41" s="80"/>
       <c r="AJ41" s="80"/>
     </row>
-    <row r="42" spans="3:50">
+    <row r="42" spans="3:55">
       <c r="AI42" s="80"/>
       <c r="AJ42" s="80"/>
     </row>
-    <row r="43" spans="3:50">
+    <row r="43" spans="3:55">
       <c r="AI43" s="80"/>
       <c r="AJ43" s="80"/>
     </row>
-    <row r="44" spans="3:50">
+    <row r="44" spans="3:55">
       <c r="AI44" s="80"/>
       <c r="AJ44" s="80"/>
     </row>
-    <row r="45" spans="3:50">
+    <row r="45" spans="3:55">
       <c r="AI45" s="80"/>
       <c r="AJ45" s="80"/>
     </row>
-    <row r="46" spans="3:50">
+    <row r="46" spans="3:55">
       <c r="AI46" s="80"/>
       <c r="AJ46" s="80"/>
     </row>
-    <row r="47" spans="3:50">
+    <row r="47" spans="3:55">
       <c r="AI47" s="80"/>
       <c r="AJ47" s="80"/>
     </row>
-    <row r="48" spans="3:50">
+    <row r="48" spans="3:55">
       <c r="AI48" s="80"/>
       <c r="AJ48" s="80"/>
     </row>
@@ -6833,8 +6996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6860,7 +7023,7 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="121" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="121"/>
       <c r="C1" s="121"/>
@@ -6870,7 +7033,7 @@
       <c r="G1" s="121"/>
       <c r="H1" s="121"/>
       <c r="I1" s="122" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J1" s="122"/>
       <c r="K1" s="122"/>
@@ -6883,7 +7046,7 @@
     </row>
     <row r="2" spans="1:17" ht="17">
       <c r="A2" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>31</v>
@@ -6901,28 +7064,28 @@
         <v>35</v>
       </c>
       <c r="G2" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="I2" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="J2" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="K2" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="L2" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="M2" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="68" t="s">
+      <c r="N2" s="68" t="s">
         <v>105</v>
-      </c>
-      <c r="N2" s="68" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -7089,7 +7252,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="73" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6" s="74">
         <v>-22.21</v>
@@ -7143,7 +7306,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="73" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B7" s="74">
         <v>1.71</v>
@@ -7197,7 +7360,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="73" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B8" s="74">
         <v>17.11</v>
@@ -7251,7 +7414,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="63"/>
       <c r="C9" s="63"/>
@@ -7286,7 +7449,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="120"/>
       <c r="B11" s="75" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="75"/>
       <c r="D11" s="120"/>
@@ -7302,10 +7465,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="66" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>110</v>
       </c>
       <c r="D12" s="66" t="s">
         <v>26</v>
@@ -7314,22 +7477,22 @@
         <v>27</v>
       </c>
       <c r="F12" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="H12" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="66" t="s">
+      <c r="I12" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="66" t="s">
-        <v>114</v>
-      </c>
       <c r="J12" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>108</v>
       </c>
       <c r="M12" s="66"/>
       <c r="O12" s="66"/>
@@ -7340,11 +7503,11 @@
         <v>ATM_EQ_SW</v>
       </c>
       <c r="B13" s="73">
-        <f t="shared" ref="B13:C15" si="7">M3</f>
+        <f>M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C13" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="B13:C15" si="7">N3</f>
         <v>1.0044225086731247</v>
       </c>
       <c r="D13" s="117">
@@ -7356,19 +7519,19 @@
         <v>1.0075218399408568</v>
       </c>
       <c r="F13" s="72">
-        <f t="shared" ref="F13:F27" si="8">LN(D13)</f>
+        <f>LN(D13)</f>
         <v>5.6690060748599133E-3</v>
       </c>
       <c r="G13" s="72">
-        <f t="shared" ref="G13:G27" si="9">LN(E13)</f>
+        <f t="shared" ref="G13:G27" si="8">LN(E13)</f>
         <v>7.4936919644022753E-3</v>
       </c>
       <c r="H13" s="72">
-        <f t="shared" ref="H13:I19" si="10">LN(B13)</f>
+        <f t="shared" ref="H13:I19" si="9">LN(B13)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I13" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4.412758119012896E-3</v>
       </c>
       <c r="J13" s="77">
@@ -7402,19 +7565,19 @@
         <v>0.99497700286985102</v>
       </c>
       <c r="F14" s="72">
+        <f t="shared" ref="F14:F27" si="10">LN(D14)</f>
+        <v>-3.3157633670658081E-3</v>
+      </c>
+      <c r="G14" s="72">
         <f t="shared" si="8"/>
-        <v>-3.3157633670658081E-3</v>
-      </c>
-      <c r="G14" s="72">
+        <v>-5.0356547842637621E-3</v>
+      </c>
+      <c r="H14" s="72">
         <f t="shared" si="9"/>
-        <v>-5.0356547842637621E-3</v>
-      </c>
-      <c r="H14" s="72">
-        <f t="shared" si="10"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I14" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -7440,19 +7603,19 @@
         <v>1.0043106480077921</v>
       </c>
       <c r="F15" s="72">
+        <f t="shared" si="10"/>
+        <v>3.8320385549917295E-4</v>
+      </c>
+      <c r="G15" s="72">
         <f t="shared" si="8"/>
-        <v>3.8320385549917295E-4</v>
-      </c>
-      <c r="G15" s="72">
+        <v>4.3013837783483656E-3</v>
+      </c>
+      <c r="H15" s="72">
         <f t="shared" si="9"/>
-        <v>4.3013837783483656E-3</v>
-      </c>
-      <c r="H15" s="72">
-        <f t="shared" si="10"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I15" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -7478,19 +7641,19 @@
         <v>1.0077071570383731</v>
       </c>
       <c r="F16" s="72">
+        <f t="shared" si="10"/>
+        <v>6.3855513126554056E-3</v>
+      </c>
+      <c r="G16" s="72">
         <f t="shared" si="8"/>
-        <v>6.3855513126554056E-3</v>
-      </c>
-      <c r="G16" s="72">
+        <v>7.6776086292741075E-3</v>
+      </c>
+      <c r="H16" s="72">
         <f t="shared" si="9"/>
-        <v>7.6776086292741075E-3</v>
-      </c>
-      <c r="H16" s="72">
-        <f t="shared" si="10"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I16" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -7516,19 +7679,19 @@
         <v>0.9951628615034982</v>
       </c>
       <c r="F17" s="72">
+        <f t="shared" si="10"/>
+        <v>-3.3736683280273967E-3</v>
+      </c>
+      <c r="G17" s="72">
         <f t="shared" si="8"/>
-        <v>-3.3736683280273967E-3</v>
-      </c>
-      <c r="G17" s="72">
+        <v>-4.8488753146248009E-3</v>
+      </c>
+      <c r="H17" s="72">
         <f t="shared" si="9"/>
-        <v>-4.8488753146248009E-3</v>
-      </c>
-      <c r="H17" s="72">
-        <f t="shared" si="10"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I17" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -7554,19 +7717,19 @@
         <v>1.0023860907979212</v>
       </c>
       <c r="F18" s="72">
+        <f t="shared" si="10"/>
+        <v>-8.2966123175853173E-4</v>
+      </c>
+      <c r="G18" s="72">
         <f t="shared" si="8"/>
-        <v>-8.2966123175853173E-4</v>
-      </c>
-      <c r="G18" s="72">
+        <v>2.3832486035312902E-3</v>
+      </c>
+      <c r="H18" s="72">
         <f t="shared" si="9"/>
-        <v>2.3832486035312902E-3</v>
-      </c>
-      <c r="H18" s="72">
-        <f t="shared" si="10"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I18" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -7592,19 +7755,19 @@
         <v>1.0057116133646442</v>
       </c>
       <c r="F19" s="72">
+        <f t="shared" si="10"/>
+        <v>5.0812199816469847E-3</v>
+      </c>
+      <c r="G19" s="72">
         <f t="shared" si="8"/>
-        <v>5.0812199816469847E-3</v>
-      </c>
-      <c r="G19" s="72">
+        <v>5.6953639452707308E-3</v>
+      </c>
+      <c r="H19" s="72">
         <f t="shared" si="9"/>
-        <v>5.6953639452707308E-3</v>
-      </c>
-      <c r="H19" s="72">
-        <f t="shared" si="10"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I19" s="72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -7624,11 +7787,11 @@
         <v>1.0049378092932522</v>
       </c>
       <c r="F20" s="72">
+        <f t="shared" si="10"/>
+        <v>-9.1141789753790732E-3</v>
+      </c>
+      <c r="G20" s="72">
         <f t="shared" si="8"/>
-        <v>-9.1141789753790732E-3</v>
-      </c>
-      <c r="G20" s="72">
-        <f t="shared" si="9"/>
         <v>4.9256582960658154E-3</v>
       </c>
       <c r="H20" s="72"/>
@@ -7656,11 +7819,11 @@
         <v>1.0054625917600983</v>
       </c>
       <c r="F21" s="72">
+        <f t="shared" si="10"/>
+        <v>5.7029884167436144E-3</v>
+      </c>
+      <c r="G21" s="72">
         <f t="shared" si="8"/>
-        <v>5.7029884167436144E-3</v>
-      </c>
-      <c r="G21" s="72">
-        <f t="shared" si="9"/>
         <v>5.4477259185061388E-3</v>
       </c>
       <c r="H21" s="72">
@@ -7694,11 +7857,11 @@
         <v>0.99378130442821833</v>
       </c>
       <c r="F22" s="72">
+        <f t="shared" si="10"/>
+        <v>-3.5945739634335372E-3</v>
+      </c>
+      <c r="G22" s="72">
         <f t="shared" si="8"/>
-        <v>-3.5945739634335372E-3</v>
-      </c>
-      <c r="G22" s="72">
-        <f t="shared" si="9"/>
         <v>-6.2381121983366193E-3</v>
       </c>
       <c r="H22" s="72">
@@ -7732,11 +7895,11 @@
         <v>1.0040343543858852</v>
       </c>
       <c r="F23" s="72">
+        <f t="shared" si="10"/>
+        <v>1.7966870305363727E-4</v>
+      </c>
+      <c r="G23" s="72">
         <f t="shared" si="8"/>
-        <v>1.7966870305363727E-4</v>
-      </c>
-      <c r="G23" s="72">
-        <f t="shared" si="9"/>
         <v>4.0262381999534996E-3</v>
       </c>
       <c r="H23" s="72">
@@ -7770,11 +7933,11 @@
         <v>1.0053599727245706</v>
       </c>
       <c r="F24" s="72">
+        <f t="shared" si="10"/>
+        <v>4.8686826228146419E-3</v>
+      </c>
+      <c r="G24" s="72">
         <f t="shared" si="8"/>
-        <v>4.8686826228146419E-3</v>
-      </c>
-      <c r="G24" s="72">
-        <f t="shared" si="9"/>
         <v>5.3456591947391319E-3</v>
       </c>
       <c r="H24" s="72">
@@ -7808,11 +7971,11 @@
         <v>1.0064676550191509</v>
       </c>
       <c r="F25" s="72">
+        <f t="shared" si="10"/>
+        <v>5.6228928832132777E-3</v>
+      </c>
+      <c r="G25" s="72">
         <f t="shared" si="8"/>
-        <v>5.6228928832132777E-3</v>
-      </c>
-      <c r="G25" s="72">
-        <f t="shared" si="9"/>
         <v>6.446829485110093E-3</v>
       </c>
       <c r="H25" s="72">
@@ -7846,11 +8009,11 @@
         <v>0.99474403428411884</v>
       </c>
       <c r="F26" s="72">
+        <f t="shared" si="10"/>
+        <v>-3.6734640658408848E-3</v>
+      </c>
+      <c r="G26" s="72">
         <f t="shared" si="8"/>
-        <v>-3.6734640658408848E-3</v>
-      </c>
-      <c r="G26" s="72">
-        <f t="shared" si="9"/>
         <v>-5.2698268942697113E-3</v>
       </c>
       <c r="H26" s="72">
@@ -7878,11 +8041,11 @@
         <v>1.0044001925480899</v>
       </c>
       <c r="F27" s="72">
+        <f t="shared" si="10"/>
+        <v>-6.5263177824188435E-3</v>
+      </c>
+      <c r="G27" s="72">
         <f t="shared" si="8"/>
-        <v>-6.5263177824188435E-3</v>
-      </c>
-      <c r="G27" s="72">
-        <f t="shared" si="9"/>
         <v>4.3905400058642007E-3</v>
       </c>
       <c r="H27" s="72"/>
@@ -7980,10 +8143,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A9B09D-1008-4441-AE31-949281019A29}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7997,180 +8160,121 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="M1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1">
-        <v>3.7990000000000002E-4</v>
-      </c>
-      <c r="O1" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
+        <v>182</v>
+      </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N2">
-        <v>2.0052E-3</v>
-      </c>
+        <v>3.7990000000000002E-4</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
       <c r="R2" s="84"/>
       <c r="S2" s="84"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="123" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="124" t="s">
-        <v>177</v>
-      </c>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
+      <c r="A3" s="1"/>
       <c r="M3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N3">
-        <v>0.51600000000000001</v>
+        <v>2.0052E-3</v>
       </c>
       <c r="R3" s="84"/>
       <c r="S3" s="84"/>
     </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:25">
+      <c r="A4" s="123" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="124" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N4">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+    </row>
+    <row r="5" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="119" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="119" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="119" t="s">
+        <v>142</v>
+      </c>
+      <c r="N5" s="119" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="119" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L4" s="119" t="s">
-        <v>145</v>
-      </c>
-      <c r="M4" s="119" t="s">
-        <v>143</v>
-      </c>
-      <c r="N4" s="119" t="s">
-        <v>146</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="119" t="s">
+      <c r="Q5" s="119" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="R4" s="119" t="s">
-        <v>96</v>
-      </c>
-      <c r="V4" s="119"/>
-      <c r="Y4" s="119"/>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="73">
-        <v>3.73422105E-3</v>
-      </c>
-      <c r="B5" s="73">
-        <v>3.6643675499999999E-3</v>
-      </c>
-      <c r="C5" s="73">
-        <v>3.7689117349450109E-3</v>
-      </c>
-      <c r="D5" s="73">
-        <v>7.7934998191650307E-3</v>
-      </c>
-      <c r="E5" s="118">
-        <v>2.1164798861162191E-3</v>
-      </c>
-      <c r="F5" s="73">
-        <v>0</v>
-      </c>
-      <c r="G5" s="73">
-        <v>3.6750148213719339E-3</v>
-      </c>
-      <c r="H5" s="73">
-        <v>3.6759553300949816E-3</v>
-      </c>
-      <c r="I5" s="73">
-        <v>3.7228017752489761E-3</v>
-      </c>
-      <c r="J5" s="73">
-        <v>7.7441640342372194E-3</v>
-      </c>
-      <c r="K5" s="118">
-        <v>2.109788966545483E-3</v>
-      </c>
-      <c r="L5" s="73">
-        <v>0</v>
-      </c>
-      <c r="M5" s="72" cm="1">
-        <f t="array" ref="M5">Rsolve18(E5,10,D5,E5,F5,$N$3,$N$2,$N$1)</f>
-        <v>2.0998927031414612E-3</v>
-      </c>
-      <c r="N5" s="72" cm="1">
-        <f t="array" ref="N5">Rsolve18(K5,10,J5,K5,L5,$N$3,$N$2,$N$1)</f>
-        <v>2.0934050628434882E-3</v>
-      </c>
-      <c r="O5" s="72">
-        <f>$N$1*(M5/$N$2)^$N$3</f>
-        <v>3.8905377024749663E-4</v>
-      </c>
-      <c r="P5" s="72">
-        <f>$N$1*(N5/$N$2)^$N$3</f>
-        <v>3.8843308121852137E-4</v>
-      </c>
-      <c r="Q5" s="91">
-        <f>(A5+R5*B5+A5*B5-(C5-O5)*(1+(1-R5)*B5))/(A5*(1+C5-O5))</f>
-        <v>0.20872209614007559</v>
-      </c>
-      <c r="R5" s="91">
-        <f>((A5-C5+O5)*(1+B5)/(A5*(1+C5-O5)) - (G5-I5+P5)*(1+H5)/(G5*(1+I5-P5)))/(H5/G5-B5/A5)</f>
-        <v>0.1159684103244177</v>
-      </c>
+      <c r="V5" s="119"/>
+      <c r="Y5" s="119"/>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="73">
@@ -8198,40 +8302,40 @@
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I6" s="73">
-        <v>3.7199285353648262E-3</v>
+        <v>3.7228017752489761E-3</v>
       </c>
       <c r="J6" s="73">
-        <v>7.7342329865834319E-3</v>
+        <v>7.7441640342372194E-3</v>
       </c>
       <c r="K6" s="118">
-        <v>2.105997079923158E-3</v>
+        <v>2.109788966545483E-3</v>
       </c>
       <c r="L6" s="73">
         <v>0</v>
       </c>
       <c r="M6" s="72" cm="1">
-        <f t="array" ref="M6">Rsolve18(E6,10,D6,E6,F6,$N$3,$N$2,$N$1)</f>
+        <f t="array" ref="M6">Rsolve18(E6,10,D6,E6,F6,$N$4,$N$3,$N$2)</f>
         <v>2.0998927031414612E-3</v>
       </c>
       <c r="N6" s="72" cm="1">
-        <f t="array" ref="N6">Rsolve18(K6,10,J6,K6,L6,$N$3,$N$2,$N$1)</f>
-        <v>2.0896547141455901E-3</v>
+        <f t="array" ref="N6">Rsolve18(K6,10,J6,K6,L6,$N$4,$N$3,$N$2)</f>
+        <v>2.0934050628434882E-3</v>
       </c>
       <c r="O6" s="72">
-        <f>$N$1*(M6/$N$2)^$N$3</f>
+        <f>$N$2*(M6/$N$3)^$N$4</f>
         <v>3.8905377024749663E-4</v>
       </c>
       <c r="P6" s="72">
-        <f>$N$1*(N6/$N$2)^$N$3</f>
-        <v>3.8807385113215798E-4</v>
+        <f>$N$2*(N6/$N$3)^$N$4</f>
+        <v>3.8843308121852137E-4</v>
       </c>
       <c r="Q6" s="91">
         <f>(A6+R6*B6+A6*B6-(C6-O6)*(1+(1-R6)*B6))/(A6*(1+C6-O6))</f>
-        <v>0.17329677501906443</v>
+        <v>0.20872209614007559</v>
       </c>
       <c r="R6" s="91">
         <f>((A6-C6+O6)*(1+B6)/(A6*(1+C6-O6)) - (G6-I6+P6)*(1+H6)/(G6*(1+I6-P6)))/(H6/G6-B6/A6)</f>
-        <v>7.9867779580351114E-2</v>
+        <v>0.1159684103244177</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -8242,13 +8346,13 @@
         <v>3.6643675499999999E-3</v>
       </c>
       <c r="C7" s="73">
-        <v>3.770760540076305E-3</v>
+        <v>3.7689117349450109E-3</v>
       </c>
       <c r="D7" s="73">
-        <v>7.7827523186501267E-3</v>
-      </c>
-      <c r="E7" s="73">
-        <v>2.1125489546459449E-3</v>
+        <v>7.7934998191650307E-3</v>
+      </c>
+      <c r="E7" s="118">
+        <v>2.1164798861162191E-3</v>
       </c>
       <c r="F7" s="73">
         <v>0</v>
@@ -8260,40 +8364,40 @@
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I7" s="73">
-        <v>3.7228017752489761E-3</v>
+        <v>3.7199285353648262E-3</v>
       </c>
       <c r="J7" s="73">
-        <v>7.7441640342372194E-3</v>
-      </c>
-      <c r="K7" s="73">
-        <v>2.109788966545483E-3</v>
+        <v>7.7342329865834319E-3</v>
+      </c>
+      <c r="K7" s="118">
+        <v>2.105997079923158E-3</v>
       </c>
       <c r="L7" s="73">
         <v>0</v>
       </c>
       <c r="M7" s="72" cm="1">
-        <f t="array" ref="M7">Rsolve18(E7,10,D7,E7,F7,$N$3,$N$2,$N$1)</f>
-        <v>2.096006943235472E-3</v>
+        <f t="array" ref="M7">Rsolve18(E7,10,D7,E7,F7,$N$4,$N$3,$N$2)</f>
+        <v>2.0998927031414612E-3</v>
       </c>
       <c r="N7" s="72" cm="1">
-        <f t="array" ref="N7">Rsolve18(K7,10,J7,K7,L7,$N$3,$N$2,$N$1)</f>
-        <v>2.0934050628434882E-3</v>
+        <f t="array" ref="N7">Rsolve18(K7,10,J7,K7,L7,$N$4,$N$3,$N$2)</f>
+        <v>2.0896547141455901E-3</v>
       </c>
       <c r="O7" s="72">
-        <f t="shared" ref="O7:O11" si="0">$N$1*(M7/$N$2)^$N$3</f>
-        <v>3.8868212138784054E-4</v>
+        <f>$N$2*(M7/$N$3)^$N$4</f>
+        <v>3.8905377024749663E-4</v>
       </c>
       <c r="P7" s="72">
-        <f t="shared" ref="P7:P11" si="1">$N$1*(N7/$N$2)^$N$3</f>
-        <v>3.8843308121852137E-4</v>
+        <f>$N$2*(N7/$N$3)^$N$4</f>
+        <v>3.8807385113215798E-4</v>
       </c>
       <c r="Q7" s="91">
-        <f t="shared" ref="Q7:Q11" si="2">(A7+R7*B7+A7*B7-(C7-O7)*(1+(1-R7)*B7))/(A7*(1+C7-O7))</f>
-        <v>0.17733587859609368</v>
+        <f>(A7+R7*B7+A7*B7-(C7-O7)*(1+(1-R7)*B7))/(A7*(1+C7-O7))</f>
+        <v>0.17329677501906443</v>
       </c>
       <c r="R7" s="91">
-        <f t="shared" ref="R7:R11" si="3">((A7-C7+O7)*(1+B7)/(A7*(1+C7-O7)) - (G7-I7+P7)*(1+H7)/(G7*(1+I7-P7)))/(H7/G7-B7/A7)</f>
-        <v>8.4590223076979915E-2</v>
+        <f>((A7-C7+O7)*(1+B7)/(A7*(1+C7-O7)) - (G7-I7+P7)*(1+H7)/(G7*(1+I7-P7)))/(H7/G7-B7/A7)</f>
+        <v>7.9867779580351114E-2</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -8322,40 +8426,40 @@
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I8" s="73">
-        <v>3.7199285353648262E-3</v>
+        <v>3.7228017752489761E-3</v>
       </c>
       <c r="J8" s="73">
-        <v>7.7342329865834319E-3</v>
+        <v>7.7441640342372194E-3</v>
       </c>
       <c r="K8" s="73">
-        <v>2.105997079923158E-3</v>
+        <v>2.109788966545483E-3</v>
       </c>
       <c r="L8" s="73">
         <v>0</v>
       </c>
       <c r="M8" s="72" cm="1">
-        <f t="array" ref="M8">Rsolve18(E8,10,D8,E8,F8,$N$3,$N$2,$N$1)</f>
+        <f t="array" ref="M8">Rsolve18(E8,10,D8,E8,F8,$N$4,$N$3,$N$2)</f>
         <v>2.096006943235472E-3</v>
       </c>
       <c r="N8" s="72" cm="1">
-        <f t="array" ref="N8">Rsolve18(K8,10,J8,K8,L8,$N$3,$N$2,$N$1)</f>
-        <v>2.0896547141455901E-3</v>
+        <f t="array" ref="N8">Rsolve18(K8,10,J8,K8,L8,$N$4,$N$3,$N$2)</f>
+        <v>2.0934050628434882E-3</v>
       </c>
       <c r="O8" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O8:O12" si="0">$N$2*(M8/$N$3)^$N$4</f>
         <v>3.8868212138784054E-4</v>
       </c>
       <c r="P8" s="72">
-        <f t="shared" si="1"/>
-        <v>3.8807385113215798E-4</v>
+        <f t="shared" ref="P8:P12" si="1">$N$2*(N8/$N$3)^$N$4</f>
+        <v>3.8843308121852137E-4</v>
       </c>
       <c r="Q8" s="91">
-        <f t="shared" si="2"/>
-        <v>0.14191055747508233</v>
+        <f t="shared" ref="Q8:Q12" si="2">(A8+R8*B8+A8*B8-(C8-O8)*(1+(1-R8)*B8))/(A8*(1+C8-O8))</f>
+        <v>0.17733587859609368</v>
       </c>
       <c r="R8" s="91">
-        <f t="shared" si="3"/>
-        <v>4.8489592332913341E-2</v>
+        <f t="shared" ref="R8:R12" si="3">((A8-C8+O8)*(1+B8)/(A8*(1+C8-O8)) - (G8-I8+P8)*(1+H8)/(G8*(1+I8-P8)))/(H8/G8-B8/A8)</f>
+        <v>8.4590223076979915E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -8366,13 +8470,13 @@
         <v>3.6643675499999999E-3</v>
       </c>
       <c r="C9" s="73">
-        <v>3.774157409185728E-3</v>
+        <v>3.770760540076305E-3</v>
       </c>
       <c r="D9" s="73">
-        <v>7.7878737502717673E-3</v>
+        <v>7.7827523186501267E-3</v>
       </c>
       <c r="E9" s="73">
-        <v>2.11205838421125E-3</v>
+        <v>2.1125489546459449E-3</v>
       </c>
       <c r="F9" s="73">
         <v>0</v>
@@ -8384,40 +8488,40 @@
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I9" s="73">
-        <v>3.7242631653031061E-3</v>
+        <v>3.7199285353648262E-3</v>
       </c>
       <c r="J9" s="73">
-        <v>7.742496580265385E-3</v>
+        <v>7.7342329865834319E-3</v>
       </c>
       <c r="K9" s="73">
-        <v>2.1092446228371492E-3</v>
+        <v>2.105997079923158E-3</v>
       </c>
       <c r="L9" s="73">
         <v>0</v>
       </c>
       <c r="M9" s="72" cm="1">
-        <f t="array" ref="M9">Rsolve18(E9,10,D9,E9,F9,$N$3,$N$2,$N$1)</f>
-        <v>2.0954956035312334E-3</v>
+        <f t="array" ref="M9">Rsolve18(E9,10,D9,E9,F9,$N$4,$N$3,$N$2)</f>
+        <v>2.096006943235472E-3</v>
       </c>
       <c r="N9" s="72" cm="1">
-        <f t="array" ref="N9">Rsolve18(K9,10,J9,K9,L9,$N$3,$N$2,$N$1)</f>
-        <v>2.0928676680247141E-3</v>
+        <f t="array" ref="N9">Rsolve18(K9,10,J9,K9,L9,$N$4,$N$3,$N$2)</f>
+        <v>2.0896547141455901E-3</v>
       </c>
       <c r="O9" s="72">
         <f t="shared" si="0"/>
-        <v>3.886331900931322E-4</v>
+        <v>3.8868212138784054E-4</v>
       </c>
       <c r="P9" s="72">
         <f t="shared" si="1"/>
-        <v>3.883816255649651E-4</v>
+        <v>3.8807385113215798E-4</v>
       </c>
       <c r="Q9" s="91">
         <f t="shared" si="2"/>
-        <v>0.14994727862657609</v>
+        <v>0.14191055747508233</v>
       </c>
       <c r="R9" s="91">
         <f t="shared" si="3"/>
-        <v>5.7620461575761298E-2</v>
+        <v>4.8489592332913341E-2</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -8428,13 +8532,13 @@
         <v>3.6643675499999999E-3</v>
       </c>
       <c r="C10" s="73">
-        <v>3.7661587198913019E-3</v>
+        <v>3.774157409185728E-3</v>
       </c>
       <c r="D10" s="73">
-        <v>7.7810024465572326E-3</v>
+        <v>7.7878737502717673E-3</v>
       </c>
       <c r="E10" s="73">
-        <v>2.1118562233900968E-3</v>
+        <v>2.11205838421125E-3</v>
       </c>
       <c r="F10" s="73">
         <v>0</v>
@@ -8458,16 +8562,16 @@
         <v>0</v>
       </c>
       <c r="M10" s="72" cm="1">
-        <f t="array" ref="M10">Rsolve18(E10,10,D10,E10,F10,$N$3,$N$2,$N$1)</f>
-        <v>2.0953215776226782E-3</v>
+        <f t="array" ref="M10">Rsolve18(E10,10,D10,E10,F10,$N$4,$N$3,$N$2)</f>
+        <v>2.0954956035312334E-3</v>
       </c>
       <c r="N10" s="72" cm="1">
-        <f t="array" ref="N10">Rsolve18(K10,10,J10,K10,L10,$N$3,$N$2,$N$1)</f>
+        <f t="array" ref="N10">Rsolve18(K10,10,J10,K10,L10,$N$4,$N$3,$N$2)</f>
         <v>2.0928676680247141E-3</v>
       </c>
       <c r="O10" s="72">
         <f t="shared" si="0"/>
-        <v>3.8861653582803027E-4</v>
+        <v>3.886331900931322E-4</v>
       </c>
       <c r="P10" s="72">
         <f t="shared" si="1"/>
@@ -8475,11 +8579,11 @@
       </c>
       <c r="Q10" s="91">
         <f t="shared" si="2"/>
-        <v>0.26277357755180591</v>
+        <v>0.14994727862657609</v>
       </c>
       <c r="R10" s="91">
         <f t="shared" si="3"/>
-        <v>0.17041789341507743</v>
+        <v>5.7620461575761298E-2</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -8490,13 +8594,13 @@
         <v>3.6643675499999999E-3</v>
       </c>
       <c r="C11" s="73">
-        <v>3.7730126315774341E-3</v>
+        <v>3.7661587198913019E-3</v>
       </c>
       <c r="D11" s="73">
-        <v>7.7872138239604956E-3</v>
+        <v>7.7810024465572326E-3</v>
       </c>
       <c r="E11" s="73">
-        <v>2.114038303996214E-3</v>
+        <v>2.1118562233900968E-3</v>
       </c>
       <c r="F11" s="73">
         <v>0</v>
@@ -8520,16 +8624,16 @@
         <v>0</v>
       </c>
       <c r="M11" s="72" cm="1">
-        <f t="array" ref="M11">Rsolve18(E11,10,D11,E11,F11,$N$3,$N$2,$N$1)</f>
-        <v>2.0974775933835267E-3</v>
+        <f t="array" ref="M11">Rsolve18(E11,10,D11,E11,F11,$N$4,$N$3,$N$2)</f>
+        <v>2.0953215776226782E-3</v>
       </c>
       <c r="N11" s="72" cm="1">
-        <f t="array" ref="N11">Rsolve18(K11,10,J11,K11,L11,$N$3,$N$2,$N$1)</f>
+        <f t="array" ref="N11">Rsolve18(K11,10,J11,K11,L11,$N$4,$N$3,$N$2)</f>
         <v>2.0928676680247141E-3</v>
       </c>
       <c r="O11" s="72">
         <f t="shared" si="0"/>
-        <v>3.888228191523488E-4</v>
+        <v>3.8861653582803027E-4</v>
       </c>
       <c r="P11" s="72">
         <f t="shared" si="1"/>
@@ -8537,37 +8641,99 @@
       </c>
       <c r="Q11" s="91">
         <f t="shared" si="2"/>
-        <v>0.16880903099141051</v>
+        <v>0.26277357755180591</v>
       </c>
       <c r="R11" s="91">
         <f t="shared" si="3"/>
+        <v>0.17041789341507743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="73">
+        <v>3.73422105E-3</v>
+      </c>
+      <c r="B12" s="73">
+        <v>3.6643675499999999E-3</v>
+      </c>
+      <c r="C12" s="73">
+        <v>3.7730126315774341E-3</v>
+      </c>
+      <c r="D12" s="73">
+        <v>7.7872138239604956E-3</v>
+      </c>
+      <c r="E12" s="73">
+        <v>2.114038303996214E-3</v>
+      </c>
+      <c r="F12" s="73">
+        <v>0</v>
+      </c>
+      <c r="G12" s="73">
+        <v>3.6750148213719339E-3</v>
+      </c>
+      <c r="H12" s="73">
+        <v>3.6759553300949816E-3</v>
+      </c>
+      <c r="I12" s="73">
+        <v>3.7242631653031061E-3</v>
+      </c>
+      <c r="J12" s="73">
+        <v>7.742496580265385E-3</v>
+      </c>
+      <c r="K12" s="73">
+        <v>2.1092446228371492E-3</v>
+      </c>
+      <c r="L12" s="73">
+        <v>0</v>
+      </c>
+      <c r="M12" s="72" cm="1">
+        <f t="array" ref="M12">Rsolve18(E12,10,D12,E12,F12,$N$4,$N$3,$N$2)</f>
+        <v>2.0974775933835267E-3</v>
+      </c>
+      <c r="N12" s="72" cm="1">
+        <f t="array" ref="N12">Rsolve18(K12,10,J12,K12,L12,$N$4,$N$3,$N$2)</f>
+        <v>2.0928676680247141E-3</v>
+      </c>
+      <c r="O12" s="72">
+        <f t="shared" si="0"/>
+        <v>3.888228191523488E-4</v>
+      </c>
+      <c r="P12" s="72">
+        <f t="shared" si="1"/>
+        <v>3.883816255649651E-4</v>
+      </c>
+      <c r="Q12" s="91">
+        <f t="shared" si="2"/>
+        <v>0.16880903099141051</v>
+      </c>
+      <c r="R12" s="91">
+        <f t="shared" si="3"/>
         <v>7.6477388081454753E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="Q13" s="91">
-        <f>AVERAGE(Q5:Q11)</f>
-        <v>0.18325645634287266</v>
-      </c>
-      <c r="R13" s="91">
-        <f>AVERAGE(R5:R11)</f>
-        <v>9.0490249769565087E-2</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="Q14" s="91">
-        <f>STDEV(Q5:Q11)</f>
+        <f>AVERAGE(Q6:Q12)</f>
+        <v>0.18325645634287266</v>
+      </c>
+      <c r="R14" s="91">
+        <f>AVERAGE(R6:R12)</f>
+        <v>9.0490249769565087E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="Q15" s="91">
+        <f>STDEV(Q6:Q12)</f>
         <v>4.1096294725866948E-2</v>
       </c>
-      <c r="R14" s="91">
-        <f>STDEV(R5:R11)</f>
+      <c r="R15" s="91">
+        <f>STDEV(R6:R12)</f>
         <v>4.1283674266355812E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8593,7 +8759,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -8604,28 +8770,28 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" s="87">
         <f>B12</f>
         <v>0.4623614635092998</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2" s="87">
         <f>C12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L2" s="86"/>
       <c r="M2" s="86"/>
@@ -8634,7 +8800,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="87">
         <f>B13</f>
@@ -8652,20 +8818,20 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="87">
         <v>1.026</v>
       </c>
       <c r="C4" s="85"/>
       <c r="E4" s="85" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4">
         <v>0.99819999999999998</v>
       </c>
       <c r="H4" s="85" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I4">
         <v>1.002</v>
@@ -8679,7 +8845,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="91">
         <f>1/B4</f>
@@ -8687,14 +8853,14 @@
       </c>
       <c r="C5" s="85"/>
       <c r="E5" s="85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F5" s="91">
         <f>1/F4</f>
         <v>1.0018032458425166</v>
       </c>
       <c r="H5" s="85" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I5" s="91">
         <f>1/I4</f>
@@ -8710,7 +8876,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="94">
         <f>B5/1000</f>
@@ -8718,14 +8884,14 @@
       </c>
       <c r="C6" s="85"/>
       <c r="E6" s="85" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F6" s="94">
         <f>F5/1000</f>
         <v>1.0018032458425166E-3</v>
       </c>
       <c r="H6" s="85" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I6" s="94">
         <f>I5/1000</f>
@@ -8754,7 +8920,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" s="99"/>
       <c r="C10" s="99"/>
@@ -8768,10 +8934,10 @@
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="F11" s="85"/>
       <c r="G11" s="24"/>
@@ -8790,7 +8956,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13">
         <v>8.0186890671505306E-3</v>

</xml_diff>

<commit_message>
Update concentration calculation in README
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740BCB92-82AE-C443-B4DB-225142A18541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C64CDD8-EECC-2949-89B4-3E26DAC09EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36620" yWindow="-5500" windowWidth="36620" windowHeight="21860" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-36620" yWindow="-5500" windowWidth="36620" windowHeight="21860" activeTab="3" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="scrambling" sheetId="4" r:id="rId3"/>
     <sheet name="concentration_constants" sheetId="5" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Rsolve18">_xlfn.LAMBDA(_xlpm.Rsam18,_xlpm.n,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17,       IF(_xlpm.n&gt;0,Rsolve18(_xlfn.LET(_xlpm.Rsam17,(1 + _xlpm.D17O / 1000) * _xlpm.RVSMOW17 * (_xlpm.Rsam18/_xlpm.RVSMOW18) ^ _xlpm.k,         _xlpm.Rsam46 - (_xlpm.Rsam45 - _xlpm.Rsam17) * _xlpm.Rsam17 - (_xlpm.Rsam45 - _xlpm.Rsam17) ^ 2/4),_xlpm.n-1,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17),               _xlpm.Rsam18))</definedName>
   </definedNames>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="214">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -546,9 +549,6 @@
     <t>freshwater L/g</t>
   </si>
   <si>
-    <t>Linest results</t>
-  </si>
-  <si>
     <t>SLOPE</t>
   </si>
   <si>
@@ -619,13 +619,106 @@
   </si>
   <si>
     <t>Requires recent version of Excel: 16.58 on the Current Channel, or 16.45 on the Beta Channel.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Mass analyzed (g)</t>
+  </si>
+  <si>
+    <t>N2O injected (nmol)</t>
+  </si>
+  <si>
+    <t>N2O Analyzed (nmol)</t>
+  </si>
+  <si>
+    <t>B6_lin_1</t>
+  </si>
+  <si>
+    <t>B6_lin_2</t>
+  </si>
+  <si>
+    <t>B6_lin_3</t>
+  </si>
+  <si>
+    <t>B6_lin_4</t>
+  </si>
+  <si>
+    <t>B6_lin_5</t>
+  </si>
+  <si>
+    <t>B6_lin_6</t>
+  </si>
+  <si>
+    <t>B6_lin_7</t>
+  </si>
+  <si>
+    <t>B6_lin_8</t>
+  </si>
+  <si>
+    <t>B6_lin_9</t>
+  </si>
+  <si>
+    <t>B6_lin_10</t>
+  </si>
+  <si>
+    <t>B6_lin_11</t>
+  </si>
+  <si>
+    <t>B6_lin_12</t>
+  </si>
+  <si>
+    <t>A01_lin_1</t>
+  </si>
+  <si>
+    <t>A01_lin_2</t>
+  </si>
+  <si>
+    <t>A01_lin_3</t>
+  </si>
+  <si>
+    <t>A01_lin_4</t>
+  </si>
+  <si>
+    <t>A01_lin_5</t>
+  </si>
+  <si>
+    <t>A01_lin_6</t>
+  </si>
+  <si>
+    <t>A01_lin_7</t>
+  </si>
+  <si>
+    <t>A01_lin_8</t>
+  </si>
+  <si>
+    <t>A01_lin_9</t>
+  </si>
+  <si>
+    <t>A01_lin_10</t>
+  </si>
+  <si>
+    <t>A01_lin_11</t>
+  </si>
+  <si>
+    <t>A01_lin_12</t>
+  </si>
+  <si>
+    <t>Example calibration curve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000000000000"/>
@@ -637,8 +730,9 @@
     <numFmt numFmtId="172" formatCode="0.00000000"/>
     <numFmt numFmtId="173" formatCode="0.0000E+00"/>
     <numFmt numFmtId="174" formatCode="0.000000"/>
+    <numFmt numFmtId="175" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -760,16 +854,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="MS Sans Serif"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="MS Sans Serif"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="MS Sans Serif"/>
     </font>
   </fonts>
@@ -1108,7 +1192,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1292,13 +1376,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1327,18 +1404,6 @@
     <xf numFmtId="2" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1353,6 +1418,20 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -2158,6 +2237,539 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1754025149841343E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>concentration_constants!$I$13:$I$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4.4359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7729999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.257</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.527999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.356000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39.363</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.569000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.9049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.589</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.387</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.463999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.53</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.491</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45.164999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.104999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44.793999999999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80.105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>83.078000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>89.230999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>concentration_constants!$H$13:$H$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2.4838709677419355</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4838709677419355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4838709677419355</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.612903225806452</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.67741935483871</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.870967741935484</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.35483870967742</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.967741935483871</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.935483870967742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.935483870967742</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.870967741935484</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.935483870967742</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.612903225806452</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.870967741935484</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.483870967741936</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39.225806451612904</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39.741935483870968</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>38.967741935483872</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8BFF-D44F-8E42-49C84A2BCB7E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="246077232"/>
+        <c:axId val="264632128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="246077232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Area 44</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264632128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="264632128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N2O (nmol)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246077232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2198,7 +2810,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2757,6 +3925,257 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDACCB66-B834-B245-954E-DA42B85A8A74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="raw_data"/>
+      <sheetName val="Ref_curves"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="61">
+          <cell r="H61">
+            <v>2.4838709677419355</v>
+          </cell>
+          <cell r="I61">
+            <v>4.4359999999999999</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="H62">
+            <v>2.4838709677419355</v>
+          </cell>
+          <cell r="I62">
+            <v>5.0330000000000004</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="H63">
+            <v>2.4838709677419355</v>
+          </cell>
+          <cell r="I63">
+            <v>5.1760000000000002</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="H64">
+            <v>5</v>
+          </cell>
+          <cell r="I64">
+            <v>9.7729999999999997</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="H65">
+            <v>5</v>
+          </cell>
+          <cell r="I65">
+            <v>9.73</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="H66">
+            <v>5</v>
+          </cell>
+          <cell r="I66">
+            <v>10.257</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="H67">
+            <v>9.612903225806452</v>
+          </cell>
+          <cell r="I67">
+            <v>20.527999999999999</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="H68">
+            <v>9.67741935483871</v>
+          </cell>
+          <cell r="I68">
+            <v>20.356000000000002</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="H69">
+            <v>10</v>
+          </cell>
+          <cell r="I69">
+            <v>20.91</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="H70">
+            <v>19.870967741935484</v>
+          </cell>
+          <cell r="I70">
+            <v>40.497</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="H71">
+            <v>19.35483870967742</v>
+          </cell>
+          <cell r="I71">
+            <v>39.363</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="H72">
+            <v>20</v>
+          </cell>
+          <cell r="I72">
+            <v>41.569000000000003</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="H73">
+            <v>4.967741935483871</v>
+          </cell>
+          <cell r="I73">
+            <v>9.9049999999999994</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="H74">
+            <v>4.935483870967742</v>
+          </cell>
+          <cell r="I74">
+            <v>10.589</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="H75">
+            <v>5</v>
+          </cell>
+          <cell r="I75">
+            <v>11.387</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="H76">
+            <v>9.935483870967742</v>
+          </cell>
+          <cell r="I76">
+            <v>23.463999999999999</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="H77">
+            <v>9.870967741935484</v>
+          </cell>
+          <cell r="I77">
+            <v>22.53</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="H78">
+            <v>9.935483870967742</v>
+          </cell>
+          <cell r="I78">
+            <v>22.491</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="H79">
+            <v>19.612903225806452</v>
+          </cell>
+          <cell r="I79">
+            <v>45.164999999999999</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="H80">
+            <v>19.870967741935484</v>
+          </cell>
+          <cell r="I80">
+            <v>43.104999999999997</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="H81">
+            <v>19.483870967741936</v>
+          </cell>
+          <cell r="I81">
+            <v>44.793999999999997</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="H82">
+            <v>39.225806451612904</v>
+          </cell>
+          <cell r="I82">
+            <v>80.105000000000004</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="H83">
+            <v>39.741935483870968</v>
+          </cell>
+          <cell r="I83">
+            <v>83.078000000000003</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="H84">
+            <v>38.967741935483872</v>
+          </cell>
+          <cell r="I84">
+            <v>89.230999999999995</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3056,8 +4475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AW36" sqref="AW36"/>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BI4" sqref="BI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3116,13 +4535,13 @@
       <c r="AO1" s="58"/>
       <c r="AP1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="118" t="s">
+      <c r="AT1" s="113" t="s">
+        <v>179</v>
+      </c>
+      <c r="AU1" s="113"/>
+      <c r="AV1" s="113"/>
+      <c r="AX1" s="38" t="s">
         <v>180</v>
-      </c>
-      <c r="AU1" s="118"/>
-      <c r="AV1" s="118"/>
-      <c r="AX1" s="38" t="s">
-        <v>181</v>
       </c>
       <c r="AY1" s="38"/>
       <c r="AZ1" s="38" t="s">
@@ -3133,17 +4552,17 @@
       <c r="BC1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="BE1" s="106" t="s">
-        <v>165</v>
-      </c>
-      <c r="BF1" s="106"/>
-      <c r="BG1" s="106"/>
-      <c r="BH1" s="106"/>
-      <c r="BI1" s="107"/>
-      <c r="BJ1" s="108"/>
-      <c r="BK1" s="108"/>
-      <c r="BL1" s="108"/>
-      <c r="BM1" s="108"/>
+      <c r="BE1" s="101" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF1" s="101"/>
+      <c r="BG1" s="101"/>
+      <c r="BH1" s="101"/>
+      <c r="BI1" s="102"/>
+      <c r="BJ1" s="103"/>
+      <c r="BK1" s="103"/>
+      <c r="BL1" s="103"/>
+      <c r="BM1" s="103"/>
     </row>
     <row r="2" spans="1:65" ht="52" thickBot="1">
       <c r="A2" s="8" t="s">
@@ -3265,13 +4684,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="119" t="s">
+      <c r="AT2" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="120" t="s">
+      <c r="AU2" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="121" t="s">
+      <c r="AV2" s="116" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -3293,32 +4712,32 @@
         <v>34</v>
       </c>
       <c r="BD2" s="44"/>
-      <c r="BE2" s="109" t="s">
+      <c r="BE2" s="104" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF2" s="104" t="s">
         <v>166</v>
       </c>
-      <c r="BF2" s="109" t="s">
+      <c r="BG2" s="104" t="s">
         <v>167</v>
       </c>
-      <c r="BG2" s="109" t="s">
+      <c r="BH2" s="104" t="s">
         <v>168</v>
       </c>
-      <c r="BH2" s="109" t="s">
+      <c r="BI2" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="BI2" s="110" t="s">
+      <c r="BJ2" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="BJ2" s="111" t="s">
+      <c r="BK2" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="BK2" s="112" t="s">
+      <c r="BL2" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="BL2" s="111" t="s">
-        <v>173</v>
-      </c>
-      <c r="BM2" s="113" t="s">
-        <v>172</v>
+      <c r="BM2" s="108" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:65" ht="17" thickBot="1">
@@ -3489,7 +4908,7 @@
         <v>156</v>
       </c>
       <c r="BH3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI3" s="81">
         <f>BG3*concentration_constants!$B$6</f>
@@ -4049,7 +5468,7 @@
         <v>156</v>
       </c>
       <c r="BH6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI6" s="81">
         <f>BG6*concentration_constants!$B$6</f>
@@ -4606,7 +6025,7 @@
         <v>156</v>
       </c>
       <c r="BH9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI9" s="81">
         <f>BG9*concentration_constants!$B$6</f>
@@ -4977,7 +6396,7 @@
         <v>156</v>
       </c>
       <c r="BH11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI11" s="81">
         <f>BG11*concentration_constants!$B$6</f>
@@ -5517,7 +6936,7 @@
         <v>156</v>
       </c>
       <c r="BH14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI14" s="81">
         <f>BG14*concentration_constants!$B$6</f>
@@ -5697,7 +7116,7 @@
         <v>156</v>
       </c>
       <c r="BH15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BI15" s="81">
         <f>BG15*concentration_constants!$B$6</f>
@@ -7003,7 +8422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
@@ -7032,28 +8451,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="123" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="123" t="s">
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
       <c r="S1" s="73" t="s">
         <v>125</v>
       </c>
@@ -7065,73 +8484,73 @@
       <c r="Y1" s="64"/>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" ht="39" customHeight="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="127" t="s">
+      <c r="C2" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="127" t="s">
+      <c r="E2" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="127" t="s">
+      <c r="F2" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="128" t="s">
+      <c r="G2" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="128" t="s">
+      <c r="H2" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="128" t="s">
+      <c r="I2" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="128" t="s">
+      <c r="K2" s="119" t="s">
         <v>102</v>
       </c>
-      <c r="L2" s="128" t="s">
+      <c r="L2" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="128" t="s">
+      <c r="M2" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="N2" s="128" t="s">
+      <c r="N2" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="129" t="s">
+      <c r="P2" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="130" t="s">
+      <c r="Q2" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="131" t="s">
+      <c r="R2" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="130" t="s">
+      <c r="S2" s="121" t="s">
         <v>108</v>
       </c>
-      <c r="T2" s="130" t="s">
+      <c r="T2" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="U2" s="130" t="s">
+      <c r="U2" s="121" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="130" t="s">
+      <c r="V2" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="130" t="s">
+      <c r="W2" s="121" t="s">
         <v>112</v>
       </c>
-      <c r="X2" s="130" t="s">
+      <c r="X2" s="121" t="s">
         <v>113</v>
       </c>
       <c r="Y2" s="1" t="s">
@@ -7194,40 +8613,40 @@
         <f>L3/size_correction!Y$3</f>
         <v>1.0044225086731247</v>
       </c>
-      <c r="P3" s="114" t="str">
+      <c r="P3" s="109" t="str">
         <f>size_correction!D3</f>
         <v>ATM_EQ_SW</v>
       </c>
-      <c r="Q3" s="114">
+      <c r="Q3" s="109">
         <f>size_correction!AF3</f>
         <v>1.0056851052976181</v>
       </c>
-      <c r="R3" s="114">
+      <c r="R3" s="109">
         <f>size_correction!AG3</f>
         <v>1.0075218399408568</v>
       </c>
       <c r="S3" s="71">
-        <f>M3</f>
+        <f t="shared" ref="S3:T5" si="0">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="T3" s="71">
-        <f>N3</f>
+        <f t="shared" si="0"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="U3" s="70">
-        <f>LN(Q3)</f>
+        <f t="shared" ref="U3:U17" si="1">LN(Q3)</f>
         <v>5.6690060748599133E-3</v>
       </c>
       <c r="V3" s="70">
-        <f>LN(R3)</f>
+        <f t="shared" ref="V3:V17" si="2">LN(R3)</f>
         <v>7.4936919644022753E-3</v>
       </c>
       <c r="W3" s="70">
-        <f t="shared" ref="W3:X9" si="0">LN(S3)</f>
+        <f t="shared" ref="W3:X9" si="3">LN(S3)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X3" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
       <c r="Y3" s="75">
@@ -7257,7 +8676,7 @@
         <v>32.729999999999997</v>
       </c>
       <c r="F4" s="72">
-        <f t="shared" ref="F4:F8" si="1">B4-C4</f>
+        <f t="shared" ref="F4:F8" si="4">B4-C4</f>
         <v>18.419999999999998</v>
       </c>
       <c r="G4" s="68">
@@ -7292,40 +8711,40 @@
         <f>L4/size_correction!Y$3</f>
         <v>0.99323347721175648</v>
       </c>
-      <c r="P4" s="114" t="str">
+      <c r="P4" s="109" t="str">
         <f>size_correction!D4</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="Q4" s="114">
+      <c r="Q4" s="109">
         <f>size_correction!AF4</f>
         <v>0.99668972770557829</v>
       </c>
-      <c r="R4" s="114">
+      <c r="R4" s="109">
         <f>size_correction!AG4</f>
         <v>0.99497700286985102</v>
       </c>
       <c r="S4" s="71">
-        <f>M4</f>
+        <f t="shared" si="0"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="T4" s="71">
-        <f>N4</f>
+        <f t="shared" si="0"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="U4" s="70">
-        <f>LN(Q4)</f>
+        <f t="shared" si="1"/>
         <v>-3.3157633670658081E-3</v>
       </c>
       <c r="V4" s="70">
-        <f>LN(R4)</f>
+        <f t="shared" si="2"/>
         <v>-5.0356547842637621E-3</v>
       </c>
       <c r="W4" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X4" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -7347,31 +8766,31 @@
         <v>41.949257311111111</v>
       </c>
       <c r="F5" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.25581632613833338</v>
       </c>
       <c r="G5" s="68">
-        <f t="shared" ref="G5:H8" si="2">(B5/1000+1)*0.0036765</f>
+        <f t="shared" ref="G5:H8" si="5">(B5/1000+1)*0.0036765</f>
         <v>3.6750148213719339E-3</v>
       </c>
       <c r="H5" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I5" s="68">
-        <f t="shared" ref="I5:I8" si="3">(E5/1000+1)*0.0020052</f>
+        <f t="shared" ref="I5:I8" si="6">(E5/1000+1)*0.0020052</f>
         <v>2.0893166507602399E-3</v>
       </c>
       <c r="J5" s="68">
-        <f t="shared" ref="J5:J8" si="4">(I5/0.0020052)^0.516*0.0003799</f>
+        <f t="shared" ref="J5:J8" si="7">(I5/0.0020052)^0.516*0.0003799</f>
         <v>3.8804145413997107E-4</v>
       </c>
       <c r="K5" s="69">
-        <f t="shared" ref="K5:K8" si="5">G5+H5+J5</f>
+        <f t="shared" ref="K5:K8" si="8">G5+H5+J5</f>
         <v>7.7390116056068863E-3</v>
       </c>
       <c r="L5" s="69">
-        <f t="shared" ref="L5:L8" si="6">(G5+H5)*J5+I5+G5*H5</f>
+        <f t="shared" ref="L5:L8" si="9">(G5+H5)*J5+I5+G5*H5</f>
         <v>2.1056783222279545E-3</v>
       </c>
       <c r="M5" s="70">
@@ -7382,46 +8801,46 @@
         <f>L5/size_correction!Y$3</f>
         <v>1.0020859042591113</v>
       </c>
-      <c r="P5" s="114" t="str">
+      <c r="P5" s="109" t="str">
         <f>size_correction!D5</f>
         <v>B6_ref_1</v>
       </c>
-      <c r="Q5" s="114">
+      <c r="Q5" s="109">
         <f>size_correction!AF5</f>
         <v>1.0003832772874761</v>
       </c>
-      <c r="R5" s="114">
+      <c r="R5" s="109">
         <f>size_correction!AG5</f>
         <v>1.0043106480077921</v>
       </c>
       <c r="S5" s="71">
-        <f>M5</f>
+        <f t="shared" si="0"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="T5" s="71">
-        <f>N5</f>
+        <f t="shared" si="0"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="U5" s="70">
-        <f>LN(Q5)</f>
+        <f t="shared" si="1"/>
         <v>3.8320385549917295E-4</v>
       </c>
       <c r="V5" s="70">
-        <f>LN(R5)</f>
+        <f t="shared" si="2"/>
         <v>4.3013837783483656E-3</v>
       </c>
       <c r="W5" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X5" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A6" s="71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" s="72">
         <v>-22.21</v>
@@ -7430,38 +8849,38 @@
         <v>-49.28</v>
       </c>
       <c r="D6" s="72">
-        <f t="shared" ref="D6:D8" si="7">AVERAGE(B6:C6)</f>
+        <f t="shared" ref="D6:D8" si="10">AVERAGE(B6:C6)</f>
         <v>-35.745000000000005</v>
       </c>
       <c r="E6" s="72">
         <v>26.94</v>
       </c>
       <c r="F6" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>27.07</v>
       </c>
       <c r="G6" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.5948449350000004E-3</v>
       </c>
       <c r="H6" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.49532208E-3</v>
       </c>
       <c r="I6" s="68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0592200879999997E-3</v>
       </c>
       <c r="J6" s="68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.8514702697154833E-4</v>
       </c>
       <c r="K6" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.4753140419715489E-3</v>
       </c>
       <c r="L6" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.0745159856220404E-3</v>
       </c>
       <c r="M6" s="70">
@@ -7472,46 +8891,46 @@
         <f>L6/size_correction!Y$3</f>
         <v>0.98725584312065418</v>
       </c>
-      <c r="P6" s="114" t="str">
+      <c r="P6" s="109" t="str">
         <f>size_correction!D6</f>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="Q6" s="114">
+      <c r="Q6" s="109">
         <f>size_correction!AF6</f>
         <v>1.0064059824102283</v>
       </c>
-      <c r="R6" s="114">
+      <c r="R6" s="109">
         <f>size_correction!AG6</f>
         <v>1.0077071570383731</v>
       </c>
       <c r="S6" s="71">
-        <f>M3</f>
+        <f t="shared" ref="S6:T8" si="11">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="T6" s="71">
-        <f>N3</f>
+        <f t="shared" si="11"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="U6" s="70">
-        <f>LN(Q6)</f>
+        <f t="shared" si="1"/>
         <v>6.3855513126554056E-3</v>
       </c>
       <c r="V6" s="70">
-        <f>LN(R6)</f>
+        <f t="shared" si="2"/>
         <v>7.6776086292741075E-3</v>
       </c>
       <c r="W6" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X6" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A7" s="71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="72">
         <v>1.71</v>
@@ -7520,14 +8939,14 @@
         <v>94.44</v>
       </c>
       <c r="D7" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>48.074999999999996</v>
       </c>
       <c r="E7" s="72">
         <v>36.01</v>
       </c>
       <c r="F7" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-92.73</v>
       </c>
       <c r="G7" s="68">
@@ -7535,23 +8954,23 @@
         <v>3.6827868150000006E-3</v>
       </c>
       <c r="H7" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.0237086600000008E-3</v>
       </c>
       <c r="I7" s="68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0774072520000002E-3</v>
       </c>
       <c r="J7" s="68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.8689853960154226E-4</v>
       </c>
       <c r="K7" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.0933940146015442E-3</v>
       </c>
       <c r="L7" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.0952073450451725E-3</v>
       </c>
       <c r="M7" s="70">
@@ -7562,46 +8981,46 @@
         <f>L7/size_correction!Y$3</f>
         <v>0.99710279808951241</v>
       </c>
-      <c r="P7" s="114" t="str">
+      <c r="P7" s="109" t="str">
         <f>size_correction!D7</f>
         <v>S2_ref_2</v>
       </c>
-      <c r="Q7" s="114">
+      <c r="Q7" s="109">
         <f>size_correction!AF7</f>
         <v>0.99663201609671503</v>
       </c>
-      <c r="R7" s="114">
+      <c r="R7" s="109">
         <f>size_correction!AG7</f>
         <v>0.9951628615034982</v>
       </c>
       <c r="S7" s="71">
-        <f>M4</f>
+        <f t="shared" si="11"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="T7" s="71">
-        <f>N4</f>
+        <f t="shared" si="11"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="U7" s="70">
-        <f>LN(Q7)</f>
+        <f t="shared" si="1"/>
         <v>-3.3736683280273967E-3</v>
       </c>
       <c r="V7" s="70">
-        <f>LN(R7)</f>
+        <f t="shared" si="2"/>
         <v>-4.8488753146248009E-3</v>
       </c>
       <c r="W7" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X7" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A8" s="71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="72">
         <v>17.11</v>
@@ -7610,38 +9029,38 @@
         <v>-3.43</v>
       </c>
       <c r="D8" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>6.84</v>
       </c>
       <c r="E8" s="72">
         <v>35.29</v>
       </c>
       <c r="F8" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20.54</v>
       </c>
       <c r="G8" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.7394049149999998E-3</v>
       </c>
       <c r="H8" s="68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.6638896049999998E-3</v>
       </c>
       <c r="I8" s="68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0759635080000003E-3</v>
       </c>
       <c r="J8" s="68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.8675977189798279E-4</v>
       </c>
       <c r="K8" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.7900542918979817E-3</v>
       </c>
       <c r="L8" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2.0925275712968031E-3</v>
       </c>
       <c r="M8" s="70">
@@ -7652,40 +9071,40 @@
         <f>L8/size_correction!Y$3</f>
         <v>0.99582750191939118</v>
       </c>
-      <c r="P8" s="114" t="str">
+      <c r="P8" s="109" t="str">
         <f>size_correction!D8</f>
         <v>B6_ref_2</v>
       </c>
-      <c r="Q8" s="114">
+      <c r="Q8" s="109">
         <f>size_correction!AF8</f>
         <v>0.99917068284195976</v>
       </c>
-      <c r="R8" s="114">
+      <c r="R8" s="109">
         <f>size_correction!AG8</f>
         <v>1.0023860907979212</v>
       </c>
       <c r="S8" s="71">
-        <f>M5</f>
+        <f t="shared" si="11"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="T8" s="71">
-        <f>N5</f>
+        <f t="shared" si="11"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="U8" s="70">
-        <f>LN(Q8)</f>
+        <f t="shared" si="1"/>
         <v>-8.2966123175853173E-4</v>
       </c>
       <c r="V8" s="70">
-        <f>LN(R8)</f>
+        <f t="shared" si="2"/>
         <v>2.3832486035312902E-3</v>
       </c>
       <c r="W8" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X8" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -7703,15 +9122,15 @@
       <c r="L9" s="63"/>
       <c r="M9" s="67"/>
       <c r="N9" s="67"/>
-      <c r="P9" s="114" t="str">
+      <c r="P9" s="109" t="str">
         <f>size_correction!D9</f>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="Q9" s="114">
+      <c r="Q9" s="109">
         <f>size_correction!AF9</f>
         <v>1.0050941512728657</v>
       </c>
-      <c r="R9" s="114">
+      <c r="R9" s="109">
         <f>size_correction!AG9</f>
         <v>1.0057116133646442</v>
       </c>
@@ -7724,19 +9143,19 @@
         <v>1.0044225086731247</v>
       </c>
       <c r="U9" s="70">
-        <f>LN(Q9)</f>
+        <f t="shared" si="1"/>
         <v>5.0812199816469847E-3</v>
       </c>
       <c r="V9" s="70">
-        <f>LN(R9)</f>
+        <f t="shared" si="2"/>
         <v>5.6953639452707308E-3</v>
       </c>
       <c r="W9" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X9" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -7754,26 +9173,26 @@
       <c r="M10" s="65"/>
       <c r="N10" s="65"/>
       <c r="O10" s="65"/>
-      <c r="P10" s="114" t="str">
+      <c r="P10" s="109" t="str">
         <f>size_correction!D10</f>
         <v>DI</v>
       </c>
-      <c r="Q10" s="114">
+      <c r="Q10" s="109">
         <f>size_correction!AF10</f>
         <v>0.99092722925764687</v>
       </c>
-      <c r="R10" s="114">
+      <c r="R10" s="109">
         <f>size_correction!AG10</f>
         <v>1.0049378092932522</v>
       </c>
       <c r="S10" s="71"/>
       <c r="T10" s="71"/>
       <c r="U10" s="70">
-        <f>LN(Q10)</f>
+        <f t="shared" si="1"/>
         <v>-9.1141789753790732E-3</v>
       </c>
       <c r="V10" s="70">
-        <f>LN(R10)</f>
+        <f t="shared" si="2"/>
         <v>4.9256582960658154E-3</v>
       </c>
       <c r="W10" s="70"/>
@@ -7782,132 +9201,132 @@
     <row r="11" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="L11" s="65"/>
       <c r="M11" s="65"/>
-      <c r="P11" s="114" t="str">
+      <c r="P11" s="109" t="str">
         <f>size_correction!D11</f>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="Q11" s="114">
+      <c r="Q11" s="109">
         <f>size_correction!AF11</f>
         <v>1.0057192814133826</v>
       </c>
-      <c r="R11" s="114">
+      <c r="R11" s="109">
         <f>size_correction!AG11</f>
         <v>1.0054625917600983</v>
       </c>
       <c r="S11" s="71">
-        <f>M3</f>
+        <f t="shared" ref="S11:T13" si="12">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="T11" s="71">
-        <f>N3</f>
+        <f t="shared" si="12"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="U11" s="70">
-        <f>LN(Q11)</f>
+        <f t="shared" si="1"/>
         <v>5.7029884167436144E-3</v>
       </c>
       <c r="V11" s="70">
-        <f>LN(R11)</f>
+        <f t="shared" si="2"/>
         <v>5.4477259185061388E-3</v>
       </c>
       <c r="W11" s="70">
-        <f t="shared" ref="W11:X16" si="8">LN(S11)</f>
+        <f t="shared" ref="W11:X16" si="13">LN(S11)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X11" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1">
       <c r="M12" s="65"/>
-      <c r="P12" s="114" t="str">
+      <c r="P12" s="109" t="str">
         <f>size_correction!D12</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="Q12" s="114">
+      <c r="Q12" s="109">
         <f>size_correction!AF12</f>
         <v>0.99641187878361481</v>
       </c>
-      <c r="R12" s="114">
+      <c r="R12" s="109">
         <f>size_correction!AG12</f>
         <v>0.99378130442821833</v>
       </c>
       <c r="S12" s="71">
-        <f>M4</f>
+        <f t="shared" si="12"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="T12" s="71">
-        <f>N4</f>
+        <f t="shared" si="12"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="U12" s="70">
-        <f>LN(Q12)</f>
+        <f t="shared" si="1"/>
         <v>-3.5945739634335372E-3</v>
       </c>
       <c r="V12" s="70">
-        <f>LN(R12)</f>
+        <f t="shared" si="2"/>
         <v>-6.2381121983366193E-3</v>
       </c>
       <c r="W12" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X12" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
       <c r="Y12"/>
       <c r="Z12"/>
     </row>
     <row r="13" spans="1:26" ht="18" thickTop="1" thickBot="1">
-      <c r="P13" s="114" t="str">
+      <c r="P13" s="109" t="str">
         <f>size_correction!D13</f>
         <v>B6_ref_1</v>
       </c>
-      <c r="Q13" s="114">
+      <c r="Q13" s="109">
         <f>size_correction!AF13</f>
         <v>1.0001796848444418</v>
       </c>
-      <c r="R13" s="114">
+      <c r="R13" s="109">
         <f>size_correction!AG13</f>
         <v>1.0040343543858852</v>
       </c>
       <c r="S13" s="71">
-        <f>M5</f>
+        <f t="shared" si="12"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="T13" s="71">
-        <f>N5</f>
+        <f t="shared" si="12"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="U13" s="70">
-        <f>LN(Q13)</f>
+        <f t="shared" si="1"/>
         <v>1.7966870305363727E-4</v>
       </c>
       <c r="V13" s="70">
-        <f>LN(R13)</f>
+        <f t="shared" si="2"/>
         <v>4.0262381999534996E-3</v>
       </c>
       <c r="W13" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X13" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="18" thickTop="1" thickBot="1">
-      <c r="P14" s="114" t="str">
+      <c r="P14" s="109" t="str">
         <f>size_correction!D14</f>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="Q14" s="114">
+      <c r="Q14" s="109">
         <f>size_correction!AF14</f>
         <v>1.0048805539160894</v>
       </c>
-      <c r="R14" s="114">
+      <c r="R14" s="109">
         <f>size_correction!AG14</f>
         <v>1.0053599727245706</v>
       </c>
@@ -7920,32 +9339,32 @@
         <v>1.0044225086731247</v>
       </c>
       <c r="U14" s="70">
-        <f>LN(Q14)</f>
+        <f t="shared" si="1"/>
         <v>4.8686826228146419E-3</v>
       </c>
       <c r="V14" s="70">
-        <f>LN(R14)</f>
+        <f t="shared" si="2"/>
         <v>5.3456591947391319E-3</v>
       </c>
       <c r="W14" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X14" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="18" thickTop="1" thickBot="1">
-      <c r="P15" s="114" t="str">
+      <c r="P15" s="109" t="str">
         <f>size_correction!D15</f>
         <v>ATM_EQ_SW_3</v>
       </c>
-      <c r="Q15" s="114">
+      <c r="Q15" s="109">
         <f>size_correction!AF15</f>
         <v>1.0056387310168626</v>
       </c>
-      <c r="R15" s="114">
+      <c r="R15" s="109">
         <f>size_correction!AG15</f>
         <v>1.0064676550191509</v>
       </c>
@@ -7958,32 +9377,32 @@
         <v>1.0044225086731247</v>
       </c>
       <c r="U15" s="70">
-        <f>LN(Q15)</f>
+        <f t="shared" si="1"/>
         <v>5.6228928832132777E-3</v>
       </c>
       <c r="V15" s="70">
-        <f>LN(R15)</f>
+        <f t="shared" si="2"/>
         <v>6.446829485110093E-3</v>
       </c>
       <c r="W15" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X15" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="18" thickTop="1" thickBot="1">
-      <c r="P16" s="114" t="str">
+      <c r="P16" s="109" t="str">
         <f>size_correction!D16</f>
         <v>S2_ref_2</v>
       </c>
-      <c r="Q16" s="114">
+      <c r="Q16" s="109">
         <f>size_correction!AF16</f>
         <v>0.99633327484903467</v>
       </c>
-      <c r="R16" s="114">
+      <c r="R16" s="109">
         <f>size_correction!AG16</f>
         <v>0.99474403428411884</v>
       </c>
@@ -7996,43 +9415,43 @@
         <v>0.99323347721175648</v>
       </c>
       <c r="U16" s="70">
-        <f>LN(Q16)</f>
+        <f t="shared" si="1"/>
         <v>-3.6734640658408848E-3</v>
       </c>
       <c r="V16" s="70">
-        <f>LN(R16)</f>
+        <f t="shared" si="2"/>
         <v>-5.2698268942697113E-3</v>
       </c>
       <c r="W16" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X16" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
     <row r="17" spans="4:24" ht="18" thickTop="1" thickBot="1">
-      <c r="P17" s="114" t="str">
+      <c r="P17" s="109" t="str">
         <f>size_correction!D17</f>
         <v>DI</v>
       </c>
-      <c r="Q17" s="114">
+      <c r="Q17" s="109">
         <f>size_correction!AF17</f>
         <v>0.99349493237592013</v>
       </c>
-      <c r="R17" s="114">
+      <c r="R17" s="109">
         <f>size_correction!AG17</f>
         <v>1.0044001925480899</v>
       </c>
       <c r="S17" s="71"/>
       <c r="T17" s="71"/>
       <c r="U17" s="70">
-        <f>LN(Q17)</f>
+        <f t="shared" si="1"/>
         <v>-6.5263177824188435E-3</v>
       </c>
       <c r="V17" s="70">
-        <f>LN(R17)</f>
+        <f t="shared" si="2"/>
         <v>4.3905400058642007E-3</v>
       </c>
       <c r="W17" s="70"/>
@@ -8148,12 +9567,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M2" t="s">
         <v>126</v>
@@ -8181,22 +9600,22 @@
       <c r="S3" s="81"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="126" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="125" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
       <c r="M4" t="s">
         <v>129</v>
       </c>
@@ -8222,7 +9641,7 @@
       <c r="E5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="116" t="s">
+      <c r="F5" s="111" t="s">
         <v>141</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -8240,13 +9659,13 @@
       <c r="K5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L5" s="116" t="s">
+      <c r="L5" s="111" t="s">
         <v>144</v>
       </c>
-      <c r="M5" s="116" t="s">
+      <c r="M5" s="111" t="s">
         <v>142</v>
       </c>
-      <c r="N5" s="116" t="s">
+      <c r="N5" s="111" t="s">
         <v>145</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -8255,14 +9674,14 @@
       <c r="P5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q5" s="116" t="s">
+      <c r="Q5" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="R5" s="116" t="s">
+      <c r="R5" s="111" t="s">
         <v>95</v>
       </c>
-      <c r="V5" s="116"/>
-      <c r="Y5" s="116"/>
+      <c r="V5" s="111"/>
+      <c r="Y5" s="111"/>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="71">
@@ -8277,7 +9696,7 @@
       <c r="D6" s="71">
         <v>7.7934998191650307E-3</v>
       </c>
-      <c r="E6" s="115">
+      <c r="E6" s="110">
         <v>2.1164798861162191E-3</v>
       </c>
       <c r="F6" s="71">
@@ -8295,7 +9714,7 @@
       <c r="J6" s="71">
         <v>7.7441640342372194E-3</v>
       </c>
-      <c r="K6" s="115">
+      <c r="K6" s="110">
         <v>2.109788966545483E-3</v>
       </c>
       <c r="L6" s="71">
@@ -8339,7 +9758,7 @@
       <c r="D7" s="71">
         <v>7.7934998191650307E-3</v>
       </c>
-      <c r="E7" s="115">
+      <c r="E7" s="110">
         <v>2.1164798861162191E-3</v>
       </c>
       <c r="F7" s="71">
@@ -8357,7 +9776,7 @@
       <c r="J7" s="71">
         <v>7.7342329865834319E-3</v>
       </c>
-      <c r="K7" s="115">
+      <c r="K7" s="110">
         <v>2.105997079923158E-3</v>
       </c>
       <c r="L7" s="71">
@@ -8729,10 +10148,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29A51B0-D147-5349-B907-3D4412BB9071}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8745,7 +10164,7 @@
     <col min="13" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -8756,47 +10175,47 @@
       <c r="M1" s="83"/>
       <c r="N1" s="83"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="84">
-        <f>B12</f>
+        <f>R12</f>
         <v>0.4623614635092998</v>
       </c>
       <c r="C2" s="82" t="s">
         <v>148</v>
       </c>
       <c r="D2" s="84">
-        <f>C12</f>
+        <f>S12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L2" s="83"/>
       <c r="M2" s="83"/>
       <c r="N2" s="83"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>149</v>
       </c>
       <c r="B3" s="84">
-        <f>B13</f>
+        <f>R13</f>
         <v>8.0186890671505306E-3</v>
       </c>
       <c r="C3" s="82"/>
       <c r="D3" s="84">
-        <f>C13</f>
+        <f>S13</f>
         <v>0.30903560626553517</v>
       </c>
       <c r="L3" s="83"/>
@@ -8804,7 +10223,7 @@
       <c r="N3" s="83"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -8831,7 +10250,7 @@
       <c r="P4" s="87"/>
       <c r="Q4" s="87"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -8862,7 +10281,7 @@
       <c r="Q5" s="90"/>
       <c r="R5" s="85"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -8892,23 +10311,23 @@
       <c r="P6" s="85"/>
       <c r="Q6" s="90"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="L7" s="85"/>
       <c r="M7" s="93"/>
       <c r="N7" s="85"/>
     </row>
-    <row r="8" spans="1:18" ht="18">
+    <row r="8" spans="1:19" ht="18">
       <c r="L8" s="85"/>
       <c r="M8" s="94"/>
       <c r="N8" s="85"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="M9" s="95"/>
       <c r="N9" s="85"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" s="96" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="B10" s="96"/>
       <c r="C10" s="96"/>
@@ -8920,92 +10339,953 @@
       <c r="M10" s="95"/>
       <c r="N10" s="85"/>
     </row>
-    <row r="11" spans="1:18">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:19">
+      <c r="R11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="127" t="s">
+        <v>147</v>
+      </c>
+      <c r="R12" s="81" cm="1">
+        <f t="array" ref="R12:S16">LINEST(H13:H36,I13:I36,TRUE,TRUE)</f>
+        <v>0.4623614635092998</v>
+      </c>
+      <c r="S12" s="81">
+        <v>0.10975712247295455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="128">
+        <v>44232</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13">
+        <v>264</v>
+      </c>
+      <c r="E13">
+        <v>110</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13" si="0">D13-E13</f>
+        <v>154</v>
+      </c>
+      <c r="G13">
+        <v>2.5</v>
+      </c>
+      <c r="H13">
+        <f>F13/155*G13</f>
+        <v>2.4838709677419355</v>
+      </c>
+      <c r="I13">
+        <v>4.4359999999999999</v>
+      </c>
+      <c r="J13" s="50">
+        <f>H13/I13</f>
+        <v>0.5599348439454318</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F11" s="82"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="B12">
-        <v>0.4623614635092998</v>
-      </c>
-      <c r="C12">
-        <v>0.10975712247295455</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13">
+      <c r="R13" s="81">
         <v>8.0186890671505306E-3</v>
       </c>
-      <c r="C13">
+      <c r="S13" s="81">
         <v>0.30903560626553517</v>
       </c>
-      <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="1:18">
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="128">
+        <f t="shared" ref="A14:A24" si="1">A13</f>
+        <v>44232</v>
+      </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14">
+        <v>262</v>
+      </c>
+      <c r="E14">
+        <v>108</v>
+      </c>
+      <c r="F14">
+        <f>D14-E14</f>
+        <v>154</v>
+      </c>
+      <c r="G14">
+        <v>2.5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H36" si="2">F14/155*G14</f>
+        <v>2.4838709677419355</v>
+      </c>
+      <c r="I14">
+        <v>5.0330000000000004</v>
+      </c>
+      <c r="J14" s="50">
+        <f t="shared" ref="J14:J36" si="3">H14/I14</f>
+        <v>0.49351698147068057</v>
+      </c>
+      <c r="R14">
         <v>0.99342642117731605</v>
       </c>
-      <c r="C14" s="50">
+      <c r="S14">
         <v>0.96347094633189312</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-    </row>
-    <row r="15" spans="1:18">
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
       <c r="B15">
+        <f t="shared" ref="B15:B24" si="4">B14+1</f>
+        <v>3</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15">
+        <v>264</v>
+      </c>
+      <c r="E15">
+        <v>110</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:F25" si="5">D15-E15</f>
+        <v>154</v>
+      </c>
+      <c r="G15">
+        <v>2.5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>2.4838709677419355</v>
+      </c>
+      <c r="I15">
+        <v>5.1760000000000002</v>
+      </c>
+      <c r="J15" s="50">
+        <f t="shared" si="3"/>
+        <v>0.47988233534426883</v>
+      </c>
+      <c r="R15">
         <v>3324.7309959200538</v>
       </c>
-      <c r="C15" s="50">
+      <c r="S15">
         <v>22</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="I15" s="50"/>
-    </row>
-    <row r="16" spans="1:18">
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
       <c r="B16">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16">
+        <v>264</v>
+      </c>
+      <c r="E16">
+        <v>109</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>9.7729999999999997</v>
+      </c>
+      <c r="J16" s="50">
+        <f t="shared" si="3"/>
+        <v>0.51161362938708688</v>
+      </c>
+      <c r="R16">
         <v>3086.2688691129169</v>
       </c>
-      <c r="C16">
+      <c r="S16">
         <v>20.422077817364819</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="50"/>
-      <c r="I16" s="50"/>
-    </row>
-    <row r="17" spans="4:10">
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="103"/>
-    </row>
-    <row r="18" spans="4:10">
-      <c r="G18" s="50"/>
-      <c r="I18" s="104"/>
-    </row>
-    <row r="20" spans="4:10">
-      <c r="J20" s="105"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17">
+        <v>264</v>
+      </c>
+      <c r="E17">
+        <v>109</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>9.73</v>
+      </c>
+      <c r="J17" s="50">
+        <f t="shared" si="3"/>
+        <v>0.51387461459403905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18">
+        <v>265</v>
+      </c>
+      <c r="E18">
+        <v>110</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="G18">
+        <f>G19/2</f>
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>10.257</v>
+      </c>
+      <c r="J18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.4874719703617042</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19">
+        <v>258</v>
+      </c>
+      <c r="E19">
+        <v>109</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>149</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>9.612903225806452</v>
+      </c>
+      <c r="I19">
+        <v>20.527999999999999</v>
+      </c>
+      <c r="J19" s="50">
+        <f t="shared" si="3"/>
+        <v>0.46828250320569237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="128">
+        <f t="shared" si="1"/>
+        <v>44232</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20">
+        <v>259</v>
+      </c>
+      <c r="E20">
+        <v>109</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="I20">
+        <v>20.356000000000002</v>
+      </c>
+      <c r="J20" s="50">
+        <f t="shared" si="3"/>
+        <v>0.47540869300642113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="128">
+        <v>44233</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21">
+        <v>264</v>
+      </c>
+      <c r="E21">
+        <v>109</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>20.91</v>
+      </c>
+      <c r="J21" s="50">
+        <f t="shared" si="3"/>
+        <v>0.47824007651841222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="128">
+        <f t="shared" si="1"/>
+        <v>44233</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22">
+        <v>262</v>
+      </c>
+      <c r="E22">
+        <v>108</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>154</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>19.870967741935484</v>
+      </c>
+      <c r="I22">
+        <v>40.497</v>
+      </c>
+      <c r="J22" s="50">
+        <f t="shared" si="3"/>
+        <v>0.49067752529657715</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="128">
+        <f t="shared" si="1"/>
+        <v>44233</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23">
+        <v>259</v>
+      </c>
+      <c r="E23">
+        <v>109</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>19.35483870967742</v>
+      </c>
+      <c r="I23">
+        <v>39.363</v>
+      </c>
+      <c r="J23" s="50">
+        <f t="shared" si="3"/>
+        <v>0.49170131112154614</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="128">
+        <f t="shared" si="1"/>
+        <v>44233</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>263</v>
+      </c>
+      <c r="E24">
+        <v>108</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I24">
+        <v>41.569000000000003</v>
+      </c>
+      <c r="J24" s="50">
+        <f t="shared" si="3"/>
+        <v>0.48112776347759145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="128">
+        <v>44248</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25">
+        <v>265</v>
+      </c>
+      <c r="E25">
+        <v>111</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="5"/>
+        <v>154</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>4.967741935483871</v>
+      </c>
+      <c r="I25">
+        <v>9.9049999999999994</v>
+      </c>
+      <c r="J25" s="50">
+        <f t="shared" si="3"/>
+        <v>0.50153881226490371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="128">
+        <v>44249</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26">
+        <v>264</v>
+      </c>
+      <c r="E26">
+        <v>111</v>
+      </c>
+      <c r="F26">
+        <f>D26-E26</f>
+        <v>153</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>4.935483870967742</v>
+      </c>
+      <c r="I26">
+        <v>10.589</v>
+      </c>
+      <c r="J26" s="50">
+        <f t="shared" si="3"/>
+        <v>0.46609536981468902</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="128">
+        <v>44250</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ref="B27:B36" si="6">B26+1</f>
+        <v>3</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27">
+        <v>264</v>
+      </c>
+      <c r="E27">
+        <v>109</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F36" si="7">D27-E27</f>
+        <v>155</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>11.387</v>
+      </c>
+      <c r="J27" s="50">
+        <f t="shared" si="3"/>
+        <v>0.43909721612364977</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="128">
+        <v>44251</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28">
+        <v>263</v>
+      </c>
+      <c r="E28">
+        <v>109</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>9.935483870967742</v>
+      </c>
+      <c r="I28">
+        <v>23.463999999999999</v>
+      </c>
+      <c r="J28" s="50">
+        <f t="shared" si="3"/>
+        <v>0.42343521441219495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="128">
+        <v>44252</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29">
+        <v>264</v>
+      </c>
+      <c r="E29">
+        <v>111</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>153</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>9.870967741935484</v>
+      </c>
+      <c r="I29">
+        <v>22.53</v>
+      </c>
+      <c r="J29" s="50">
+        <f t="shared" si="3"/>
+        <v>0.43812551007259137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="128">
+        <v>44253</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30">
+        <v>263</v>
+      </c>
+      <c r="E30">
+        <v>109</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>9.935483870967742</v>
+      </c>
+      <c r="I30">
+        <v>22.491</v>
+      </c>
+      <c r="J30" s="50">
+        <f t="shared" si="3"/>
+        <v>0.44175376243687442</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="128">
+        <v>44254</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31">
+        <v>259</v>
+      </c>
+      <c r="E31">
+        <v>107</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="7"/>
+        <v>152</v>
+      </c>
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>19.612903225806452</v>
+      </c>
+      <c r="I31">
+        <v>45.164999999999999</v>
+      </c>
+      <c r="J31" s="50">
+        <f t="shared" si="3"/>
+        <v>0.43425004374640658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="128">
+        <v>44255</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D32">
+        <v>263</v>
+      </c>
+      <c r="E32">
+        <v>109</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="G32">
+        <v>20</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>19.870967741935484</v>
+      </c>
+      <c r="I32">
+        <v>43.104999999999997</v>
+      </c>
+      <c r="J32" s="50">
+        <f t="shared" si="3"/>
+        <v>0.46098985597808806</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="128">
+        <v>44256</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D33">
+        <v>259</v>
+      </c>
+      <c r="E33">
+        <v>108</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="7"/>
+        <v>151</v>
+      </c>
+      <c r="G33">
+        <v>20</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>19.483870967741936</v>
+      </c>
+      <c r="I33">
+        <v>44.793999999999997</v>
+      </c>
+      <c r="J33" s="50">
+        <f t="shared" si="3"/>
+        <v>0.43496608848823365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="128">
+        <v>44257</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34">
+        <v>258</v>
+      </c>
+      <c r="E34">
+        <v>106</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="7"/>
+        <v>152</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <f>F34/155*G34</f>
+        <v>39.225806451612904</v>
+      </c>
+      <c r="I34">
+        <v>80.105000000000004</v>
+      </c>
+      <c r="J34" s="50">
+        <f t="shared" si="3"/>
+        <v>0.48967987580816308</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="128">
+        <v>44258</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35">
+        <v>263</v>
+      </c>
+      <c r="E35">
+        <v>109</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="G35">
+        <v>40</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>39.741935483870968</v>
+      </c>
+      <c r="I35">
+        <v>83.078000000000003</v>
+      </c>
+      <c r="J35" s="50">
+        <f t="shared" si="3"/>
+        <v>0.47836894826393228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="128">
+        <v>44259</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36">
+        <v>261</v>
+      </c>
+      <c r="E36">
+        <v>110</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="7"/>
+        <v>151</v>
+      </c>
+      <c r="G36">
+        <v>40</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>38.967741935483872</v>
+      </c>
+      <c r="I36">
+        <v>89.230999999999995</v>
+      </c>
+      <c r="J36" s="50">
+        <f t="shared" si="3"/>
+        <v>0.43670632331234521</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small changes to flowchart
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C64CDD8-EECC-2949-89B4-3E26DAC09EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0FFDD0-6383-B943-A5D5-3B98B44C9E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36620" yWindow="-5500" windowWidth="36620" windowHeight="21860" activeTab="3" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -10151,7 +10151,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
get rid of old constants.py and constants.csv; start adding isotope standards
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E327A18-0C90-DB4D-9E05-AC7FD8FAEC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C761BFA-60E4-7944-93EF-751E388425F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35340" yWindow="-5500" windowWidth="28760" windowHeight="15820" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -7657,7 +7657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -8842,8 +8842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A9B09D-1008-4441-AE31-949281019A29}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add adjustable isotope standards to pre-scrambling 17R calculation
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C761BFA-60E4-7944-93EF-751E388425F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB24A5B-9122-A74E-9D76-0EE8C6A88ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="182">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -348,9 +348,6 @@
     <t>run_date</t>
   </si>
   <si>
-    <t>PYTHON/MATLAB INPUTS</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -433,9 +430,6 @@
   </si>
   <si>
     <t>scale normalized 45R and 46R</t>
-  </si>
-  <si>
-    <t>USER INPUT: CALIBRATED DELTA VALS FOR EACH REFERENCE MATERIAL</t>
   </si>
   <si>
     <t>USER INPUT: REFERENCE APPROPRIATE VALUES IN COLUMNS M &amp; N</t>
@@ -609,7 +603,16 @@
     <t>CA08214</t>
   </si>
   <si>
-    <t>"ref_tag" should match scale_normalization tab</t>
+    <t>PYTHON INPUTS: CALIBRATED DELTA VALS FOR EACH REFERENCE MATERIAL</t>
+  </si>
+  <si>
+    <t>PYTHON INPUTS</t>
+  </si>
+  <si>
+    <t>D17O</t>
+  </si>
+  <si>
+    <t>SCRAMBLING OUTPUT: CHECK VALUES</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +887,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1146,7 +1155,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1371,6 +1380,13 @@
     <xf numFmtId="169" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3845,10 +3861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
-  <dimension ref="A1:BH54"/>
+  <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AT27" sqref="AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3864,26 +3880,26 @@
     <col min="35" max="35" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="40" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.6640625" style="61" customWidth="1"/>
-    <col min="42" max="42" width="10.1640625" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" style="44" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" customWidth="1"/>
-    <col min="46" max="46" width="13.5" customWidth="1"/>
+    <col min="41" max="41" width="7.83203125" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" style="61" customWidth="1"/>
+    <col min="43" max="43" width="10.1640625" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" style="44" customWidth="1"/>
+    <col min="45" max="45" width="14.33203125" customWidth="1"/>
+    <col min="46" max="48" width="10.83203125" style="50"/>
+    <col min="51" max="51" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="17" thickBot="1">
+    <row r="1" spans="1:65" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="G1" s="1"/>
       <c r="W1" s="71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
@@ -3895,42 +3911,48 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AI1" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AJ1" s="74"/>
       <c r="AL1" s="51" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="AM1" s="51"/>
       <c r="AN1" s="51"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="45"/>
-      <c r="AS1" s="38" t="s">
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="45"/>
+      <c r="AT1" s="125" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU1" s="125"/>
+      <c r="AV1" s="125"/>
+      <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38" t="s">
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38" t="s">
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="103" t="s">
-        <v>164</v>
-      </c>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="103"/>
-      <c r="BC1" s="103"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="105"/>
-      <c r="BF1" s="105"/>
-      <c r="BG1" s="105"/>
-      <c r="BH1" s="105"/>
-    </row>
-    <row r="2" spans="1:60" ht="52" thickBot="1">
+      <c r="BE1" s="103" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF1" s="103"/>
+      <c r="BG1" s="103"/>
+      <c r="BH1" s="103"/>
+      <c r="BI1" s="104"/>
+      <c r="BJ1" s="105"/>
+      <c r="BK1" s="105"/>
+      <c r="BL1" s="105"/>
+      <c r="BM1" s="105"/>
+    </row>
+    <row r="2" spans="1:65" ht="52" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>93</v>
       </c>
@@ -4023,10 +4045,10 @@
         <v>27</v>
       </c>
       <c r="AI2" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ2" s="75" t="s">
         <v>120</v>
-      </c>
-      <c r="AJ2" s="75" t="s">
-        <v>121</v>
       </c>
       <c r="AK2" s="23"/>
       <c r="AL2" s="55" t="s">
@@ -4038,66 +4060,78 @@
       <c r="AN2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AO2" s="59" t="s">
+      <c r="AO2" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="AP2" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AP2" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ2" s="46" t="s">
+      <c r="AR2" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="39" t="s">
+      <c r="AT2" s="126" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU2" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="128" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="AT2" s="39" t="s">
+      <c r="AY2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AU2" s="39" t="s">
+      <c r="AZ2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AV2" s="39" t="s">
+      <c r="BA2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AW2" s="39" t="s">
+      <c r="BB2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="40" t="s">
+      <c r="BC2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="106" t="s">
+      <c r="BD2" s="44"/>
+      <c r="BE2" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="BF2" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="BG2" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="BA2" s="106" t="s">
+      <c r="BH2" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="BB2" s="106" t="s">
+      <c r="BI2" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="BC2" s="106" t="s">
+      <c r="BJ2" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="BD2" s="107" t="s">
+      <c r="BK2" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="BE2" s="108" t="s">
+      <c r="BL2" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="BF2" s="109" t="s">
-        <v>171</v>
-      </c>
-      <c r="BG2" s="108" t="s">
-        <v>172</v>
-      </c>
-      <c r="BH2" s="110" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:60" ht="17" thickBot="1">
+      <c r="BM2" s="110" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" ht="17" thickBot="1">
       <c r="A3">
         <v>201204</v>
       </c>
@@ -4213,74 +4247,86 @@
         <f>AJ3*$Y$3</f>
         <v>2.1161148587211971E-3</v>
       </c>
-      <c r="AO3" s="56">
+      <c r="AO3" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP3" s="57">
+      <c r="AQ3" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ3" s="47">
+      <c r="AR3" s="47">
         <f>A3</f>
         <v>201204</v>
       </c>
-      <c r="AR3" t="str">
+      <c r="AS3" t="str">
         <f>D3</f>
         <v>ATM_EQ_SW</v>
       </c>
-      <c r="AS3" s="50">
+      <c r="AT3" s="50">
+        <v>6.8201115908412797</v>
+      </c>
+      <c r="AU3" s="50">
+        <v>11.9612881084705</v>
+      </c>
+      <c r="AV3" s="50">
+        <v>23.3107973301986</v>
+      </c>
+      <c r="AX3" s="50">
         <v>15.105455486877901</v>
       </c>
-      <c r="AT3" s="50">
+      <c r="AY3" s="50">
         <v>-2.7098456777153701</v>
       </c>
-      <c r="AU3" s="50">
+      <c r="AZ3" s="50">
         <v>17.815301164593201</v>
       </c>
-      <c r="AV3" s="50">
+      <c r="BA3" s="50">
         <v>6.19780490458127</v>
       </c>
-      <c r="AW3" s="50">
+      <c r="BB3" s="50">
         <v>24.009727067820499</v>
       </c>
-      <c r="AX3" s="50">
+      <c r="BC3" s="50">
         <v>47.054171086232202</v>
       </c>
-      <c r="AY3" s="44"/>
-      <c r="AZ3">
+      <c r="BD3" s="44"/>
+      <c r="BE3">
         <v>265</v>
       </c>
-      <c r="BA3">
+      <c r="BF3">
         <v>109</v>
       </c>
-      <c r="BB3">
-        <f>AZ3-BA3</f>
+      <c r="BG3">
+        <f>BE3-BF3</f>
         <v>156</v>
       </c>
-      <c r="BC3" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD3" s="78">
-        <f>BB3*concentration_constants!$B$6</f>
+      <c r="BH3" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI3" s="78">
+        <f>BG3*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE3" s="50">
+      <c r="BJ3" s="50">
         <f>I3*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3147589419488055</v>
       </c>
-      <c r="BF3" s="50">
-        <f>BE3*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK3" s="50">
+        <f>BJ3*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32759693848642901</v>
       </c>
-      <c r="BG3" s="50">
-        <f>BE3/BD3</f>
+      <c r="BL3" s="50">
+        <f>BJ3/BI3</f>
         <v>15.223991502817144</v>
       </c>
-      <c r="BH3" s="50">
-        <f>BF3/BD3</f>
+      <c r="BM3" s="50">
+        <f>BK3/BI3</f>
         <v>2.1545798646607448</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="17" thickBot="1">
+    <row r="4" spans="1:65" ht="17" thickBot="1">
       <c r="A4">
         <v>201205</v>
       </c>
@@ -4387,74 +4433,86 @@
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
         <v>2.09139498425152E-3</v>
       </c>
-      <c r="AO4" s="56">
+      <c r="AO4" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP4" s="57">
+      <c r="AQ4" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ4" s="47">
-        <f t="shared" ref="AQ4:AQ17" si="10">A4</f>
+      <c r="AR4" s="47">
+        <f t="shared" ref="AR4:AR17" si="10">A4</f>
         <v>201205</v>
       </c>
-      <c r="AR4" s="41" t="str">
-        <f t="shared" ref="AR4:AR17" si="11">D4</f>
+      <c r="AS4" s="41" t="str">
+        <f t="shared" ref="AS4:AS17" si="11">D4</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS4" s="50">
+      <c r="AT4" s="50">
+        <v>-2.8751161584865601</v>
+      </c>
+      <c r="AU4" s="50">
+        <v>5.8210338883950499</v>
+      </c>
+      <c r="AV4" s="50">
+        <v>11.311867280397299</v>
+      </c>
+      <c r="AX4" s="50">
         <v>6.8736240880515798</v>
       </c>
-      <c r="AT4" s="50">
+      <c r="AY4" s="50">
         <v>-13.881471917271901</v>
       </c>
-      <c r="AU4" s="50">
+      <c r="AZ4" s="50">
         <v>20.755096005323502</v>
       </c>
-      <c r="AV4" s="50">
+      <c r="BA4" s="50">
         <v>-3.5039239146101799</v>
       </c>
-      <c r="AW4" s="50">
+      <c r="BB4" s="50">
         <v>17.848649659933699</v>
       </c>
-      <c r="AX4" s="50">
+      <c r="BC4" s="50">
         <v>34.879852068524698</v>
       </c>
-      <c r="AY4" s="44"/>
-      <c r="AZ4">
+      <c r="BD4" s="44"/>
+      <c r="BE4">
         <v>265</v>
       </c>
-      <c r="BA4">
+      <c r="BF4">
         <v>109</v>
       </c>
-      <c r="BB4">
-        <f t="shared" ref="BB4:BB5" si="12">AZ4-BA4</f>
+      <c r="BG4">
+        <f t="shared" ref="BG4:BG5" si="12">BE4-BF4</f>
         <v>156</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BH4" t="s">
         <v>39</v>
       </c>
-      <c r="BD4" s="78">
-        <f>BB4*concentration_constants!$F$6</f>
+      <c r="BI4" s="78">
+        <f>BG4*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE4" s="50">
+      <c r="BJ4" s="50">
         <f>I4*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.0120000289208293</v>
       </c>
-      <c r="BF4" s="50">
-        <f>BE4*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK4" s="50">
+        <f>BJ4*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33318789796769971</v>
       </c>
-      <c r="BG4" s="50">
-        <f t="shared" ref="BG4:BG5" si="13">BE4/BD4</f>
+      <c r="BL4" s="50">
+        <f t="shared" ref="BL4:BL5" si="13">BJ4/BI4</f>
         <v>19.272938646594689</v>
       </c>
-      <c r="BH4" s="50">
-        <f t="shared" ref="BH4:BH5" si="14">BF4/BD4</f>
+      <c r="BM4" s="50">
+        <f t="shared" ref="BM4:BM5" si="14">BK4/BI4</f>
         <v>2.1319753830215245</v>
       </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:65">
       <c r="A5">
         <v>201205</v>
       </c>
@@ -4517,7 +4575,7 @@
         <v>0.42933650000000001</v>
       </c>
       <c r="W5" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
@@ -4566,74 +4624,86 @@
         <f t="shared" si="9"/>
         <v>2.1097889665454826E-3</v>
       </c>
-      <c r="AO5" s="56">
+      <c r="AO5" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP5" s="57">
+      <c r="AQ5" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ5" s="47">
+      <c r="AR5" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR5" s="41" t="str">
+      <c r="AS5" s="41" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_1</v>
       </c>
-      <c r="AS5" s="50">
+      <c r="AT5" s="50">
+        <v>0.99377060764127501</v>
+      </c>
+      <c r="AU5" s="50">
+        <v>10.4153664211945</v>
+      </c>
+      <c r="AV5" s="50">
+        <v>20.283394786421098</v>
+      </c>
+      <c r="AX5" s="50">
         <v>-0.53970856962448599</v>
       </c>
-      <c r="AT5" s="50">
+      <c r="AY5" s="50">
         <v>1.2825215740412901</v>
       </c>
-      <c r="AU5" s="50">
+      <c r="AZ5" s="50">
         <v>-1.82223014366578</v>
       </c>
-      <c r="AV5" s="50">
+      <c r="BA5" s="50">
         <v>0.37140650220840399</v>
       </c>
-      <c r="AW5" s="50">
+      <c r="BB5" s="50">
         <v>22.461390435589401</v>
       </c>
-      <c r="AX5" s="50">
+      <c r="BC5" s="50">
         <v>43.988167450184299</v>
       </c>
-      <c r="AY5" s="44"/>
-      <c r="AZ5">
+      <c r="BD5" s="44"/>
+      <c r="BE5">
         <v>265</v>
       </c>
-      <c r="BA5">
+      <c r="BF5">
         <v>109</v>
       </c>
-      <c r="BB5">
+      <c r="BG5">
         <f t="shared" si="12"/>
         <v>156</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BH5" t="s">
         <v>39</v>
       </c>
-      <c r="BD5" s="78">
-        <f>BB5*concentration_constants!$F$6</f>
+      <c r="BI5" s="78">
+        <f>BG5*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE5" s="50">
+      <c r="BJ5" s="50">
         <f>I5*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.9048847269174694</v>
       </c>
-      <c r="BF5" s="50">
-        <f>BE5*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK5" s="50">
+        <f>BJ5*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38845979713665457</v>
       </c>
-      <c r="BG5" s="50">
+      <c r="BL5" s="50">
         <f t="shared" si="13"/>
         <v>63.378563682109089</v>
       </c>
-      <c r="BH5" s="50">
+      <c r="BM5" s="50">
         <f t="shared" si="14"/>
         <v>2.4856446762936448</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:65">
       <c r="A6">
         <v>201205</v>
       </c>
@@ -4749,74 +4819,86 @@
         <f t="shared" si="9"/>
         <v>2.1164798861162187E-3</v>
       </c>
-      <c r="AO6" s="56">
+      <c r="AO6" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP6" s="57">
+      <c r="AQ6" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ6" s="47">
+      <c r="AR6" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR6" t="str">
+      <c r="AS6" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS6" s="50">
+      <c r="AT6" s="50">
+        <v>7.6188552572193897</v>
+      </c>
+      <c r="AU6" s="50">
+        <v>12.047032369804301</v>
+      </c>
+      <c r="AV6" s="50">
+        <v>23.478838724644199</v>
+      </c>
+      <c r="AX6" s="50">
         <v>14.851574153242799</v>
       </c>
-      <c r="AT6" s="50">
+      <c r="AY6" s="50">
         <v>-0.85838254078074405</v>
       </c>
-      <c r="AU6" s="50">
+      <c r="AZ6" s="50">
         <v>15.7099566940236</v>
       </c>
-      <c r="AV6" s="50">
+      <c r="BA6" s="50">
         <v>6.9965958062310696</v>
       </c>
-      <c r="AW6" s="50">
+      <c r="BB6" s="50">
         <v>24.095420378555701</v>
       </c>
-      <c r="AX6" s="50">
+      <c r="BC6" s="50">
         <v>47.223987370547697</v>
       </c>
-      <c r="AY6" s="44"/>
-      <c r="AZ6">
+      <c r="BD6" s="44"/>
+      <c r="BE6">
         <v>265</v>
       </c>
-      <c r="BA6">
+      <c r="BF6">
         <v>109</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB17" si="15">AZ6-BA6</f>
+      <c r="BG6">
+        <f t="shared" ref="BG6:BG17" si="15">BE6-BF6</f>
         <v>156</v>
       </c>
-      <c r="BC6" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD6" s="78">
-        <f>BB6*concentration_constants!$B$6</f>
+      <c r="BH6" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI6" s="78">
+        <f>BG6*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE6" s="50">
+      <c r="BJ6" s="50">
         <f>I6*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4178655483113793</v>
       </c>
-      <c r="BF6" s="50">
-        <f>BE6*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK6" s="50">
+        <f>BJ6*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32842371830361955</v>
       </c>
-      <c r="BG6" s="50">
-        <f t="shared" ref="BG6:BG17" si="16">BE6/BD6</f>
+      <c r="BL6" s="50">
+        <f t="shared" ref="BL6:BL17" si="16">BJ6/BI6</f>
         <v>15.90211572158638</v>
       </c>
-      <c r="BH6" s="50">
-        <f t="shared" ref="BH6:BH17" si="17">BF6/BD6</f>
+      <c r="BM6" s="50">
+        <f t="shared" ref="BM6:BM17" si="17">BK6/BI6</f>
         <v>2.1600175319199595</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="17" thickBot="1">
+    <row r="7" spans="1:65" ht="17" thickBot="1">
       <c r="A7">
         <v>201205</v>
       </c>
@@ -4932,74 +5014,86 @@
         <f t="shared" si="9"/>
         <v>2.0917613635465034E-3</v>
       </c>
-      <c r="AO7" s="56">
+      <c r="AO7" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP7" s="57">
+      <c r="AQ7" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ7" s="47">
+      <c r="AR7" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR7" t="str">
+      <c r="AS7" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS7" s="50">
+      <c r="AT7" s="50">
+        <v>-2.9437994939993599</v>
+      </c>
+      <c r="AU7" s="50">
+        <v>5.91354798399224</v>
+      </c>
+      <c r="AV7" s="50">
+        <v>11.492144698644401</v>
+      </c>
+      <c r="AX7" s="50">
         <v>6.6566362138331598</v>
       </c>
-      <c r="AT7" s="50">
+      <c r="AY7" s="50">
         <v>-13.8026489120794</v>
       </c>
-      <c r="AU7" s="50">
+      <c r="AZ7" s="50">
         <v>20.459285125912601</v>
       </c>
-      <c r="AV7" s="50">
+      <c r="BA7" s="50">
         <v>-3.5730063491231601</v>
       </c>
-      <c r="AW7" s="50">
+      <c r="BB7" s="50">
         <v>17.941820061995799</v>
       </c>
-      <c r="AX7" s="50">
+      <c r="BC7" s="50">
         <v>35.063444020270097</v>
       </c>
-      <c r="AY7" s="44"/>
-      <c r="AZ7">
+      <c r="BD7" s="44"/>
+      <c r="BE7">
         <v>265</v>
       </c>
-      <c r="BA7">
+      <c r="BF7">
         <v>109</v>
       </c>
-      <c r="BB7">
+      <c r="BG7">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BH7" t="s">
         <v>39</v>
       </c>
-      <c r="BD7" s="78">
-        <f>BB7*concentration_constants!$F$6</f>
+      <c r="BI7" s="78">
+        <f>BG7*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE7" s="50">
+      <c r="BJ7" s="50">
         <f>I7*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>17.089981869851989</v>
       </c>
-      <c r="BF7" s="50">
-        <f>BE7*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK7" s="50">
+        <f>BJ7*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.44607485704311811</v>
       </c>
-      <c r="BG7" s="50">
+      <c r="BL7" s="50">
         <f t="shared" si="16"/>
         <v>109.35397373388625</v>
       </c>
-      <c r="BH7" s="50">
+      <c r="BM7" s="50">
         <f t="shared" si="17"/>
         <v>2.8543071942335927</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="17" thickBot="1">
+    <row r="8" spans="1:65" ht="17" thickBot="1">
       <c r="A8">
         <v>201205</v>
       </c>
@@ -5106,74 +5200,86 @@
         <f t="shared" si="9"/>
         <v>2.1059970799231576E-3</v>
       </c>
-      <c r="AO8" s="56">
+      <c r="AO8" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP8" s="57">
+      <c r="AQ8" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ8" s="47">
+      <c r="AR8" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR8" t="str">
+      <c r="AS8" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_2</v>
       </c>
-      <c r="AS8" s="50">
+      <c r="AT8" s="50">
+        <v>-0.30811082163339998</v>
+      </c>
+      <c r="AU8" s="50">
+        <v>9.4723024409240004</v>
+      </c>
+      <c r="AV8" s="50">
+        <v>18.438709928632498</v>
+      </c>
+      <c r="AX8" s="50">
         <v>-1.15628904358433</v>
       </c>
-      <c r="AT8" s="50">
+      <c r="AY8" s="50">
         <v>-0.70441124849329695</v>
       </c>
-      <c r="AU8" s="50">
+      <c r="AZ8" s="50">
         <v>-0.45187779509103798</v>
       </c>
-      <c r="AV8" s="50">
+      <c r="BA8" s="50">
         <v>-0.93035014603881605</v>
       </c>
-      <c r="AW8" s="50">
+      <c r="BB8" s="50">
         <v>21.5157968077277</v>
       </c>
-      <c r="AX8" s="50">
+      <c r="BC8" s="50">
         <v>42.117851051899301</v>
       </c>
-      <c r="AY8" s="44"/>
-      <c r="AZ8">
+      <c r="BD8" s="44"/>
+      <c r="BE8">
         <v>265</v>
       </c>
-      <c r="BA8">
+      <c r="BF8">
         <v>109</v>
       </c>
-      <c r="BB8">
+      <c r="BG8">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BH8" t="s">
         <v>39</v>
       </c>
-      <c r="BD8" s="78">
-        <f>BB8*concentration_constants!$F$6</f>
+      <c r="BI8" s="78">
+        <f>BG8*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE8" s="50">
+      <c r="BJ8" s="50">
         <f>I8*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.8350681459275666</v>
       </c>
-      <c r="BF8" s="50">
-        <f>BE8*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK8" s="50">
+        <f>BJ8*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.387899959681965</v>
       </c>
-      <c r="BG8" s="50">
+      <c r="BL8" s="50">
         <f t="shared" si="16"/>
         <v>62.931827072210872</v>
       </c>
-      <c r="BH8" s="50">
+      <c r="BM8" s="50">
         <f t="shared" si="17"/>
         <v>2.4820624343239581</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:65">
       <c r="A9">
         <v>201205</v>
       </c>
@@ -5236,7 +5342,7 @@
         <v>0.42850050000000001</v>
       </c>
       <c r="X9" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y9" s="3"/>
       <c r="AA9" s="28">
@@ -5283,73 +5389,85 @@
         <f t="shared" si="9"/>
         <v>2.1125489546459449E-3</v>
       </c>
-      <c r="AO9" s="56">
+      <c r="AO9" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP9" s="57">
+      <c r="AQ9" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ9" s="47">
+      <c r="AR9" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR9" s="41" t="str">
+      <c r="AS9" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS9" s="50">
+      <c r="AT9" s="50">
+        <v>6.2077712220716101</v>
+      </c>
+      <c r="AU9" s="50">
+        <v>11.069837232340699</v>
+      </c>
+      <c r="AV9" s="50">
+        <v>21.5645252666334</v>
+      </c>
+      <c r="AX9" s="50">
         <v>16.036656468840999</v>
       </c>
-      <c r="AT9" s="50">
+      <c r="AY9" s="50">
         <v>-4.8656873390863202</v>
       </c>
-      <c r="AU9" s="50">
+      <c r="AZ9" s="50">
         <v>20.902343807927299</v>
       </c>
-      <c r="AV9" s="50">
+      <c r="BA9" s="50">
         <v>5.5854845648773397</v>
       </c>
-      <c r="AW9" s="50">
+      <c r="BB9" s="50">
         <v>23.117269398744899</v>
       </c>
-      <c r="AX9" s="50">
+      <c r="BC9" s="50">
         <v>45.286402388126902</v>
       </c>
-      <c r="AZ9">
+      <c r="BE9">
         <v>265</v>
       </c>
-      <c r="BA9">
+      <c r="BF9">
         <v>109</v>
       </c>
-      <c r="BB9">
+      <c r="BG9">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC9" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD9" s="78">
-        <f>BB9*concentration_constants!$B$6</f>
+      <c r="BH9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI9" s="78">
+        <f>BG9*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE9" s="50">
+      <c r="BJ9" s="50">
         <f>I9*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4132419336762863</v>
       </c>
-      <c r="BF9" s="50">
-        <f>BE9*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK9" s="50">
+        <f>BJ9*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32838664297549441</v>
       </c>
-      <c r="BG9" s="50">
+      <c r="BL9" s="50">
         <f t="shared" si="16"/>
         <v>15.871706563794037</v>
       </c>
-      <c r="BH9" s="50">
+      <c r="BM9" s="50">
         <f t="shared" si="17"/>
         <v>2.1597736903388287</v>
       </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:65">
       <c r="A10">
         <v>201205</v>
       </c>
@@ -5457,73 +5575,85 @@
         <f t="shared" si="9"/>
         <v>2.1110245425008428E-3</v>
       </c>
-      <c r="AO10" s="56">
+      <c r="AO10" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP10" s="57">
+      <c r="AQ10" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ10" s="47">
+      <c r="AR10" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR10" t="str">
+      <c r="AS10" t="str">
         <f t="shared" si="11"/>
         <v>DI</v>
       </c>
-      <c r="AS10" s="50">
+      <c r="AT10" s="50">
+        <v>-9.4703270270268796</v>
+      </c>
+      <c r="AU10" s="50">
+        <v>10.789277677641399</v>
+      </c>
+      <c r="AV10" s="50">
+        <v>21.0152329961257</v>
+      </c>
+      <c r="AX10" s="50">
         <v>14.4579715364672</v>
       </c>
-      <c r="AT10" s="50">
+      <c r="AY10" s="50">
         <v>-34.815304667159701</v>
       </c>
-      <c r="AU10" s="50">
+      <c r="AZ10" s="50">
         <v>49.273276203626899</v>
       </c>
-      <c r="AV10" s="50">
+      <c r="BA10" s="50">
         <v>-10.1786665653462</v>
       </c>
-      <c r="AW10" s="50">
+      <c r="BB10" s="50">
         <v>22.853627356464699</v>
       </c>
-      <c r="AX10" s="50">
+      <c r="BC10" s="50">
         <v>44.764460247631298</v>
       </c>
-      <c r="AZ10">
+      <c r="BE10">
         <v>265</v>
       </c>
-      <c r="BA10">
+      <c r="BF10">
         <v>109</v>
       </c>
-      <c r="BB10">
+      <c r="BG10">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC10" t="s">
+      <c r="BH10" t="s">
         <v>39</v>
       </c>
-      <c r="BD10" s="78">
-        <f>BB10*concentration_constants!$F$6</f>
+      <c r="BI10" s="78">
+        <f>BG10*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE10" s="50">
+      <c r="BJ10" s="50">
         <f>I10*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>7.9745256167661447</v>
       </c>
-      <c r="BF10" s="50">
-        <f>BE10*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK10" s="50">
+        <f>BJ10*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3729808476444097</v>
       </c>
-      <c r="BG10" s="50">
+      <c r="BL10" s="50">
         <f t="shared" si="16"/>
         <v>51.026740196512598</v>
       </c>
-      <c r="BH10" s="50">
+      <c r="BM10" s="50">
         <f t="shared" si="17"/>
         <v>2.386599244350319</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="17" thickBot="1">
+    <row r="11" spans="1:65" ht="17" thickBot="1">
       <c r="A11">
         <v>201207</v>
       </c>
@@ -5637,73 +5767,85 @@
         <f t="shared" si="9"/>
         <v>2.11205838421125E-3</v>
       </c>
-      <c r="AO11" s="56">
+      <c r="AO11" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP11" s="57">
+      <c r="AQ11" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ11" s="47">
+      <c r="AR11" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR11" s="41" t="str">
+      <c r="AS11" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS11" s="50">
+      <c r="AT11" s="50">
+        <v>6.9108857559516599</v>
+      </c>
+      <c r="AU11" s="50">
+        <v>10.9413033548062</v>
+      </c>
+      <c r="AV11" s="50">
+        <v>21.312858040510601</v>
+      </c>
+      <c r="AX11" s="50">
         <v>17.1518234709566</v>
       </c>
-      <c r="AT11" s="50">
+      <c r="AY11" s="50">
         <v>-4.5745335204508901</v>
       </c>
-      <c r="AU11" s="50">
+      <c r="AZ11" s="50">
         <v>21.726356991407499</v>
       </c>
-      <c r="AV11" s="50">
+      <c r="BA11" s="50">
         <v>6.2886449752528799</v>
       </c>
-      <c r="AW11" s="50">
+      <c r="BB11" s="50">
         <v>22.988533215933799</v>
       </c>
-      <c r="AX11" s="50">
+      <c r="BC11" s="50">
         <v>45.031522726332703</v>
       </c>
-      <c r="AZ11">
+      <c r="BE11">
         <v>265</v>
       </c>
-      <c r="BA11">
+      <c r="BF11">
         <v>109</v>
       </c>
-      <c r="BB11">
+      <c r="BG11">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC11" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD11" s="78">
-        <f>BB11*concentration_constants!$B$6</f>
+      <c r="BH11" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI11" s="78">
+        <f>BG11*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE11" s="50">
+      <c r="BJ11" s="50">
         <f>I11*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2611250121817261</v>
       </c>
-      <c r="BF11" s="50">
-        <f>BE11*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK11" s="50">
+        <f>BJ11*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32716686468017736</v>
       </c>
-      <c r="BG11" s="50">
+      <c r="BL11" s="50">
         <f t="shared" si="16"/>
         <v>14.871245272425968</v>
       </c>
-      <c r="BH11" s="50">
+      <c r="BM11" s="50">
         <f t="shared" si="17"/>
         <v>2.151751302319628</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:65">
       <c r="A12">
         <v>201207</v>
       </c>
@@ -5809,73 +5951,85 @@
         <f t="shared" si="9"/>
         <v>2.0890378267892978E-3</v>
       </c>
-      <c r="AO12" s="56">
+      <c r="AO12" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP12" s="57">
+      <c r="AQ12" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ12" s="47">
+      <c r="AR12" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR12" s="41" t="str">
+      <c r="AS12" s="41" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS12" s="50">
+      <c r="AT12" s="50">
+        <v>-3.1523293237588601</v>
+      </c>
+      <c r="AU12" s="50">
+        <v>5.2305070201659198</v>
+      </c>
+      <c r="AV12" s="50">
+        <v>10.1615046903504</v>
+      </c>
+      <c r="AX12" s="50">
         <v>7.0098620813652204</v>
       </c>
-      <c r="AT12" s="50">
+      <c r="AY12" s="50">
         <v>-14.5751415214816</v>
       </c>
-      <c r="AU12" s="50">
+      <c r="AZ12" s="50">
         <v>21.5850036028468</v>
       </c>
-      <c r="AV12" s="50">
+      <c r="BA12" s="50">
         <v>-3.78263972005821</v>
       </c>
-      <c r="AW12" s="50">
+      <c r="BB12" s="50">
         <v>17.254451999306699</v>
       </c>
-      <c r="AX12" s="50">
+      <c r="BC12" s="50">
         <v>33.709358475152598</v>
       </c>
-      <c r="AZ12">
+      <c r="BE12">
         <v>265</v>
       </c>
-      <c r="BA12">
+      <c r="BF12">
         <v>109</v>
       </c>
-      <c r="BB12">
+      <c r="BG12">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC12" t="s">
+      <c r="BH12" t="s">
         <v>39</v>
       </c>
-      <c r="BD12" s="78">
-        <f>BB12*concentration_constants!$F$6</f>
+      <c r="BI12" s="78">
+        <f>BG12*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE12" s="50">
+      <c r="BJ12" s="50">
         <f>I12*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.6625426080784145</v>
       </c>
-      <c r="BF12" s="50">
-        <f>BE12*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK12" s="50">
+        <f>BJ12*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33840439663490651</v>
       </c>
-      <c r="BG12" s="50">
+      <c r="BL12" s="50">
         <f t="shared" si="16"/>
         <v>23.435577124255598</v>
       </c>
-      <c r="BH12" s="50">
+      <c r="BM12" s="50">
         <f t="shared" si="17"/>
         <v>2.1653542866728439</v>
       </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:65">
       <c r="A13">
         <v>201207</v>
       </c>
@@ -5981,73 +6135,85 @@
         <f t="shared" si="9"/>
         <v>2.1092446228371492E-3</v>
       </c>
-      <c r="AO13" s="56">
+      <c r="AO13" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP13" s="57">
+      <c r="AQ13" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ13" s="47">
+      <c r="AR13" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR13" s="41" t="str">
+      <c r="AS13" s="41" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_1</v>
       </c>
-      <c r="AS13" s="50">
+      <c r="AT13" s="50">
+        <v>0.77398247028148603</v>
+      </c>
+      <c r="AU13" s="50">
+        <v>10.280231459846</v>
+      </c>
+      <c r="AV13" s="50">
+        <v>20.018964220354299</v>
+      </c>
+      <c r="AX13" s="50">
         <v>8.2241945278393999E-2</v>
       </c>
-      <c r="AT13" s="50">
+      <c r="AY13" s="50">
         <v>0.22102332359041901</v>
       </c>
-      <c r="AU13" s="50">
+      <c r="AZ13" s="50">
         <v>-0.138781378312025</v>
       </c>
-      <c r="AV13" s="50">
+      <c r="BA13" s="50">
         <v>0.151632634434406</v>
       </c>
-      <c r="AW13" s="50">
+      <c r="BB13" s="50">
         <v>22.3259423648012</v>
       </c>
-      <c r="AX13" s="50">
+      <c r="BC13" s="50">
         <v>43.720161276728597</v>
       </c>
-      <c r="AZ13">
+      <c r="BE13">
         <v>265</v>
       </c>
-      <c r="BA13">
+      <c r="BF13">
         <v>109</v>
       </c>
-      <c r="BB13">
+      <c r="BG13">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC13" t="s">
+      <c r="BH13" t="s">
         <v>39</v>
       </c>
-      <c r="BD13" s="78">
-        <f>BB13*concentration_constants!$F$6</f>
+      <c r="BI13" s="78">
+        <f>BG13*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE13" s="50">
+      <c r="BJ13" s="50">
         <f>I13*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.6085110288080102</v>
       </c>
-      <c r="BF13" s="50">
-        <f>BE13*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK13" s="50">
+        <f>BJ13*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38608326860383324</v>
       </c>
-      <c r="BG13" s="50">
+      <c r="BL13" s="50">
         <f t="shared" si="16"/>
         <v>61.482151980488176</v>
       </c>
-      <c r="BH13" s="50">
+      <c r="BM13" s="50">
         <f t="shared" si="17"/>
         <v>2.4704379405150405</v>
       </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:65">
       <c r="A14">
         <v>201207</v>
       </c>
@@ -6153,73 +6319,85 @@
         <f t="shared" si="9"/>
         <v>2.1118562233900973E-3</v>
       </c>
-      <c r="AO14" s="56">
+      <c r="AO14" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP14" s="57">
+      <c r="AQ14" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ14" s="47">
+      <c r="AR14" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR14" s="41" t="str">
+      <c r="AS14" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS14" s="50">
+      <c r="AT14" s="50">
+        <v>5.9787063469953701</v>
+      </c>
+      <c r="AU14" s="50">
+        <v>10.8974837047792</v>
+      </c>
+      <c r="AV14" s="50">
+        <v>21.227066743560101</v>
+      </c>
+      <c r="AX14" s="50">
         <v>14.393773542834699</v>
       </c>
-      <c r="AT14" s="50">
+      <c r="AY14" s="50">
         <v>-3.6809189289388402</v>
       </c>
-      <c r="AU14" s="50">
+      <c r="AZ14" s="50">
         <v>18.074692471773599</v>
       </c>
-      <c r="AV14" s="50">
+      <c r="BA14" s="50">
         <v>5.3564273069479604</v>
       </c>
-      <c r="AW14" s="50">
+      <c r="BB14" s="50">
         <v>22.94455532836</v>
       </c>
-      <c r="AX14" s="50">
+      <c r="BC14" s="50">
         <v>44.944459545090702</v>
       </c>
-      <c r="AZ14">
+      <c r="BE14">
         <v>265</v>
       </c>
-      <c r="BA14">
+      <c r="BF14">
         <v>109</v>
       </c>
-      <c r="BB14">
+      <c r="BG14">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC14" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD14" s="78">
-        <f>BB14*concentration_constants!$B$6</f>
+      <c r="BH14" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI14" s="78">
+        <f>BG14*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE14" s="50">
+      <c r="BJ14" s="50">
         <f>I14*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3526725819565679</v>
       </c>
-      <c r="BF14" s="50">
-        <f>BE14*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK14" s="50">
+        <f>BJ14*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32790095617705511</v>
       </c>
-      <c r="BG14" s="50">
+      <c r="BL14" s="50">
         <f t="shared" si="16"/>
         <v>15.473346596714352</v>
       </c>
-      <c r="BH14" s="50">
+      <c r="BM14" s="50">
         <f t="shared" si="17"/>
         <v>2.1565793656260164</v>
       </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:65">
       <c r="A15">
         <v>201207</v>
       </c>
@@ -6325,73 +6503,85 @@
         <f t="shared" si="9"/>
         <v>2.1140383039962136E-3</v>
       </c>
-      <c r="AO15" s="56">
+      <c r="AO15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP15" s="57">
+      <c r="AQ15" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ15" s="47">
+      <c r="AR15" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR15" t="str">
+      <c r="AS15" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_3</v>
       </c>
-      <c r="AS15" s="50">
+      <c r="AT15" s="50">
+        <v>6.7953928308284102</v>
+      </c>
+      <c r="AU15" s="50">
+        <v>11.4396795190323</v>
+      </c>
+      <c r="AV15" s="50">
+        <v>22.288837817687501</v>
+      </c>
+      <c r="AX15" s="50">
         <v>16.679833428360201</v>
       </c>
-      <c r="AT15" s="50">
+      <c r="AY15" s="50">
         <v>-4.3336183513273898</v>
       </c>
-      <c r="AU15" s="50">
+      <c r="AZ15" s="50">
         <v>21.0134517796876</v>
       </c>
-      <c r="AV15" s="50">
+      <c r="BA15" s="50">
         <v>6.1731075385164003</v>
       </c>
-      <c r="AW15" s="50">
+      <c r="BB15" s="50">
         <v>23.487665779901398</v>
       </c>
-      <c r="AX15" s="50">
+      <c r="BC15" s="50">
         <v>46.019903286484897</v>
       </c>
-      <c r="AZ15">
+      <c r="BE15">
         <v>265</v>
       </c>
-      <c r="BA15">
+      <c r="BF15">
         <v>109</v>
       </c>
-      <c r="BB15">
+      <c r="BG15">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC15" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD15" s="78">
-        <f>BB15*concentration_constants!$B$6</f>
+      <c r="BH15" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI15" s="78">
+        <f>BG15*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE15" s="50">
+      <c r="BJ15" s="50">
         <f>I15*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2375445775427525</v>
       </c>
-      <c r="BF15" s="50">
-        <f>BE15*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK15" s="50">
+        <f>BJ15*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3269777805067392</v>
       </c>
-      <c r="BG15" s="50">
+      <c r="BL15" s="50">
         <f t="shared" si="16"/>
         <v>14.716158567685026</v>
       </c>
-      <c r="BH15" s="50">
+      <c r="BM15" s="50">
         <f t="shared" si="17"/>
         <v>2.1505077102558618</v>
       </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:65">
       <c r="A16">
         <v>201207</v>
       </c>
@@ -6497,73 +6687,85 @@
         <f t="shared" si="9"/>
         <v>2.0909357320700551E-3</v>
       </c>
-      <c r="AO16" s="56">
+      <c r="AO16" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP16" s="57">
+      <c r="AQ16" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ16" s="47">
+      <c r="AR16" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR16" t="str">
+      <c r="AS16" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS16" s="50">
+      <c r="AT16" s="50">
+        <v>-3.26393620207998</v>
+      </c>
+      <c r="AU16" s="50">
+        <v>5.7081423934837101</v>
+      </c>
+      <c r="AV16" s="50">
+        <v>11.091902549817901</v>
+      </c>
+      <c r="AX16" s="50">
         <v>7.1029978910310803</v>
       </c>
-      <c r="AT16" s="50">
+      <c r="AY16" s="50">
         <v>-14.893050092214599</v>
       </c>
-      <c r="AU16" s="50">
+      <c r="AZ16" s="50">
         <v>21.996047983245699</v>
       </c>
-      <c r="AV16" s="50">
+      <c r="BA16" s="50">
         <v>-3.8950261005917799</v>
       </c>
-      <c r="AW16" s="50">
+      <c r="BB16" s="50">
         <v>17.735485742880101</v>
       </c>
-      <c r="AX16" s="50">
+      <c r="BC16" s="50">
         <v>34.656884164523802</v>
       </c>
-      <c r="AZ16">
+      <c r="BE16">
         <v>265</v>
       </c>
-      <c r="BA16">
+      <c r="BF16">
         <v>109</v>
       </c>
-      <c r="BB16">
+      <c r="BG16">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC16" t="s">
+      <c r="BH16" t="s">
         <v>39</v>
       </c>
-      <c r="BD16" s="78">
-        <f>BB16*concentration_constants!$F$6</f>
+      <c r="BI16" s="78">
+        <f>BG16*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE16" s="50">
+      <c r="BJ16" s="50">
         <f>I16*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.9394971247204844</v>
       </c>
-      <c r="BF16" s="50">
-        <f>BE16*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK16" s="50">
+        <f>BJ16*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.34062520878960229</v>
       </c>
-      <c r="BG16" s="50">
+      <c r="BL16" s="50">
         <f t="shared" si="16"/>
         <v>25.207730960871714</v>
       </c>
-      <c r="BH16" s="50">
+      <c r="BM16" s="50">
         <f t="shared" si="17"/>
         <v>2.179564637267827</v>
       </c>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:65">
       <c r="A17">
         <v>201207</v>
       </c>
@@ -6665,73 +6867,85 @@
         <f t="shared" si="9"/>
         <v>2.1099653819650526E-3</v>
       </c>
-      <c r="AO17" s="56">
+      <c r="AO17" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP17" s="57">
+      <c r="AQ17" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ17" s="47">
+      <c r="AR17" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR17" s="41" t="str">
+      <c r="AS17" s="41" t="str">
         <f t="shared" si="11"/>
         <v>DI</v>
       </c>
-      <c r="AS17" s="50">
+      <c r="AT17" s="50">
+        <v>-6.6415725392230396</v>
+      </c>
+      <c r="AU17" s="50">
+        <v>10.5097585385409</v>
+      </c>
+      <c r="AV17" s="50">
+        <v>20.468119894696301</v>
+      </c>
+      <c r="AX17" s="50">
         <v>13.725240315331099</v>
       </c>
-      <c r="AT17" s="50">
+      <c r="AY17" s="50">
         <v>-28.3353648321477</v>
       </c>
-      <c r="AU17" s="50">
+      <c r="AZ17" s="50">
         <v>42.060605147478803</v>
       </c>
-      <c r="AV17" s="50">
+      <c r="BA17" s="50">
         <v>-7.3050622584082596</v>
       </c>
-      <c r="AW17" s="50">
+      <c r="BB17" s="50">
         <v>22.565126816266901</v>
       </c>
-      <c r="AX17" s="50">
+      <c r="BC17" s="50">
         <v>44.193449376003002</v>
       </c>
-      <c r="AZ17">
+      <c r="BE17">
         <v>265</v>
       </c>
-      <c r="BA17">
+      <c r="BF17">
         <v>109</v>
       </c>
-      <c r="BB17">
+      <c r="BG17">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC17" t="s">
+      <c r="BH17" t="s">
         <v>39</v>
       </c>
-      <c r="BD17" s="78">
-        <f>BB17*concentration_constants!$F$6</f>
+      <c r="BI17" s="78">
+        <f>BG17*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE17" s="50">
+      <c r="BJ17" s="50">
         <f>I17*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>6.3978730261994317</v>
       </c>
-      <c r="BF17" s="50">
-        <f>BE17*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK17" s="50">
+        <f>BJ17*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.36033816075373781</v>
       </c>
-      <c r="BG17" s="50">
+      <c r="BL17" s="50">
         <f t="shared" si="16"/>
         <v>40.938184966360723</v>
       </c>
-      <c r="BH17" s="50">
+      <c r="BM17" s="50">
         <f t="shared" si="17"/>
         <v>2.3057022568229555</v>
       </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:65">
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -6761,18 +6975,19 @@
       <c r="AL18" s="33"/>
       <c r="AM18" s="33"/>
       <c r="AN18" s="33"/>
-      <c r="AO18" s="56"/>
-      <c r="AP18" s="54"/>
-      <c r="AQ18" s="49"/>
-      <c r="AR18" s="48"/>
+      <c r="AO18" s="33"/>
+      <c r="AP18" s="56"/>
+      <c r="AQ18" s="54"/>
+      <c r="AR18" s="49"/>
       <c r="AS18" s="48"/>
-      <c r="AT18" s="48"/>
-      <c r="AU18" s="48"/>
-      <c r="AV18" s="48"/>
-      <c r="AW18" s="48"/>
       <c r="AX18" s="48"/>
-    </row>
-    <row r="19" spans="1:60">
+      <c r="AY18" s="48"/>
+      <c r="AZ18" s="48"/>
+      <c r="BA18" s="48"/>
+      <c r="BB18" s="48"/>
+      <c r="BC18" s="48"/>
+    </row>
+    <row r="19" spans="1:65">
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -6802,18 +7017,19 @@
       <c r="AL19" s="33"/>
       <c r="AM19" s="33"/>
       <c r="AN19" s="33"/>
-      <c r="AO19" s="56"/>
-      <c r="AP19" s="54"/>
-      <c r="AQ19" s="49"/>
-      <c r="AR19" s="48"/>
+      <c r="AO19" s="33"/>
+      <c r="AP19" s="56"/>
+      <c r="AQ19" s="54"/>
+      <c r="AR19" s="49"/>
       <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="48"/>
-      <c r="AV19" s="48"/>
-      <c r="AW19" s="48"/>
       <c r="AX19" s="48"/>
-    </row>
-    <row r="20" spans="1:60">
+      <c r="AY19" s="48"/>
+      <c r="AZ19" s="48"/>
+      <c r="BA19" s="48"/>
+      <c r="BB19" s="48"/>
+      <c r="BC19" s="48"/>
+    </row>
+    <row r="20" spans="1:65">
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -6843,18 +7059,19 @@
       <c r="AL20" s="33"/>
       <c r="AM20" s="33"/>
       <c r="AN20" s="33"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="54"/>
-      <c r="AQ20" s="49"/>
-      <c r="AR20" s="48"/>
+      <c r="AO20" s="33"/>
+      <c r="AP20" s="56"/>
+      <c r="AQ20" s="54"/>
+      <c r="AR20" s="49"/>
       <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
-      <c r="AV20" s="48"/>
-      <c r="AW20" s="48"/>
       <c r="AX20" s="48"/>
-    </row>
-    <row r="21" spans="1:60">
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+      <c r="BA20" s="48"/>
+      <c r="BB20" s="48"/>
+      <c r="BC20" s="48"/>
+    </row>
+    <row r="21" spans="1:65">
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -6884,18 +7101,19 @@
       <c r="AL21" s="33"/>
       <c r="AM21" s="33"/>
       <c r="AN21" s="33"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="54"/>
-      <c r="AQ21" s="49"/>
-      <c r="AR21" s="48"/>
+      <c r="AO21" s="33"/>
+      <c r="AP21" s="56"/>
+      <c r="AQ21" s="54"/>
+      <c r="AR21" s="49"/>
       <c r="AS21" s="48"/>
-      <c r="AT21" s="48"/>
-      <c r="AU21" s="48"/>
-      <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
       <c r="AX21" s="48"/>
-    </row>
-    <row r="22" spans="1:60">
+      <c r="AY21" s="48"/>
+      <c r="AZ21" s="48"/>
+      <c r="BA21" s="48"/>
+      <c r="BB21" s="48"/>
+      <c r="BC21" s="48"/>
+    </row>
+    <row r="22" spans="1:65">
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -6925,18 +7143,19 @@
       <c r="AL22" s="33"/>
       <c r="AM22" s="33"/>
       <c r="AN22" s="33"/>
-      <c r="AO22" s="56"/>
-      <c r="AP22" s="54"/>
-      <c r="AQ22" s="49"/>
-      <c r="AR22" s="48"/>
+      <c r="AO22" s="33"/>
+      <c r="AP22" s="56"/>
+      <c r="AQ22" s="54"/>
+      <c r="AR22" s="49"/>
       <c r="AS22" s="48"/>
-      <c r="AT22" s="48"/>
-      <c r="AU22" s="48"/>
-      <c r="AV22" s="48"/>
-      <c r="AW22" s="48"/>
       <c r="AX22" s="48"/>
-    </row>
-    <row r="23" spans="1:60">
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="48"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+    </row>
+    <row r="23" spans="1:65">
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -6966,18 +7185,19 @@
       <c r="AL23" s="33"/>
       <c r="AM23" s="33"/>
       <c r="AN23" s="33"/>
-      <c r="AO23" s="56"/>
-      <c r="AP23" s="54"/>
-      <c r="AQ23" s="49"/>
-      <c r="AR23" s="48"/>
+      <c r="AO23" s="33"/>
+      <c r="AP23" s="56"/>
+      <c r="AQ23" s="54"/>
+      <c r="AR23" s="49"/>
       <c r="AS23" s="48"/>
-      <c r="AT23" s="48"/>
-      <c r="AU23" s="48"/>
-      <c r="AV23" s="48"/>
-      <c r="AW23" s="48"/>
       <c r="AX23" s="48"/>
-    </row>
-    <row r="24" spans="1:60">
+      <c r="AY23" s="48"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48"/>
+      <c r="BC23" s="48"/>
+    </row>
+    <row r="24" spans="1:65">
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -7007,18 +7227,19 @@
       <c r="AL24" s="33"/>
       <c r="AM24" s="33"/>
       <c r="AN24" s="33"/>
-      <c r="AO24" s="56"/>
-      <c r="AP24" s="54"/>
-      <c r="AQ24" s="49"/>
-      <c r="AR24" s="48"/>
+      <c r="AO24" s="33"/>
+      <c r="AP24" s="56"/>
+      <c r="AQ24" s="54"/>
+      <c r="AR24" s="49"/>
       <c r="AS24" s="48"/>
-      <c r="AT24" s="48"/>
-      <c r="AU24" s="48"/>
-      <c r="AV24" s="48"/>
-      <c r="AW24" s="48"/>
       <c r="AX24" s="48"/>
-    </row>
-    <row r="25" spans="1:60">
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="48"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="48"/>
+      <c r="BC24" s="48"/>
+    </row>
+    <row r="25" spans="1:65">
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
@@ -7048,18 +7269,19 @@
       <c r="AL25" s="33"/>
       <c r="AM25" s="33"/>
       <c r="AN25" s="33"/>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="54"/>
-      <c r="AQ25" s="49"/>
-      <c r="AR25" s="48"/>
+      <c r="AO25" s="33"/>
+      <c r="AP25" s="56"/>
+      <c r="AQ25" s="54"/>
+      <c r="AR25" s="49"/>
       <c r="AS25" s="48"/>
-      <c r="AT25" s="48"/>
-      <c r="AU25" s="48"/>
-      <c r="AV25" s="48"/>
-      <c r="AW25" s="48"/>
       <c r="AX25" s="48"/>
-    </row>
-    <row r="26" spans="1:60">
+      <c r="AY25" s="48"/>
+      <c r="AZ25" s="48"/>
+      <c r="BA25" s="48"/>
+      <c r="BB25" s="48"/>
+      <c r="BC25" s="48"/>
+    </row>
+    <row r="26" spans="1:65">
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -7089,18 +7311,19 @@
       <c r="AL26" s="33"/>
       <c r="AM26" s="33"/>
       <c r="AN26" s="33"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="54"/>
-      <c r="AQ26" s="49"/>
-      <c r="AR26" s="48"/>
+      <c r="AO26" s="33"/>
+      <c r="AP26" s="56"/>
+      <c r="AQ26" s="54"/>
+      <c r="AR26" s="49"/>
       <c r="AS26" s="48"/>
-      <c r="AT26" s="48"/>
-      <c r="AU26" s="48"/>
-      <c r="AV26" s="48"/>
-      <c r="AW26" s="48"/>
       <c r="AX26" s="48"/>
-    </row>
-    <row r="27" spans="1:60">
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="48"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="48"/>
+      <c r="BC26" s="48"/>
+    </row>
+    <row r="27" spans="1:65">
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -7130,18 +7353,19 @@
       <c r="AL27" s="33"/>
       <c r="AM27" s="33"/>
       <c r="AN27" s="33"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="54"/>
-      <c r="AQ27" s="49"/>
-      <c r="AR27" s="48"/>
+      <c r="AO27" s="33"/>
+      <c r="AP27" s="56"/>
+      <c r="AQ27" s="54"/>
+      <c r="AR27" s="49"/>
       <c r="AS27" s="48"/>
-      <c r="AT27" s="48"/>
-      <c r="AU27" s="48"/>
-      <c r="AV27" s="48"/>
-      <c r="AW27" s="48"/>
       <c r="AX27" s="48"/>
-    </row>
-    <row r="28" spans="1:60">
+      <c r="AY27" s="48"/>
+      <c r="AZ27" s="48"/>
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="48"/>
+      <c r="BC27" s="48"/>
+    </row>
+    <row r="28" spans="1:65">
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -7171,18 +7395,19 @@
       <c r="AL28" s="33"/>
       <c r="AM28" s="33"/>
       <c r="AN28" s="33"/>
-      <c r="AO28" s="56"/>
-      <c r="AP28" s="54"/>
-      <c r="AQ28" s="49"/>
-      <c r="AR28" s="48"/>
+      <c r="AO28" s="33"/>
+      <c r="AP28" s="56"/>
+      <c r="AQ28" s="54"/>
+      <c r="AR28" s="49"/>
       <c r="AS28" s="48"/>
-      <c r="AT28" s="48"/>
-      <c r="AU28" s="48"/>
-      <c r="AV28" s="48"/>
-      <c r="AW28" s="48"/>
       <c r="AX28" s="48"/>
-    </row>
-    <row r="29" spans="1:60">
+      <c r="AY28" s="48"/>
+      <c r="AZ28" s="48"/>
+      <c r="BA28" s="48"/>
+      <c r="BB28" s="48"/>
+      <c r="BC28" s="48"/>
+    </row>
+    <row r="29" spans="1:65">
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -7212,18 +7437,19 @@
       <c r="AL29" s="33"/>
       <c r="AM29" s="33"/>
       <c r="AN29" s="33"/>
-      <c r="AO29" s="56"/>
-      <c r="AP29" s="54"/>
-      <c r="AQ29" s="49"/>
-      <c r="AR29" s="48"/>
+      <c r="AO29" s="33"/>
+      <c r="AP29" s="56"/>
+      <c r="AQ29" s="54"/>
+      <c r="AR29" s="49"/>
       <c r="AS29" s="48"/>
-      <c r="AT29" s="48"/>
-      <c r="AU29" s="48"/>
-      <c r="AV29" s="48"/>
-      <c r="AW29" s="48"/>
       <c r="AX29" s="48"/>
-    </row>
-    <row r="30" spans="1:60">
+      <c r="AY29" s="48"/>
+      <c r="AZ29" s="48"/>
+      <c r="BA29" s="48"/>
+      <c r="BB29" s="48"/>
+      <c r="BC29" s="48"/>
+    </row>
+    <row r="30" spans="1:65">
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -7253,18 +7479,19 @@
       <c r="AL30" s="33"/>
       <c r="AM30" s="33"/>
       <c r="AN30" s="33"/>
-      <c r="AO30" s="60"/>
-      <c r="AP30" s="32"/>
-      <c r="AQ30" s="49"/>
-      <c r="AR30" s="48"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="45"/>
-      <c r="AU30" s="45"/>
-      <c r="AV30" s="45"/>
-      <c r="AW30" s="45"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="60"/>
+      <c r="AQ30" s="32"/>
+      <c r="AR30" s="49"/>
+      <c r="AS30" s="48"/>
       <c r="AX30" s="45"/>
-    </row>
-    <row r="31" spans="1:60">
+      <c r="AY30" s="45"/>
+      <c r="AZ30" s="45"/>
+      <c r="BA30" s="45"/>
+      <c r="BB30" s="45"/>
+      <c r="BC30" s="45"/>
+    </row>
+    <row r="31" spans="1:65">
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -7294,16 +7521,17 @@
       <c r="AL31" s="33"/>
       <c r="AM31" s="33"/>
       <c r="AN31" s="33"/>
-      <c r="AQ31" s="49"/>
-      <c r="AR31" s="48"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="45"/>
-      <c r="AU31" s="45"/>
-      <c r="AV31" s="45"/>
-      <c r="AW31" s="45"/>
+      <c r="AO31" s="33"/>
+      <c r="AR31" s="49"/>
+      <c r="AS31" s="48"/>
       <c r="AX31" s="45"/>
-    </row>
-    <row r="32" spans="1:60">
+      <c r="AY31" s="45"/>
+      <c r="AZ31" s="45"/>
+      <c r="BA31" s="45"/>
+      <c r="BB31" s="45"/>
+      <c r="BC31" s="45"/>
+    </row>
+    <row r="32" spans="1:65">
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
@@ -7333,16 +7561,17 @@
       <c r="AL32" s="33"/>
       <c r="AM32" s="33"/>
       <c r="AN32" s="33"/>
-      <c r="AQ32" s="49"/>
-      <c r="AR32" s="48"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="45"/>
-      <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
+      <c r="AO32" s="33"/>
+      <c r="AR32" s="49"/>
+      <c r="AS32" s="48"/>
       <c r="AX32" s="45"/>
-    </row>
-    <row r="33" spans="3:50">
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+    </row>
+    <row r="33" spans="3:55">
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
@@ -7360,16 +7589,17 @@
       <c r="AL33" s="33"/>
       <c r="AM33" s="33"/>
       <c r="AN33" s="33"/>
-      <c r="AQ33" s="49"/>
-      <c r="AR33" s="48"/>
-      <c r="AS33" s="45"/>
-      <c r="AT33" s="45"/>
-      <c r="AU33" s="45"/>
-      <c r="AV33" s="45"/>
-      <c r="AW33" s="45"/>
+      <c r="AO33" s="33"/>
+      <c r="AR33" s="49"/>
+      <c r="AS33" s="48"/>
       <c r="AX33" s="45"/>
-    </row>
-    <row r="34" spans="3:50">
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+    </row>
+    <row r="34" spans="3:55">
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
@@ -7387,16 +7617,17 @@
       <c r="AL34" s="33"/>
       <c r="AM34" s="33"/>
       <c r="AN34" s="33"/>
-      <c r="AQ34" s="49"/>
-      <c r="AR34" s="48"/>
-      <c r="AS34" s="45"/>
-      <c r="AT34" s="45"/>
-      <c r="AU34" s="45"/>
-      <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
+      <c r="AO34" s="33"/>
+      <c r="AR34" s="49"/>
+      <c r="AS34" s="48"/>
       <c r="AX34" s="45"/>
-    </row>
-    <row r="35" spans="3:50">
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+    </row>
+    <row r="35" spans="3:55">
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -7414,16 +7645,17 @@
       <c r="AL35" s="33"/>
       <c r="AM35" s="33"/>
       <c r="AN35" s="33"/>
-      <c r="AQ35" s="49"/>
-      <c r="AR35" s="48"/>
-      <c r="AS35" s="45"/>
-      <c r="AT35" s="45"/>
-      <c r="AU35" s="45"/>
-      <c r="AV35" s="45"/>
-      <c r="AW35" s="45"/>
+      <c r="AO35" s="33"/>
+      <c r="AR35" s="49"/>
+      <c r="AS35" s="48"/>
       <c r="AX35" s="45"/>
-    </row>
-    <row r="36" spans="3:50">
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="45"/>
+      <c r="BA35" s="45"/>
+      <c r="BB35" s="45"/>
+      <c r="BC35" s="45"/>
+    </row>
+    <row r="36" spans="3:55">
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -7453,16 +7685,17 @@
       <c r="AL36" s="33"/>
       <c r="AM36" s="33"/>
       <c r="AN36" s="33"/>
-      <c r="AQ36" s="49"/>
-      <c r="AR36" s="48"/>
-      <c r="AS36" s="45"/>
-      <c r="AT36" s="45"/>
-      <c r="AU36" s="45"/>
-      <c r="AV36" s="45"/>
-      <c r="AW36" s="45"/>
+      <c r="AO36" s="33"/>
+      <c r="AR36" s="49"/>
+      <c r="AS36" s="48"/>
       <c r="AX36" s="45"/>
-    </row>
-    <row r="37" spans="3:50">
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="45"/>
+      <c r="BA36" s="45"/>
+      <c r="BB36" s="45"/>
+      <c r="BC36" s="45"/>
+    </row>
+    <row r="37" spans="3:55">
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -7492,16 +7725,17 @@
       <c r="AL37" s="33"/>
       <c r="AM37" s="33"/>
       <c r="AN37" s="33"/>
-      <c r="AQ37" s="49"/>
-      <c r="AR37" s="48"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45"/>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
+      <c r="AO37" s="33"/>
+      <c r="AR37" s="49"/>
+      <c r="AS37" s="48"/>
       <c r="AX37" s="45"/>
-    </row>
-    <row r="38" spans="3:50">
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="45"/>
+      <c r="BA37" s="45"/>
+      <c r="BB37" s="45"/>
+      <c r="BC37" s="45"/>
+    </row>
+    <row r="38" spans="3:55">
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -7531,16 +7765,17 @@
       <c r="AL38" s="33"/>
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
-      <c r="AQ38" s="49"/>
-      <c r="AR38" s="48"/>
-      <c r="AS38" s="45"/>
-      <c r="AT38" s="45"/>
-      <c r="AU38" s="45"/>
-      <c r="AV38" s="45"/>
-      <c r="AW38" s="45"/>
+      <c r="AO38" s="33"/>
+      <c r="AR38" s="49"/>
+      <c r="AS38" s="48"/>
       <c r="AX38" s="45"/>
-    </row>
-    <row r="39" spans="3:50">
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="45"/>
+      <c r="BA38" s="45"/>
+      <c r="BB38" s="45"/>
+      <c r="BC38" s="45"/>
+    </row>
+    <row r="39" spans="3:55">
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -7570,57 +7805,58 @@
       <c r="AL39" s="33"/>
       <c r="AM39" s="33"/>
       <c r="AN39" s="33"/>
-      <c r="AQ39" s="49"/>
-      <c r="AR39" s="48"/>
-      <c r="AS39" s="45"/>
-      <c r="AT39" s="45"/>
-      <c r="AU39" s="45"/>
-      <c r="AV39" s="45"/>
-      <c r="AW39" s="45"/>
+      <c r="AO39" s="33"/>
+      <c r="AR39" s="49"/>
+      <c r="AS39" s="48"/>
       <c r="AX39" s="45"/>
-    </row>
-    <row r="40" spans="3:50">
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="45"/>
+      <c r="BA39" s="45"/>
+      <c r="BB39" s="45"/>
+      <c r="BC39" s="45"/>
+    </row>
+    <row r="40" spans="3:55">
       <c r="AA40" s="28"/>
       <c r="AI40" s="74"/>
       <c r="AJ40" s="74"/>
-      <c r="AQ40" s="45"/>
       <c r="AR40" s="45"/>
       <c r="AS40" s="45"/>
-      <c r="AT40" s="45"/>
-      <c r="AU40" s="45"/>
-      <c r="AV40" s="45"/>
-      <c r="AW40" s="45"/>
       <c r="AX40" s="45"/>
-    </row>
-    <row r="41" spans="3:50">
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="45"/>
+      <c r="BB40" s="45"/>
+      <c r="BC40" s="45"/>
+    </row>
+    <row r="41" spans="3:55">
       <c r="AI41" s="74"/>
       <c r="AJ41" s="74"/>
     </row>
-    <row r="42" spans="3:50">
+    <row r="42" spans="3:55">
       <c r="AI42" s="74"/>
       <c r="AJ42" s="74"/>
     </row>
-    <row r="43" spans="3:50">
+    <row r="43" spans="3:55">
       <c r="AI43" s="74"/>
       <c r="AJ43" s="74"/>
     </row>
-    <row r="44" spans="3:50">
+    <row r="44" spans="3:55">
       <c r="AI44" s="74"/>
       <c r="AJ44" s="74"/>
     </row>
-    <row r="45" spans="3:50">
+    <row r="45" spans="3:55">
       <c r="AI45" s="74"/>
       <c r="AJ45" s="74"/>
     </row>
-    <row r="46" spans="3:50">
+    <row r="46" spans="3:55">
       <c r="AI46" s="74"/>
       <c r="AJ46" s="74"/>
     </row>
-    <row r="47" spans="3:50">
+    <row r="47" spans="3:55">
       <c r="AI47" s="74"/>
       <c r="AJ47" s="74"/>
     </row>
-    <row r="48" spans="3:50">
+    <row r="48" spans="3:55">
       <c r="AI48" s="74"/>
       <c r="AJ48" s="74"/>
     </row>
@@ -7650,6 +7886,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7657,8 +7894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7683,26 +7920,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="124" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
+      <c r="A1" s="129" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
       <c r="O1" s="115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P1" s="116"/>
       <c r="Q1" s="115"/>
@@ -7727,28 +7964,28 @@
         <v>35</v>
       </c>
       <c r="G2" s="118" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="118" t="s">
+      <c r="I2" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="J2" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="K2" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="118" t="s">
+      <c r="L2" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="118" t="s">
+      <c r="M2" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="118" t="s">
+      <c r="N2" s="118" t="s">
         <v>105</v>
-      </c>
-      <c r="N2" s="118" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -7816,22 +8053,22 @@
         <v>-12.87</v>
       </c>
       <c r="D4" s="69">
-        <f t="shared" ref="D4:D9" si="0">AVERAGE(B4:C4)</f>
+        <f>AVERAGE(B4:C4)</f>
         <v>-3.6599999999999997</v>
       </c>
       <c r="E4" s="69">
         <v>32.729999999999997</v>
       </c>
       <c r="F4" s="69">
-        <f t="shared" ref="F4:F9" si="1">B4-C4</f>
+        <f t="shared" ref="F4:F9" si="0">B4-C4</f>
         <v>18.419999999999998</v>
       </c>
       <c r="G4" s="65">
-        <f t="shared" ref="G4:G9" si="2">(B4/1000+1)*0.0036765</f>
+        <f>(B4/1000+1)*0.0036765</f>
         <v>3.6969045749999999E-3</v>
       </c>
       <c r="H4" s="65">
-        <f t="shared" ref="H4:H9" si="3">(C4/1000+1)*0.0036765</f>
+        <f>(C4/1000+1)*0.0036765</f>
         <v>3.6291834449999998E-3</v>
       </c>
       <c r="I4" s="65">
@@ -7870,38 +8107,38 @@
         <v>-0.14814902897277774</v>
       </c>
       <c r="D5" s="69">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B5:C5)</f>
         <v>-0.27605719204194445</v>
       </c>
       <c r="E5" s="69">
         <v>41.949257311111111</v>
       </c>
       <c r="F5" s="69">
+        <f t="shared" si="0"/>
+        <v>-0.25581632613833338</v>
+      </c>
+      <c r="G5" s="65">
+        <f t="shared" ref="G5:H9" si="1">(B5/1000+1)*0.0036765</f>
+        <v>3.6750148213719339E-3</v>
+      </c>
+      <c r="H5" s="65">
         <f t="shared" si="1"/>
-        <v>-0.25581632613833338</v>
-      </c>
-      <c r="G5" s="65">
-        <f t="shared" si="2"/>
-        <v>3.6750148213719339E-3</v>
-      </c>
-      <c r="H5" s="65">
-        <f t="shared" si="3"/>
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I5" s="65">
-        <f t="shared" ref="I5:I9" si="4">(E5/1000+1)*0.0020052</f>
+        <f t="shared" ref="I5:I9" si="2">(E5/1000+1)*0.0020052</f>
         <v>2.0893166507602399E-3</v>
       </c>
       <c r="J5" s="65">
-        <f t="shared" ref="J5:J9" si="5">(I5/0.0020052)^0.516*0.0003799</f>
+        <f t="shared" ref="J5:J9" si="3">(I5/0.0020052)^0.516*0.0003799</f>
         <v>3.8804145413997107E-4</v>
       </c>
       <c r="K5" s="66">
-        <f t="shared" ref="K5:K9" si="6">G5+H5+J5</f>
+        <f t="shared" ref="K5:K9" si="4">G5+H5+J5</f>
         <v>7.7390116056068863E-3</v>
       </c>
       <c r="L5" s="66">
-        <f t="shared" ref="L5:L9" si="7">(G5+H5)*J5+I5+G5*H5</f>
+        <f t="shared" ref="L5:L9" si="5">(G5+H5)*J5+I5+G5*H5</f>
         <v>2.1056783222279545E-3</v>
       </c>
       <c r="M5" s="67">
@@ -7915,7 +8152,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="68" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B6" s="69">
         <v>-22.21</v>
@@ -7924,38 +8161,38 @@
         <v>-49.28</v>
       </c>
       <c r="D6" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D6:D9" si="6">AVERAGE(B6:C6)</f>
         <v>-35.745000000000005</v>
       </c>
       <c r="E6" s="69">
         <v>26.94</v>
       </c>
       <c r="F6" s="69">
+        <f t="shared" si="0"/>
+        <v>27.07</v>
+      </c>
+      <c r="G6" s="65">
         <f t="shared" si="1"/>
-        <v>27.07</v>
-      </c>
-      <c r="G6" s="65">
+        <v>3.5948449350000004E-3</v>
+      </c>
+      <c r="H6" s="65">
+        <f t="shared" si="1"/>
+        <v>3.49532208E-3</v>
+      </c>
+      <c r="I6" s="65">
         <f t="shared" si="2"/>
-        <v>3.5948449350000004E-3</v>
-      </c>
-      <c r="H6" s="65">
+        <v>2.0592200879999997E-3</v>
+      </c>
+      <c r="J6" s="65">
         <f t="shared" si="3"/>
-        <v>3.49532208E-3</v>
-      </c>
-      <c r="I6" s="65">
+        <v>3.8514702697154833E-4</v>
+      </c>
+      <c r="K6" s="66">
         <f t="shared" si="4"/>
-        <v>2.0592200879999997E-3</v>
-      </c>
-      <c r="J6" s="65">
+        <v>7.4753140419715489E-3</v>
+      </c>
+      <c r="L6" s="66">
         <f t="shared" si="5"/>
-        <v>3.8514702697154833E-4</v>
-      </c>
-      <c r="K6" s="66">
-        <f t="shared" si="6"/>
-        <v>7.4753140419715489E-3</v>
-      </c>
-      <c r="L6" s="66">
-        <f t="shared" si="7"/>
         <v>2.0745159856220404E-3</v>
       </c>
       <c r="M6" s="67">
@@ -7978,38 +8215,38 @@
         <v>94.44</v>
       </c>
       <c r="D7" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>48.074999999999996</v>
       </c>
       <c r="E7" s="69">
         <v>36.01</v>
       </c>
       <c r="F7" s="69">
+        <f t="shared" si="0"/>
+        <v>-92.73</v>
+      </c>
+      <c r="G7" s="65">
+        <f>(B7/1000+1)*0.0036765</f>
+        <v>3.6827868150000006E-3</v>
+      </c>
+      <c r="H7" s="65">
         <f t="shared" si="1"/>
-        <v>-92.73</v>
-      </c>
-      <c r="G7" s="65">
+        <v>4.0237086600000008E-3</v>
+      </c>
+      <c r="I7" s="65">
         <f t="shared" si="2"/>
-        <v>3.6827868150000006E-3</v>
-      </c>
-      <c r="H7" s="65">
+        <v>2.0774072520000002E-3</v>
+      </c>
+      <c r="J7" s="65">
         <f t="shared" si="3"/>
-        <v>4.0237086600000008E-3</v>
-      </c>
-      <c r="I7" s="65">
+        <v>3.8689853960154226E-4</v>
+      </c>
+      <c r="K7" s="66">
         <f t="shared" si="4"/>
-        <v>2.0774072520000002E-3</v>
-      </c>
-      <c r="J7" s="65">
+        <v>8.0933940146015442E-3</v>
+      </c>
+      <c r="L7" s="66">
         <f t="shared" si="5"/>
-        <v>3.8689853960154226E-4</v>
-      </c>
-      <c r="K7" s="66">
-        <f t="shared" si="6"/>
-        <v>8.0933940146015442E-3</v>
-      </c>
-      <c r="L7" s="66">
-        <f t="shared" si="7"/>
         <v>2.0952073450451725E-3</v>
       </c>
       <c r="M7" s="67">
@@ -8023,7 +8260,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="68" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" s="69">
         <v>17.11</v>
@@ -8032,38 +8269,38 @@
         <v>-3.43</v>
       </c>
       <c r="D8" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6.84</v>
       </c>
       <c r="E8" s="69">
         <v>35.29</v>
       </c>
       <c r="F8" s="69">
+        <f t="shared" si="0"/>
+        <v>20.54</v>
+      </c>
+      <c r="G8" s="65">
         <f t="shared" si="1"/>
-        <v>20.54</v>
-      </c>
-      <c r="G8" s="65">
+        <v>3.7394049149999998E-3</v>
+      </c>
+      <c r="H8" s="65">
+        <f t="shared" si="1"/>
+        <v>3.6638896049999998E-3</v>
+      </c>
+      <c r="I8" s="65">
         <f t="shared" si="2"/>
-        <v>3.7394049149999998E-3</v>
-      </c>
-      <c r="H8" s="65">
+        <v>2.0759635080000003E-3</v>
+      </c>
+      <c r="J8" s="65">
         <f t="shared" si="3"/>
-        <v>3.6638896049999998E-3</v>
-      </c>
-      <c r="I8" s="65">
+        <v>3.8675977189798279E-4</v>
+      </c>
+      <c r="K8" s="66">
         <f t="shared" si="4"/>
-        <v>2.0759635080000003E-3</v>
-      </c>
-      <c r="J8" s="65">
+        <v>7.7900542918979817E-3</v>
+      </c>
+      <c r="L8" s="66">
         <f t="shared" si="5"/>
-        <v>3.8675977189798279E-4</v>
-      </c>
-      <c r="K8" s="66">
-        <f t="shared" si="6"/>
-        <v>7.7900542918979817E-3</v>
-      </c>
-      <c r="L8" s="66">
-        <f t="shared" si="7"/>
         <v>2.0925275712968031E-3</v>
       </c>
       <c r="M8" s="67">
@@ -8085,39 +8322,39 @@
       <c r="C9" s="120">
         <v>25.44</v>
       </c>
-      <c r="D9" s="69">
-        <f t="shared" si="0"/>
+      <c r="D9" s="120">
+        <f t="shared" si="6"/>
         <v>25.585000000000001</v>
       </c>
       <c r="E9" s="120">
         <v>35.880000000000003</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="120">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999915</v>
+      </c>
+      <c r="G9" s="121">
         <f t="shared" si="1"/>
-        <v>0.28999999999999915</v>
-      </c>
-      <c r="G9" s="65">
+        <v>3.7710963450000002E-3</v>
+      </c>
+      <c r="H9" s="121">
+        <f t="shared" si="1"/>
+        <v>3.7700301599999995E-3</v>
+      </c>
+      <c r="I9" s="121">
         <f t="shared" si="2"/>
-        <v>3.7710963450000002E-3</v>
-      </c>
-      <c r="H9" s="65">
+        <v>2.0771465759999996E-3</v>
+      </c>
+      <c r="J9" s="121">
         <f t="shared" si="3"/>
-        <v>3.7700301599999995E-3</v>
-      </c>
-      <c r="I9" s="121">
+        <v>3.8687348777560239E-4</v>
+      </c>
+      <c r="K9" s="122">
         <f t="shared" si="4"/>
-        <v>2.0771465759999996E-3</v>
-      </c>
-      <c r="J9" s="121">
+        <v>7.9279999927756029E-3</v>
+      </c>
+      <c r="L9" s="122">
         <f t="shared" si="5"/>
-        <v>3.8687348777560239E-4</v>
-      </c>
-      <c r="K9" s="122">
-        <f t="shared" si="6"/>
-        <v>7.9279999927756029E-3</v>
-      </c>
-      <c r="L9" s="122">
-        <f t="shared" si="7"/>
         <v>2.0942811848696616E-3</v>
       </c>
       <c r="M9" s="123">
@@ -8146,7 +8383,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="114"/>
       <c r="B11" s="70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11" s="114"/>
@@ -8162,10 +8399,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>110</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>26</v>
@@ -8174,22 +8411,22 @@
         <v>27</v>
       </c>
       <c r="F12" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="H12" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="I12" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="63" t="s">
-        <v>114</v>
-      </c>
       <c r="J12" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>108</v>
       </c>
       <c r="M12" s="63"/>
       <c r="O12" s="63"/>
@@ -8200,11 +8437,11 @@
         <v>ATM_EQ_SW</v>
       </c>
       <c r="B13" s="68">
-        <f t="shared" ref="B13:C15" si="8">M3</f>
+        <f t="shared" ref="B13:C15" si="7">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C13" s="68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="D13" s="111">
@@ -8216,19 +8453,19 @@
         <v>1.0075218399408568</v>
       </c>
       <c r="F13" s="67">
-        <f t="shared" ref="F13:F27" si="9">LN(D13)</f>
+        <f t="shared" ref="F13:F27" si="8">LN(D13)</f>
         <v>5.6690060748599133E-3</v>
       </c>
       <c r="G13" s="67">
-        <f t="shared" ref="G13:G27" si="10">LN(E13)</f>
+        <f t="shared" ref="G13:G27" si="9">LN(E13)</f>
         <v>7.4936919644022753E-3</v>
       </c>
       <c r="H13" s="67">
-        <f t="shared" ref="H13:I19" si="11">LN(B13)</f>
+        <f t="shared" ref="H13:I19" si="10">LN(B13)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I13" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4.412758119012896E-3</v>
       </c>
       <c r="J13" s="72">
@@ -8246,11 +8483,11 @@
         <v>S2_ref_1</v>
       </c>
       <c r="B14" s="68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="C14" s="68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="D14" s="111">
@@ -8262,19 +8499,19 @@
         <v>0.99497700286985102</v>
       </c>
       <c r="F14" s="67">
+        <f t="shared" si="8"/>
+        <v>-3.3157633670658081E-3</v>
+      </c>
+      <c r="G14" s="67">
         <f t="shared" si="9"/>
-        <v>-3.3157633670658081E-3</v>
-      </c>
-      <c r="G14" s="67">
+        <v>-5.0356547842637621E-3</v>
+      </c>
+      <c r="H14" s="67">
         <f t="shared" si="10"/>
-        <v>-5.0356547842637621E-3</v>
-      </c>
-      <c r="H14" s="67">
-        <f t="shared" si="11"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I14" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8284,11 +8521,11 @@
         <v>B6_ref_1</v>
       </c>
       <c r="B15" s="68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="C15" s="68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="D15" s="111">
@@ -8300,19 +8537,19 @@
         <v>1.0043106480077921</v>
       </c>
       <c r="F15" s="67">
+        <f t="shared" si="8"/>
+        <v>3.8320385549917295E-4</v>
+      </c>
+      <c r="G15" s="67">
         <f t="shared" si="9"/>
-        <v>3.8320385549917295E-4</v>
-      </c>
-      <c r="G15" s="67">
+        <v>4.3013837783483656E-3</v>
+      </c>
+      <c r="H15" s="67">
         <f t="shared" si="10"/>
-        <v>4.3013837783483656E-3</v>
-      </c>
-      <c r="H15" s="67">
-        <f t="shared" si="11"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I15" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8322,11 +8559,11 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="B16" s="68">
-        <f t="shared" ref="B16:C18" si="12">M3</f>
+        <f t="shared" ref="B16:C18" si="11">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C16" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="D16" s="111">
@@ -8338,19 +8575,19 @@
         <v>1.0077071570383731</v>
       </c>
       <c r="F16" s="67">
+        <f t="shared" si="8"/>
+        <v>6.3855513126554056E-3</v>
+      </c>
+      <c r="G16" s="67">
         <f t="shared" si="9"/>
-        <v>6.3855513126554056E-3</v>
-      </c>
-      <c r="G16" s="67">
+        <v>7.6776086292741075E-3</v>
+      </c>
+      <c r="H16" s="67">
         <f t="shared" si="10"/>
-        <v>7.6776086292741075E-3</v>
-      </c>
-      <c r="H16" s="67">
-        <f t="shared" si="11"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I16" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8360,11 +8597,11 @@
         <v>S2_ref_2</v>
       </c>
       <c r="B17" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="C17" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="D17" s="111">
@@ -8376,19 +8613,19 @@
         <v>0.9951628615034982</v>
       </c>
       <c r="F17" s="67">
+        <f t="shared" si="8"/>
+        <v>-3.3736683280273967E-3</v>
+      </c>
+      <c r="G17" s="67">
         <f t="shared" si="9"/>
-        <v>-3.3736683280273967E-3</v>
-      </c>
-      <c r="G17" s="67">
+        <v>-4.8488753146248009E-3</v>
+      </c>
+      <c r="H17" s="67">
         <f t="shared" si="10"/>
-        <v>-4.8488753146248009E-3</v>
-      </c>
-      <c r="H17" s="67">
-        <f t="shared" si="11"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I17" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8398,11 +8635,11 @@
         <v>B6_ref_2</v>
       </c>
       <c r="B18" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="C18" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="D18" s="111">
@@ -8414,19 +8651,19 @@
         <v>1.0023860907979212</v>
       </c>
       <c r="F18" s="67">
+        <f t="shared" si="8"/>
+        <v>-8.2966123175853173E-4</v>
+      </c>
+      <c r="G18" s="67">
         <f t="shared" si="9"/>
-        <v>-8.2966123175853173E-4</v>
-      </c>
-      <c r="G18" s="67">
+        <v>2.3832486035312902E-3</v>
+      </c>
+      <c r="H18" s="67">
         <f t="shared" si="10"/>
-        <v>2.3832486035312902E-3</v>
-      </c>
-      <c r="H18" s="67">
-        <f t="shared" si="11"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I18" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8452,19 +8689,19 @@
         <v>1.0057116133646442</v>
       </c>
       <c r="F19" s="67">
+        <f t="shared" si="8"/>
+        <v>5.0812199816469847E-3</v>
+      </c>
+      <c r="G19" s="67">
         <f t="shared" si="9"/>
-        <v>5.0812199816469847E-3</v>
-      </c>
-      <c r="G19" s="67">
+        <v>5.6953639452707308E-3</v>
+      </c>
+      <c r="H19" s="67">
         <f t="shared" si="10"/>
-        <v>5.6953639452707308E-3</v>
-      </c>
-      <c r="H19" s="67">
-        <f t="shared" si="11"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I19" s="67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8484,11 +8721,11 @@
         <v>1.0049378092932522</v>
       </c>
       <c r="F20" s="67">
+        <f t="shared" si="8"/>
+        <v>-9.1141789753790732E-3</v>
+      </c>
+      <c r="G20" s="67">
         <f t="shared" si="9"/>
-        <v>-9.1141789753790732E-3</v>
-      </c>
-      <c r="G20" s="67">
-        <f t="shared" si="10"/>
         <v>4.9256582960658154E-3</v>
       </c>
       <c r="H20" s="67"/>
@@ -8500,11 +8737,11 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="B21" s="68">
-        <f t="shared" ref="B21:C23" si="13">M3</f>
+        <f t="shared" ref="B21:C23" si="12">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C21" s="68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="D21" s="111">
@@ -8516,19 +8753,19 @@
         <v>1.0054625917600983</v>
       </c>
       <c r="F21" s="67">
+        <f t="shared" si="8"/>
+        <v>5.7029884167436144E-3</v>
+      </c>
+      <c r="G21" s="67">
         <f t="shared" si="9"/>
-        <v>5.7029884167436144E-3</v>
-      </c>
-      <c r="G21" s="67">
-        <f t="shared" si="10"/>
         <v>5.4477259185061388E-3</v>
       </c>
       <c r="H21" s="67">
-        <f t="shared" ref="H21:I26" si="14">LN(B21)</f>
+        <f t="shared" ref="H21:I26" si="13">LN(B21)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I21" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8538,11 +8775,11 @@
         <v>S2_ref_1</v>
       </c>
       <c r="B22" s="68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="C22" s="68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="D22" s="111">
@@ -8554,19 +8791,19 @@
         <v>0.99378130442821833</v>
       </c>
       <c r="F22" s="67">
+        <f t="shared" si="8"/>
+        <v>-3.5945739634335372E-3</v>
+      </c>
+      <c r="G22" s="67">
         <f t="shared" si="9"/>
-        <v>-3.5945739634335372E-3</v>
-      </c>
-      <c r="G22" s="67">
-        <f t="shared" si="10"/>
         <v>-6.2381121983366193E-3</v>
       </c>
       <c r="H22" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I22" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8576,11 +8813,11 @@
         <v>B6_ref_1</v>
       </c>
       <c r="B23" s="68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="C23" s="68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="D23" s="111">
@@ -8592,19 +8829,19 @@
         <v>1.0040343543858852</v>
       </c>
       <c r="F23" s="67">
+        <f t="shared" si="8"/>
+        <v>1.7966870305363727E-4</v>
+      </c>
+      <c r="G23" s="67">
         <f t="shared" si="9"/>
-        <v>1.7966870305363727E-4</v>
-      </c>
-      <c r="G23" s="67">
-        <f t="shared" si="10"/>
         <v>4.0262381999534996E-3</v>
       </c>
       <c r="H23" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I23" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8630,19 +8867,19 @@
         <v>1.0053599727245706</v>
       </c>
       <c r="F24" s="67">
+        <f t="shared" si="8"/>
+        <v>4.8686826228146419E-3</v>
+      </c>
+      <c r="G24" s="67">
         <f t="shared" si="9"/>
-        <v>4.8686826228146419E-3</v>
-      </c>
-      <c r="G24" s="67">
-        <f t="shared" si="10"/>
         <v>5.3456591947391319E-3</v>
       </c>
       <c r="H24" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I24" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8668,19 +8905,19 @@
         <v>1.0064676550191509</v>
       </c>
       <c r="F25" s="67">
+        <f t="shared" si="8"/>
+        <v>5.6228928832132777E-3</v>
+      </c>
+      <c r="G25" s="67">
         <f t="shared" si="9"/>
-        <v>5.6228928832132777E-3</v>
-      </c>
-      <c r="G25" s="67">
-        <f t="shared" si="10"/>
         <v>6.446829485110093E-3</v>
       </c>
       <c r="H25" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I25" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8706,19 +8943,19 @@
         <v>0.99474403428411884</v>
       </c>
       <c r="F26" s="67">
+        <f t="shared" si="8"/>
+        <v>-3.6734640658408848E-3</v>
+      </c>
+      <c r="G26" s="67">
         <f t="shared" si="9"/>
-        <v>-3.6734640658408848E-3</v>
-      </c>
-      <c r="G26" s="67">
-        <f t="shared" si="10"/>
         <v>-5.2698268942697113E-3</v>
       </c>
       <c r="H26" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I26" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8738,11 +8975,11 @@
         <v>1.0044001925480899</v>
       </c>
       <c r="F27" s="67">
+        <f t="shared" si="8"/>
+        <v>-6.5263177824188435E-3</v>
+      </c>
+      <c r="G27" s="67">
         <f t="shared" si="9"/>
-        <v>-6.5263177824188435E-3</v>
-      </c>
-      <c r="G27" s="67">
-        <f t="shared" si="10"/>
         <v>4.3905400058642007E-3</v>
       </c>
       <c r="H27" s="67"/>
@@ -8842,8 +9079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A9B09D-1008-4441-AE31-949281019A29}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8857,16 +9094,16 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N1">
         <v>3.7990000000000002E-4</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
@@ -8875,10 +9112,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N2">
         <v>2.0052E-3</v>
@@ -8887,24 +9124,24 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="126" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="127" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
+      <c r="A3" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="132" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
       <c r="M3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N3">
         <v>0.51600000000000001</v>
@@ -8914,58 +9151,58 @@
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="113" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="113" t="s">
+        <v>141</v>
+      </c>
+      <c r="M4" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" s="113" t="s">
+        <v>142</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="113" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" s="113" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="113" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" s="113" t="s">
-        <v>144</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="Q4" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="113" t="s">
         <v>95</v>
-      </c>
-      <c r="R4" s="113" t="s">
-        <v>96</v>
       </c>
       <c r="V4" s="113"/>
       <c r="Y4" s="113"/>
@@ -9453,7 +9690,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -9464,28 +9701,28 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B2" s="81">
         <f>B12</f>
         <v>0.4623614635092998</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="81">
         <f>C12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
@@ -9494,7 +9731,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="81">
         <f>B13</f>
@@ -9512,20 +9749,20 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="81">
         <v>1.026</v>
       </c>
       <c r="C4" s="79"/>
       <c r="E4" s="79" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4">
         <v>0.99819999999999998</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I4">
         <v>1.002</v>
@@ -9539,7 +9776,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="85">
         <f>1/B4</f>
@@ -9547,14 +9784,14 @@
       </c>
       <c r="C5" s="79"/>
       <c r="E5" s="79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="85">
         <f>1/F4</f>
         <v>1.0018032458425166</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I5" s="85">
         <f>1/I4</f>
@@ -9570,7 +9807,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="88">
         <f>B5/1000</f>
@@ -9578,14 +9815,14 @@
       </c>
       <c r="C6" s="79"/>
       <c r="E6" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F6" s="88">
         <f>F5/1000</f>
         <v>1.0018032458425166E-3</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I6" s="88">
         <f>I5/1000</f>
@@ -9614,7 +9851,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="93" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -9628,10 +9865,10 @@
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="24"/>
@@ -9650,7 +9887,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13">
         <v>8.0186890671505306E-3</v>

</xml_diff>

<commit_message>
finish adding isotopestandards as adjustable parameters
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB24A5B-9122-A74E-9D76-0EE8C6A88ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB2F561-8F2C-A441-A8E3-4FCDF2785F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-38400" yWindow="-5500" windowWidth="38400" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -3863,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AT27" sqref="AT27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AY28" sqref="AY28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4251,10 +4251,10 @@
         <v>0</v>
       </c>
       <c r="AP3" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ3" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR3" s="47">
         <f>A3</f>
@@ -4274,22 +4274,22 @@
         <v>23.3107973301986</v>
       </c>
       <c r="AX3" s="50">
-        <v>15.105455486877901</v>
+        <v>14.956569881199901</v>
       </c>
       <c r="AY3" s="50">
-        <v>-2.7098456777153701</v>
+        <v>-1.30914416602279</v>
       </c>
       <c r="AZ3" s="50">
-        <v>17.815301164593201</v>
+        <v>16.265714047222701</v>
       </c>
       <c r="BA3" s="50">
-        <v>6.19780490458127</v>
+        <v>6.8237128575885899</v>
       </c>
       <c r="BB3" s="50">
-        <v>24.009727067820499</v>
+        <v>11.895220148994101</v>
       </c>
       <c r="BC3" s="50">
-        <v>47.054171086232202</v>
+        <v>23.181326613663298</v>
       </c>
       <c r="BD3" s="44"/>
       <c r="BE3">
@@ -4437,10 +4437,10 @@
         <v>0</v>
       </c>
       <c r="AP4" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ4" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR4" s="47">
         <f t="shared" ref="AR4:AR17" si="10">A4</f>
@@ -4460,22 +4460,22 @@
         <v>11.311867280397299</v>
       </c>
       <c r="AX4" s="50">
-        <v>6.8736240880515798</v>
+        <v>6.7328528090335702</v>
       </c>
       <c r="AY4" s="50">
-        <v>-13.881471917271901</v>
+        <v>-12.4964138972027</v>
       </c>
       <c r="AZ4" s="50">
-        <v>20.755096005323502</v>
+        <v>19.229266706236299</v>
       </c>
       <c r="BA4" s="50">
-        <v>-3.5039239146101799</v>
+        <v>-2.8817805440846098</v>
       </c>
       <c r="BB4" s="50">
-        <v>17.848649659933699</v>
+        <v>5.8070065868232001</v>
       </c>
       <c r="BC4" s="50">
-        <v>34.879852068524698</v>
+        <v>11.284534363441701</v>
       </c>
       <c r="BD4" s="44"/>
       <c r="BE4">
@@ -4628,10 +4628,10 @@
         <v>0</v>
       </c>
       <c r="AP5" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ5" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR5" s="47">
         <f t="shared" si="10"/>
@@ -4651,22 +4651,22 @@
         <v>20.283394786421098</v>
       </c>
       <c r="AX5" s="50">
-        <v>-0.53970856962448599</v>
+        <v>-0.69269808292826696</v>
       </c>
       <c r="AY5" s="50">
-        <v>1.2825215740412901</v>
+        <v>2.6854304734471501</v>
       </c>
       <c r="AZ5" s="50">
-        <v>-1.82223014366578</v>
+        <v>-3.3781285563754202</v>
       </c>
       <c r="BA5" s="50">
-        <v>0.37140650220840399</v>
+        <v>0.99636619525944603</v>
       </c>
       <c r="BB5" s="50">
-        <v>22.461390435589401</v>
+        <v>10.3652371768259</v>
       </c>
       <c r="BC5" s="50">
-        <v>43.988167450184299</v>
+        <v>20.1852985766362</v>
       </c>
       <c r="BD5" s="44"/>
       <c r="BE5">
@@ -4823,10 +4823,10 @@
         <v>0</v>
       </c>
       <c r="AP6" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ6" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR6" s="47">
         <f t="shared" si="10"/>
@@ -4846,22 +4846,22 @@
         <v>23.478838724644199</v>
       </c>
       <c r="AX6" s="50">
-        <v>14.851574153242799</v>
+        <v>14.6995121444024</v>
       </c>
       <c r="AY6" s="50">
-        <v>-0.85838254078074405</v>
+        <v>0.54559628287353901</v>
       </c>
       <c r="AZ6" s="50">
-        <v>15.7099566940236</v>
+        <v>14.153915861528899</v>
       </c>
       <c r="BA6" s="50">
-        <v>6.9965958062310696</v>
+        <v>7.6225542136379998</v>
       </c>
       <c r="BB6" s="50">
-        <v>24.095420378555701</v>
+        <v>11.9799369101096</v>
       </c>
       <c r="BC6" s="50">
-        <v>47.223987370547697</v>
+        <v>23.347344069793301</v>
       </c>
       <c r="BD6" s="44"/>
       <c r="BE6">
@@ -5018,10 +5018,10 @@
         <v>0</v>
       </c>
       <c r="AP7" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ7" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR7" s="47">
         <f t="shared" si="10"/>
@@ -5041,22 +5041,22 @@
         <v>11.492144698644401</v>
       </c>
       <c r="AX7" s="50">
-        <v>6.6566362138331598</v>
+        <v>6.5159608622606902</v>
       </c>
       <c r="AY7" s="50">
-        <v>-13.8026489120794</v>
+        <v>-12.4175729116019</v>
       </c>
       <c r="AZ7" s="50">
-        <v>20.459285125912601</v>
+        <v>18.9335337738626</v>
       </c>
       <c r="BA7" s="50">
-        <v>-3.5730063491231601</v>
+        <v>-2.9508060246706198</v>
       </c>
       <c r="BB7" s="50">
-        <v>17.941820061995799</v>
+        <v>5.8990746403089203</v>
       </c>
       <c r="BC7" s="50">
-        <v>35.063444020270097</v>
+        <v>11.463940218480101</v>
       </c>
       <c r="BD7" s="44"/>
       <c r="BE7">
@@ -5204,10 +5204,10 @@
         <v>0</v>
       </c>
       <c r="AP8" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ8" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR8" s="47">
         <f t="shared" si="10"/>
@@ -5227,22 +5227,22 @@
         <v>18.438709928632498</v>
       </c>
       <c r="AX8" s="50">
-        <v>-1.15628904358433</v>
+        <v>-1.3077253672634199</v>
       </c>
       <c r="AY8" s="50">
-        <v>-0.70441124849329695</v>
+        <v>0.69578908672918105</v>
       </c>
       <c r="AZ8" s="50">
-        <v>-0.45187779509103798</v>
+        <v>-2.0035144539926</v>
       </c>
       <c r="BA8" s="50">
-        <v>-0.93035014603881605</v>
+        <v>-0.30596814026712099</v>
       </c>
       <c r="BB8" s="50">
-        <v>21.5157968077277</v>
+        <v>9.4308247402374796</v>
       </c>
       <c r="BC8" s="50">
-        <v>42.117851051899301</v>
+        <v>18.3576143656101</v>
       </c>
       <c r="BD8" s="44"/>
       <c r="BE8">
@@ -5393,10 +5393,10 @@
         <v>0</v>
       </c>
       <c r="AP9" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ9" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR9" s="47">
         <f t="shared" si="10"/>
@@ -5416,22 +5416,22 @@
         <v>21.5645252666334</v>
       </c>
       <c r="AX9" s="50">
-        <v>16.036656468840999</v>
+        <v>15.8877099673331</v>
       </c>
       <c r="AY9" s="50">
-        <v>-4.8656873390863202</v>
+        <v>-3.4660191730521102</v>
       </c>
       <c r="AZ9" s="50">
-        <v>20.902343807927299</v>
+        <v>19.353729140385202</v>
       </c>
       <c r="BA9" s="50">
-        <v>5.5854845648773397</v>
+        <v>6.2108453971405</v>
       </c>
       <c r="BB9" s="50">
-        <v>23.117269398744899</v>
+        <v>11.013352053047001</v>
       </c>
       <c r="BC9" s="50">
-        <v>45.286402388126902</v>
+        <v>21.4539245146896</v>
       </c>
       <c r="BE9">
         <v>265</v>
@@ -5579,10 +5579,10 @@
         <v>0</v>
       </c>
       <c r="AP10" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ10" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR10" s="47">
         <f t="shared" si="10"/>
@@ -5602,22 +5602,22 @@
         <v>21.0152329961257</v>
       </c>
       <c r="AX10" s="50">
-        <v>14.4579715364672</v>
+        <v>14.352288139259</v>
       </c>
       <c r="AY10" s="50">
-        <v>-34.815304667159701</v>
+        <v>-33.459204607675197</v>
       </c>
       <c r="AZ10" s="50">
-        <v>49.273276203626899</v>
+        <v>47.811492746934299</v>
       </c>
       <c r="BA10" s="50">
-        <v>-10.1786665653462</v>
+        <v>-9.5534582342081098</v>
       </c>
       <c r="BB10" s="50">
-        <v>22.853627356464699</v>
+        <v>10.752661684289199</v>
       </c>
       <c r="BC10" s="50">
-        <v>44.764460247631298</v>
+        <v>20.9435550857681</v>
       </c>
       <c r="BE10">
         <v>265</v>
@@ -5771,10 +5771,10 @@
         <v>0</v>
       </c>
       <c r="AP11" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ11" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR11" s="47">
         <f t="shared" si="10"/>
@@ -5794,22 +5794,22 @@
         <v>21.312858040510601</v>
       </c>
       <c r="AX11" s="50">
-        <v>17.1518234709566</v>
+        <v>17.0031811376099</v>
       </c>
       <c r="AY11" s="50">
-        <v>-4.5745335204508901</v>
+        <v>-3.1753231352780098</v>
       </c>
       <c r="AZ11" s="50">
-        <v>21.726356991407499</v>
+        <v>20.178504272887899</v>
       </c>
       <c r="BA11" s="50">
-        <v>6.2886449752528799</v>
+        <v>6.9139290011659398</v>
       </c>
       <c r="BB11" s="50">
-        <v>22.988533215933799</v>
+        <v>10.886102464315799</v>
       </c>
       <c r="BC11" s="50">
-        <v>45.031522726332703</v>
+        <v>21.204784813545398</v>
       </c>
       <c r="BE11">
         <v>265</v>
@@ -5955,10 +5955,10 @@
         <v>0</v>
       </c>
       <c r="AP12" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ12" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR12" s="47">
         <f t="shared" si="10"/>
@@ -5978,22 +5978,22 @@
         <v>10.1615046903504</v>
       </c>
       <c r="AX12" s="50">
-        <v>7.0098620813652204</v>
+        <v>6.8691236337024</v>
       </c>
       <c r="AY12" s="50">
-        <v>-14.5751415214816</v>
+        <v>-13.1908425064558</v>
       </c>
       <c r="AZ12" s="50">
-        <v>21.5850036028468</v>
+        <v>20.059966140158199</v>
       </c>
       <c r="BA12" s="50">
-        <v>-3.78263972005821</v>
+        <v>-3.16085943637672</v>
       </c>
       <c r="BB12" s="50">
-        <v>17.254451999306699</v>
+        <v>5.2198365059918901</v>
       </c>
       <c r="BC12" s="50">
-        <v>33.709358475152598</v>
+        <v>10.140724063810501</v>
       </c>
       <c r="BE12">
         <v>265</v>
@@ -6139,10 +6139,10 @@
         <v>0</v>
       </c>
       <c r="AP13" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ13" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR13" s="47">
         <f t="shared" si="10"/>
@@ -6162,22 +6162,22 @@
         <v>20.018964220354299</v>
       </c>
       <c r="AX13" s="50">
-        <v>8.2241945278393999E-2</v>
+        <v>-6.9636109155779502E-2</v>
       </c>
       <c r="AY13" s="50">
-        <v>0.22102332359041901</v>
+        <v>1.62265568257535</v>
       </c>
       <c r="AZ13" s="50">
-        <v>-0.138781378312025</v>
+        <v>-1.69229179173113</v>
       </c>
       <c r="BA13" s="50">
-        <v>0.151632634434406</v>
+        <v>0.77650978670978898</v>
       </c>
       <c r="BB13" s="50">
-        <v>22.3259423648012</v>
+        <v>10.2313866904628</v>
       </c>
       <c r="BC13" s="50">
-        <v>43.720161276728597</v>
+        <v>19.923393489895201</v>
       </c>
       <c r="BE13">
         <v>265</v>
@@ -6323,10 +6323,10 @@
         <v>0</v>
       </c>
       <c r="AP14" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ14" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR14" s="47">
         <f t="shared" si="10"/>
@@ -6346,22 +6346,22 @@
         <v>21.227066743560101</v>
       </c>
       <c r="AX14" s="50">
-        <v>14.393773542834699</v>
+        <v>14.2431406435554</v>
       </c>
       <c r="AY14" s="50">
-        <v>-3.6809189289388402</v>
+        <v>-2.2797739750280899</v>
       </c>
       <c r="AZ14" s="50">
-        <v>18.074692471773599</v>
+        <v>16.522914618583499</v>
       </c>
       <c r="BA14" s="50">
-        <v>5.3564273069479604</v>
+        <v>5.9816833342636802</v>
       </c>
       <c r="BB14" s="50">
-        <v>22.94455532836</v>
+        <v>10.842666492212899</v>
       </c>
       <c r="BC14" s="50">
-        <v>44.944459545090702</v>
+        <v>21.119749032101499</v>
       </c>
       <c r="BE14">
         <v>265</v>
@@ -6507,10 +6507,10 @@
         <v>0</v>
       </c>
       <c r="AP15" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ15" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR15" s="47">
         <f t="shared" si="10"/>
@@ -6530,22 +6530,22 @@
         <v>22.288837817687501</v>
       </c>
       <c r="AX15" s="50">
-        <v>16.679833428360201</v>
+        <v>16.532525106017101</v>
       </c>
       <c r="AY15" s="50">
-        <v>-4.3336183513273898</v>
+        <v>-2.9351313709296001</v>
       </c>
       <c r="AZ15" s="50">
-        <v>21.0134517796876</v>
+        <v>19.467656476946701</v>
       </c>
       <c r="BA15" s="50">
-        <v>6.1731075385164003</v>
+        <v>6.7986968675437502</v>
       </c>
       <c r="BB15" s="50">
-        <v>23.487665779901398</v>
+        <v>11.379325857980101</v>
       </c>
       <c r="BC15" s="50">
-        <v>46.019903286484897</v>
+        <v>22.170622053120798</v>
       </c>
       <c r="BE15">
         <v>265</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="AP16" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ16" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR16" s="47">
         <f t="shared" si="10"/>
@@ -6714,22 +6714,22 @@
         <v>11.091902549817901</v>
       </c>
       <c r="AX16" s="50">
-        <v>7.1029978910310803</v>
+        <v>6.9634194564072098</v>
       </c>
       <c r="AY16" s="50">
-        <v>-14.893050092214599</v>
+        <v>-13.5093226554305</v>
       </c>
       <c r="AZ16" s="50">
-        <v>21.996047983245699</v>
+        <v>20.4727421118378</v>
       </c>
       <c r="BA16" s="50">
-        <v>-3.8950261005917799</v>
+        <v>-3.2729515995116798</v>
       </c>
       <c r="BB16" s="50">
-        <v>17.735485742880101</v>
+        <v>5.6951756443239798</v>
       </c>
       <c r="BC16" s="50">
-        <v>34.656884164523802</v>
+        <v>11.0666388211797</v>
       </c>
       <c r="BE16">
         <v>265</v>
@@ -6871,10 +6871,10 @@
         <v>0</v>
       </c>
       <c r="AP17" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.18304360488468446</v>
       </c>
       <c r="AQ17" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.1523129077768495E-2</v>
       </c>
       <c r="AR17" s="47">
         <f t="shared" si="10"/>
@@ -6894,22 +6894,22 @@
         <v>20.468119894696301</v>
       </c>
       <c r="AX17" s="50">
-        <v>13.725240315331099</v>
+        <v>13.6101546598585</v>
       </c>
       <c r="AY17" s="50">
-        <v>-28.3353648321477</v>
+        <v>-26.970212518336499</v>
       </c>
       <c r="AZ17" s="50">
-        <v>42.060605147478803</v>
+        <v>40.580367178195097</v>
       </c>
       <c r="BA17" s="50">
-        <v>-7.3050622584082596</v>
+        <v>-6.6800289292389596</v>
       </c>
       <c r="BB17" s="50">
-        <v>22.565126816266901</v>
+        <v>10.467548323551901</v>
       </c>
       <c r="BC17" s="50">
-        <v>44.193449376003002</v>
+        <v>20.385512621972499</v>
       </c>
       <c r="BE17">
         <v>265</v>
@@ -7895,7 +7895,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8597,11 +8597,11 @@
         <v>S2_ref_2</v>
       </c>
       <c r="B17" s="68">
-        <f t="shared" si="11"/>
+        <f>M4</f>
         <v>0.99629623559207692</v>
       </c>
       <c r="C17" s="68">
-        <f t="shared" si="11"/>
+        <f>N4</f>
         <v>0.99323347721175648</v>
       </c>
       <c r="D17" s="111">
@@ -8613,19 +8613,19 @@
         <v>0.9951628615034982</v>
       </c>
       <c r="F17" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F17" si="12">LN(D17)</f>
         <v>-3.3736683280273967E-3</v>
       </c>
       <c r="G17" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G17" si="13">LN(E17)</f>
         <v>-4.8488753146248009E-3</v>
       </c>
       <c r="H17" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="H17" si="14">LN(B17)</f>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I17" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="I17" si="15">LN(C17)</f>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8737,11 +8737,11 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="B21" s="68">
-        <f t="shared" ref="B21:C23" si="12">M3</f>
+        <f t="shared" ref="B21:C23" si="16">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C21" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="D21" s="111">
@@ -8761,11 +8761,11 @@
         <v>5.4477259185061388E-3</v>
       </c>
       <c r="H21" s="67">
-        <f t="shared" ref="H21:I26" si="13">LN(B21)</f>
+        <f t="shared" ref="H21:I26" si="17">LN(B21)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I21" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8775,11 +8775,11 @@
         <v>S2_ref_1</v>
       </c>
       <c r="B22" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="C22" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="D22" s="111">
@@ -8799,11 +8799,11 @@
         <v>-6.2381121983366193E-3</v>
       </c>
       <c r="H22" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I22" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8813,11 +8813,11 @@
         <v>B6_ref_1</v>
       </c>
       <c r="B23" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="C23" s="68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="D23" s="111">
@@ -8837,11 +8837,11 @@
         <v>4.0262381999534996E-3</v>
       </c>
       <c r="H23" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="I23" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8875,11 +8875,11 @@
         <v>5.3456591947391319E-3</v>
       </c>
       <c r="H24" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I24" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8913,11 +8913,11 @@
         <v>6.446829485110093E-3</v>
       </c>
       <c r="H25" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="I25" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8951,11 +8951,11 @@
         <v>-5.2698268942697113E-3</v>
       </c>
       <c r="H26" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="I26" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attempt to add D17O, issues with d18O values
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2ED6DB-7243-E345-98E0-41F48718910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FBDBD9-4BF0-5C46-B730-80777E60AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="37200" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -3983,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3:AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8014,7 +8014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
another commit no idea what's going on
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FBDBD9-4BF0-5C46-B730-80777E60AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF122A7-5BD0-9E44-8C82-51A818230959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -3983,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3:AO17"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AW26" sqref="AW26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8014,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Add D17O to calculate_17R and SPnonlineq
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF122A7-5BD0-9E44-8C82-51A818230959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF98DA7C-7400-344C-94AE-A83D801EFB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -3983,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AW26" sqref="AW26"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3:AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8014,7 +8014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
re-do adding isotope standards (15RAir, 18RVSMOW, etc.) as adjustable parameters
</commit_message>
<xml_diff>
--- a/src/00_Python_template_v2.xlsx
+++ b/src/00_Python_template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF98DA7C-7400-344C-94AE-A83D801EFB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E71807-3D2E-EF4B-A0D4-4AAFE02189AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25440" yWindow="-5500" windowWidth="25440" windowHeight="21780" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -1155,7 +1155,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1399,6 +1399,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -3983,8 +3984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3:AO17"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AT18" sqref="AT18:BD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4371,10 +4372,10 @@
         <v>0</v>
       </c>
       <c r="AP3" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ3" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR3" s="47">
         <f>A3</f>
@@ -4394,22 +4395,22 @@
         <v>47.588174908592201</v>
       </c>
       <c r="AX3" s="50">
-        <v>15.105455486877901</v>
+        <v>15.141747165380499</v>
       </c>
       <c r="AY3" s="50">
-        <v>-2.7098456777153701</v>
+        <v>-2.74613758912745</v>
       </c>
       <c r="AZ3" s="50">
-        <v>17.815301164593201</v>
+        <v>17.887884754507901</v>
       </c>
       <c r="BA3" s="50">
-        <v>6.19780490458127</v>
+        <v>6.1978047881265299</v>
       </c>
       <c r="BB3" s="50">
-        <v>24.009727067820499</v>
+        <v>24.009729321814799</v>
       </c>
       <c r="BC3" s="50">
-        <v>47.054171086232202</v>
+        <v>47.054175552740901</v>
       </c>
       <c r="BD3" s="44"/>
       <c r="BE3">
@@ -4557,10 +4558,10 @@
         <v>0</v>
       </c>
       <c r="AP4" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ4" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR4" s="47">
         <f t="shared" ref="AR4:AR17" si="10">A4</f>
@@ -4580,22 +4581,22 @@
         <v>35.169038165624201</v>
       </c>
       <c r="AX4" s="50">
-        <v>6.8736240880515798</v>
+        <v>6.9101705872438499</v>
       </c>
       <c r="AY4" s="50">
-        <v>-13.881471917271901</v>
+        <v>-13.918018685360799</v>
       </c>
       <c r="AZ4" s="50">
-        <v>20.755096005323502</v>
+        <v>20.8281892726046</v>
       </c>
       <c r="BA4" s="50">
-        <v>-3.5039239146101799</v>
+        <v>-3.5039240490584702</v>
       </c>
       <c r="BB4" s="50">
-        <v>17.848649659933699</v>
+        <v>17.848652262194701</v>
       </c>
       <c r="BC4" s="50">
-        <v>34.879852068524698</v>
+        <v>34.879857196050899</v>
       </c>
       <c r="BD4" s="44"/>
       <c r="BE4">
@@ -4748,10 +4749,10 @@
         <v>0</v>
       </c>
       <c r="AP5" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ5" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR5" s="47">
         <f t="shared" si="10"/>
@@ -4771,22 +4772,22 @@
         <v>44.4548477102446</v>
       </c>
       <c r="AX5" s="50">
-        <v>-0.53970856962448599</v>
+        <v>-0.50736518397154196</v>
       </c>
       <c r="AY5" s="50">
-        <v>1.2825215740412901</v>
+        <v>1.2501782087612701</v>
       </c>
       <c r="AZ5" s="50">
-        <v>-1.82223014366578</v>
+        <v>-1.7575433927328099</v>
       </c>
       <c r="BA5" s="50">
-        <v>0.37140650220840399</v>
+        <v>0.37140651239486699</v>
       </c>
       <c r="BB5" s="50">
-        <v>22.461390435589401</v>
+        <v>22.461390238430901</v>
       </c>
       <c r="BC5" s="50">
-        <v>43.988167450184299</v>
+        <v>43.988167060049697</v>
       </c>
       <c r="BD5" s="44"/>
       <c r="BE5">
@@ -4943,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="AP6" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ6" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR6" s="47">
         <f t="shared" si="10"/>
@@ -4966,22 +4967,22 @@
         <v>47.762096293894203</v>
       </c>
       <c r="AX6" s="50">
-        <v>14.851574153242799</v>
+        <v>14.8874962367391</v>
       </c>
       <c r="AY6" s="50">
-        <v>-0.85838254078074405</v>
+        <v>-0.89430482302266201</v>
       </c>
       <c r="AZ6" s="50">
-        <v>15.7099566940236</v>
+        <v>15.781801059761699</v>
       </c>
       <c r="BA6" s="50">
-        <v>6.9965958062310696</v>
+        <v>6.9965957068582298</v>
       </c>
       <c r="BB6" s="50">
-        <v>24.095420378555701</v>
+        <v>24.095422301925101</v>
       </c>
       <c r="BC6" s="50">
-        <v>47.223987370547697</v>
+        <v>47.223991182190296</v>
       </c>
       <c r="BD6" s="44"/>
       <c r="BE6">
@@ -5138,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="AP7" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ7" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR7" s="47">
         <f t="shared" si="10"/>
@@ -5161,22 +5162,22 @@
         <v>35.355596284351698</v>
       </c>
       <c r="AX7" s="50">
-        <v>6.6566362138331598</v>
+        <v>6.6931237200740199</v>
       </c>
       <c r="AY7" s="50">
-        <v>-13.8026489120794</v>
+        <v>-13.839136682964901</v>
       </c>
       <c r="AZ7" s="50">
-        <v>20.459285125912601</v>
+        <v>20.532260403039</v>
       </c>
       <c r="BA7" s="50">
-        <v>-3.5730063491231601</v>
+        <v>-3.5730064814454798</v>
       </c>
       <c r="BB7" s="50">
-        <v>17.941820061995799</v>
+        <v>17.9418226231091</v>
       </c>
       <c r="BC7" s="50">
-        <v>35.063444020270097</v>
+        <v>35.063449067151502</v>
       </c>
       <c r="BD7" s="44"/>
       <c r="BE7">
@@ -5324,10 +5325,10 @@
         <v>0</v>
       </c>
       <c r="AP8" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ8" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR8" s="47">
         <f t="shared" si="10"/>
@@ -5347,22 +5348,22 @@
         <v>42.5456389567846</v>
       </c>
       <c r="AX8" s="50">
-        <v>-1.15628904358433</v>
+        <v>-1.12372542594363</v>
       </c>
       <c r="AY8" s="50">
-        <v>-0.70441124849329695</v>
+        <v>-0.73697486134960399</v>
       </c>
       <c r="AZ8" s="50">
-        <v>-0.45187779509103798</v>
+        <v>-0.38675056459402901</v>
       </c>
       <c r="BA8" s="50">
-        <v>-0.93035014603881605</v>
+        <v>-0.93035014364661806</v>
       </c>
       <c r="BB8" s="50">
-        <v>21.5157968077277</v>
+        <v>21.515796761425801</v>
       </c>
       <c r="BC8" s="50">
-        <v>42.117851051899301</v>
+        <v>42.117850960357202</v>
       </c>
       <c r="BD8" s="44"/>
       <c r="BE8">
@@ -5513,10 +5514,10 @@
         <v>0</v>
       </c>
       <c r="AP9" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ9" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR9" s="47">
         <f t="shared" si="10"/>
@@ -5536,22 +5537,22 @@
         <v>45.7807904317755</v>
       </c>
       <c r="AX9" s="50">
-        <v>16.036656468840999</v>
+        <v>16.073527322729898</v>
       </c>
       <c r="AY9" s="50">
-        <v>-4.8656873390863202</v>
+        <v>-4.9025584289184003</v>
       </c>
       <c r="AZ9" s="50">
-        <v>20.902343807927299</v>
+        <v>20.976085751648299</v>
       </c>
       <c r="BA9" s="50">
-        <v>5.5854845648773397</v>
+        <v>5.5854844469057596</v>
       </c>
       <c r="BB9" s="50">
-        <v>23.117269398744899</v>
+        <v>23.117271682096799</v>
       </c>
       <c r="BC9" s="50">
-        <v>45.286402388126902</v>
+        <v>45.286406909111598</v>
       </c>
       <c r="BE9">
         <v>265</v>
@@ -5699,10 +5700,10 @@
         <v>0</v>
       </c>
       <c r="AP10" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ10" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR10" s="47">
         <f t="shared" si="10"/>
@@ -5722,22 +5723,22 @@
         <v>45.209547777639301</v>
       </c>
       <c r="AX10" s="50">
-        <v>14.4579715364672</v>
+        <v>14.499770218291401</v>
       </c>
       <c r="AY10" s="50">
-        <v>-34.815304667159701</v>
+        <v>-34.8571040740905</v>
       </c>
       <c r="AZ10" s="50">
-        <v>49.273276203626899</v>
+        <v>49.356874292382003</v>
       </c>
       <c r="BA10" s="50">
-        <v>-10.1786665653462</v>
+        <v>-10.178666927899499</v>
       </c>
       <c r="BB10" s="50">
-        <v>22.853627356464699</v>
+        <v>22.853634373716901</v>
       </c>
       <c r="BC10" s="50">
-        <v>44.764460247631298</v>
+        <v>44.764474138272199</v>
       </c>
       <c r="BE10">
         <v>265</v>
@@ -5891,10 +5892,10 @@
         <v>0</v>
       </c>
       <c r="AP11" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ11" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR11" s="47">
         <f t="shared" si="10"/>
@@ -5914,22 +5915,22 @@
         <v>45.520315450628203</v>
       </c>
       <c r="AX11" s="50">
-        <v>17.1518234709566</v>
+        <v>17.1888714035757</v>
       </c>
       <c r="AY11" s="50">
-        <v>-4.5745335204508901</v>
+        <v>-4.61158174022147</v>
       </c>
       <c r="AZ11" s="50">
-        <v>21.726356991407499</v>
+        <v>21.8004531437971</v>
       </c>
       <c r="BA11" s="50">
-        <v>6.2886449752528799</v>
+        <v>6.2886448316771197</v>
       </c>
       <c r="BB11" s="50">
-        <v>22.988533215933799</v>
+        <v>22.988535994855599</v>
       </c>
       <c r="BC11" s="50">
-        <v>45.031522726332703</v>
+        <v>45.031528227884998</v>
       </c>
       <c r="BE11">
         <v>265</v>
@@ -6075,10 +6076,10 @@
         <v>0</v>
       </c>
       <c r="AP12" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ12" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR12" s="47">
         <f t="shared" si="10"/>
@@ -6098,22 +6099,22 @@
         <v>33.978406326581499</v>
       </c>
       <c r="AX12" s="50">
-        <v>7.0098620813652204</v>
+        <v>7.0465586425019202</v>
       </c>
       <c r="AY12" s="50">
-        <v>-14.5751415214816</v>
+        <v>-14.611838363625999</v>
       </c>
       <c r="AZ12" s="50">
-        <v>21.5850036028468</v>
+        <v>21.658397006127899</v>
       </c>
       <c r="BA12" s="50">
-        <v>-3.78263972005821</v>
+        <v>-3.7826398605620399</v>
       </c>
       <c r="BB12" s="50">
-        <v>17.254451999306699</v>
+        <v>17.2544547187725</v>
       </c>
       <c r="BC12" s="50">
-        <v>33.709358475152598</v>
+        <v>33.7093638306862</v>
       </c>
       <c r="BE12">
         <v>265</v>
@@ -6259,10 +6260,10 @@
         <v>0</v>
       </c>
       <c r="AP13" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ13" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR13" s="47">
         <f t="shared" si="10"/>
@@ -6282,22 +6283,22 @@
         <v>44.181166769186902</v>
       </c>
       <c r="AX13" s="50">
-        <v>8.2241945278393999E-2</v>
+        <v>0.114900961821762</v>
       </c>
       <c r="AY13" s="50">
-        <v>0.22102332359041901</v>
+        <v>0.188364308266075</v>
       </c>
       <c r="AZ13" s="50">
-        <v>-0.138781378312025</v>
+        <v>-7.3463346444313501E-2</v>
       </c>
       <c r="BA13" s="50">
-        <v>0.151632634434406</v>
+        <v>0.151632635043919</v>
       </c>
       <c r="BB13" s="50">
-        <v>22.3259423648012</v>
+        <v>22.325942353005299</v>
       </c>
       <c r="BC13" s="50">
-        <v>43.720161276728597</v>
+        <v>43.720161253389897</v>
       </c>
       <c r="BE13">
         <v>265</v>
@@ -6443,10 +6444,10 @@
         <v>0</v>
       </c>
       <c r="AP14" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ14" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR14" s="47">
         <f t="shared" si="10"/>
@@ -6466,22 +6467,22 @@
         <v>45.431524384704502</v>
       </c>
       <c r="AX14" s="50">
-        <v>14.393773542834699</v>
+        <v>14.4300942742865</v>
       </c>
       <c r="AY14" s="50">
-        <v>-3.6809189289388402</v>
+        <v>-3.7172398582032602</v>
       </c>
       <c r="AZ14" s="50">
-        <v>18.074692471773599</v>
+        <v>18.147334132489799</v>
       </c>
       <c r="BA14" s="50">
-        <v>5.3564273069479604</v>
+        <v>5.3564272080416302</v>
       </c>
       <c r="BB14" s="50">
-        <v>22.94455532836</v>
+        <v>22.944557242700899</v>
       </c>
       <c r="BC14" s="50">
-        <v>44.944459545090702</v>
+        <v>44.9444633348417</v>
       </c>
       <c r="BE14">
         <v>265</v>
@@ -6627,10 +6628,10 @@
         <v>0</v>
       </c>
       <c r="AP15" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ15" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR15" s="47">
         <f t="shared" si="10"/>
@@ -6650,22 +6651,22 @@
         <v>46.530448225756899</v>
       </c>
       <c r="AX15" s="50">
-        <v>16.679833428360201</v>
+        <v>16.716733662545099</v>
       </c>
       <c r="AY15" s="50">
-        <v>-4.3336183513273898</v>
+        <v>-4.37051886674322</v>
       </c>
       <c r="AZ15" s="50">
-        <v>21.0134517796876</v>
+        <v>21.0872525292883</v>
       </c>
       <c r="BA15" s="50">
-        <v>6.1731075385164003</v>
+        <v>6.1731073979009397</v>
       </c>
       <c r="BB15" s="50">
-        <v>23.487665779901398</v>
+        <v>23.487668501528098</v>
       </c>
       <c r="BC15" s="50">
-        <v>46.019903286484897</v>
+        <v>46.019908677073602</v>
       </c>
       <c r="BE15">
         <v>265</v>
@@ -6811,10 +6812,10 @@
         <v>0</v>
       </c>
       <c r="AP16" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ16" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR16" s="47">
         <f t="shared" si="10"/>
@@ -6834,22 +6835,22 @@
         <v>34.941280181798497</v>
       </c>
       <c r="AX16" s="50">
-        <v>7.1029978910310803</v>
+        <v>7.1397696155843704</v>
       </c>
       <c r="AY16" s="50">
-        <v>-14.893050092214599</v>
+        <v>-14.929822103606799</v>
       </c>
       <c r="AZ16" s="50">
-        <v>21.996047983245699</v>
+        <v>22.069591719191202</v>
       </c>
       <c r="BA16" s="50">
-        <v>-3.8950261005917799</v>
+        <v>-3.8950262440112202</v>
       </c>
       <c r="BB16" s="50">
-        <v>17.735485742880101</v>
+        <v>17.735488518779</v>
       </c>
       <c r="BC16" s="50">
-        <v>34.656884164523802</v>
+        <v>34.656889633617602</v>
       </c>
       <c r="BE16">
         <v>265</v>
@@ -6991,10 +6992,10 @@
         <v>0</v>
       </c>
       <c r="AP17" s="56">
-        <v>0.18325645634287266</v>
+        <v>0.1834074217910111</v>
       </c>
       <c r="AQ17" s="57">
-        <v>9.0490249769565087E-2</v>
+        <v>9.0617489866283679E-2</v>
       </c>
       <c r="AR17" s="47">
         <f t="shared" si="10"/>
@@ -7014,22 +7015,22 @@
         <v>44.644312779463498</v>
       </c>
       <c r="AX17" s="50">
-        <v>13.725240315331099</v>
+        <v>13.7657492080405</v>
       </c>
       <c r="AY17" s="50">
-        <v>-28.3353648321477</v>
+        <v>-28.375874329284699</v>
       </c>
       <c r="AZ17" s="50">
-        <v>42.060605147478803</v>
+        <v>42.141623537325302</v>
       </c>
       <c r="BA17" s="50">
-        <v>-7.3050622584082596</v>
+        <v>-7.3050625606221304</v>
       </c>
       <c r="BB17" s="50">
-        <v>22.565126816266901</v>
+        <v>22.565132665643699</v>
       </c>
       <c r="BC17" s="50">
-        <v>44.193449376003002</v>
+        <v>44.1934609517726</v>
       </c>
       <c r="BE17">
         <v>265</v>
@@ -7142,12 +7143,16 @@
       <c r="AQ19" s="54"/>
       <c r="AR19" s="49"/>
       <c r="AS19" s="48"/>
-      <c r="AX19" s="48"/>
-      <c r="AY19" s="48"/>
-      <c r="AZ19" s="48"/>
-      <c r="BA19" s="48"/>
-      <c r="BB19" s="48"/>
-      <c r="BC19" s="48"/>
+      <c r="AT19" s="133"/>
+      <c r="AU19" s="133"/>
+      <c r="AV19" s="133"/>
+      <c r="AW19" s="133"/>
+      <c r="AX19" s="133"/>
+      <c r="AY19" s="133"/>
+      <c r="AZ19" s="133"/>
+      <c r="BA19" s="133"/>
+      <c r="BB19" s="133"/>
+      <c r="BC19" s="133"/>
     </row>
     <row r="20" spans="1:65">
       <c r="C20" s="24"/>
@@ -7184,12 +7189,16 @@
       <c r="AQ20" s="54"/>
       <c r="AR20" s="49"/>
       <c r="AS20" s="48"/>
-      <c r="AX20" s="48"/>
-      <c r="AY20" s="48"/>
-      <c r="AZ20" s="48"/>
-      <c r="BA20" s="48"/>
-      <c r="BB20" s="48"/>
-      <c r="BC20" s="48"/>
+      <c r="AT20" s="133"/>
+      <c r="AU20" s="133"/>
+      <c r="AV20" s="133"/>
+      <c r="AW20" s="133"/>
+      <c r="AX20" s="133"/>
+      <c r="AY20" s="133"/>
+      <c r="AZ20" s="133"/>
+      <c r="BA20" s="133"/>
+      <c r="BB20" s="133"/>
+      <c r="BC20" s="133"/>
     </row>
     <row r="21" spans="1:65">
       <c r="C21" s="24"/>
@@ -7226,12 +7235,16 @@
       <c r="AQ21" s="54"/>
       <c r="AR21" s="49"/>
       <c r="AS21" s="48"/>
-      <c r="AX21" s="48"/>
-      <c r="AY21" s="48"/>
-      <c r="AZ21" s="48"/>
-      <c r="BA21" s="48"/>
-      <c r="BB21" s="48"/>
-      <c r="BC21" s="48"/>
+      <c r="AT21" s="133"/>
+      <c r="AU21" s="133"/>
+      <c r="AV21" s="133"/>
+      <c r="AW21" s="133"/>
+      <c r="AX21" s="133"/>
+      <c r="AY21" s="133"/>
+      <c r="AZ21" s="133"/>
+      <c r="BA21" s="133"/>
+      <c r="BB21" s="133"/>
+      <c r="BC21" s="133"/>
     </row>
     <row r="22" spans="1:65">
       <c r="C22" s="24"/>

</xml_diff>